<commit_message>
busy morning, add more fields, more filters
send DBA about password expired, add more fields to the template, add
year and district filter to the popup window, add a pdf file for all the
tables and columns in the database, add the tables used in the analysis.
</commit_message>
<xml_diff>
--- a/2012 CALTRANS TIMESHEET 0727-0809.xlsx
+++ b/2012 CALTRANS TIMESHEET 0727-0809.xlsx
@@ -219,8 +219,8 @@
   <numFmts count="4">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[h]:mm"/>
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="[h]:mm"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -1011,7 +1011,7 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1020,13 +1020,13 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1035,30 +1035,30 @@
     <xf numFmtId="1" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1106,13 +1106,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -1188,11 +1188,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1222,19 +1222,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1244,15 +1244,15 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="19" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1423,83 +1423,44 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1507,75 +1468,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="18" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -1583,48 +1480,50 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1670,81 +1569,182 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="20" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2254,7 +2254,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -2296,7 +2296,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -2319,7 +2319,7 @@
   <dimension ref="A1:BG51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13:U13"/>
+      <selection activeCell="Y4" sqref="Y4:AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75"/>
@@ -2353,38 +2353,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="24.75" customHeight="1">
-      <c r="G1" s="192" t="s">
+      <c r="G1" s="200" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="192"/>
-      <c r="I1" s="192"/>
-      <c r="J1" s="192"/>
-      <c r="K1" s="192"/>
-      <c r="L1" s="192"/>
-      <c r="M1" s="192"/>
-      <c r="N1" s="192"/>
-      <c r="O1" s="192"/>
-      <c r="P1" s="192"/>
-      <c r="Q1" s="192"/>
-      <c r="R1" s="192"/>
-      <c r="S1" s="192"/>
-      <c r="T1" s="192"/>
-      <c r="U1" s="192"/>
-      <c r="V1" s="192"/>
-      <c r="W1" s="192"/>
-      <c r="X1" s="192"/>
-      <c r="Y1" s="192"/>
-      <c r="Z1" s="192"/>
-      <c r="AA1" s="192"/>
-      <c r="AB1" s="192"/>
-      <c r="AC1" s="192"/>
-      <c r="AD1" s="192"/>
-      <c r="AE1" s="192"/>
-      <c r="AF1" s="192"/>
-      <c r="AG1" s="192"/>
-      <c r="AH1" s="192"/>
-      <c r="AI1" s="192"/>
-      <c r="AJ1" s="192"/>
+      <c r="H1" s="200"/>
+      <c r="I1" s="200"/>
+      <c r="J1" s="200"/>
+      <c r="K1" s="200"/>
+      <c r="L1" s="200"/>
+      <c r="M1" s="200"/>
+      <c r="N1" s="200"/>
+      <c r="O1" s="200"/>
+      <c r="P1" s="200"/>
+      <c r="Q1" s="200"/>
+      <c r="R1" s="200"/>
+      <c r="S1" s="200"/>
+      <c r="T1" s="200"/>
+      <c r="U1" s="200"/>
+      <c r="V1" s="200"/>
+      <c r="W1" s="200"/>
+      <c r="X1" s="200"/>
+      <c r="Y1" s="200"/>
+      <c r="Z1" s="200"/>
+      <c r="AA1" s="200"/>
+      <c r="AB1" s="200"/>
+      <c r="AC1" s="200"/>
+      <c r="AD1" s="200"/>
+      <c r="AE1" s="200"/>
+      <c r="AF1" s="200"/>
+      <c r="AG1" s="200"/>
+      <c r="AH1" s="200"/>
+      <c r="AI1" s="200"/>
+      <c r="AJ1" s="200"/>
       <c r="AK1" s="71" t="s">
         <v>15</v>
       </c>
@@ -2456,23 +2456,23 @@
       <c r="V4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="205">
+      <c r="Y4" s="178">
         <v>41847</v>
       </c>
-      <c r="Z4" s="205"/>
-      <c r="AA4" s="205"/>
-      <c r="AB4" s="205"/>
-      <c r="AC4" s="205"/>
+      <c r="Z4" s="178"/>
+      <c r="AA4" s="178"/>
+      <c r="AB4" s="178"/>
+      <c r="AC4" s="178"/>
       <c r="AD4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="AE4" s="204">
+      <c r="AE4" s="177">
         <v>41860</v>
       </c>
-      <c r="AF4" s="204"/>
-      <c r="AG4" s="204"/>
-      <c r="AH4" s="204"/>
-      <c r="AI4" s="204"/>
+      <c r="AF4" s="177"/>
+      <c r="AG4" s="177"/>
+      <c r="AH4" s="177"/>
+      <c r="AI4" s="177"/>
       <c r="AO4" s="27"/>
       <c r="AP4" s="27"/>
       <c r="AQ4" s="3"/>
@@ -2488,66 +2488,66 @@
       <c r="R5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="Y5" s="203" t="s">
+      <c r="Y5" s="176" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="203"/>
-      <c r="AA5" s="203"/>
-      <c r="AB5" s="203"/>
-      <c r="AC5" s="203"/>
+      <c r="Z5" s="176"/>
+      <c r="AA5" s="176"/>
+      <c r="AB5" s="176"/>
+      <c r="AC5" s="176"/>
       <c r="AD5" s="33"/>
-      <c r="AE5" s="203" t="s">
+      <c r="AE5" s="176" t="s">
         <v>25</v>
       </c>
-      <c r="AF5" s="203"/>
-      <c r="AG5" s="203"/>
-      <c r="AH5" s="203"/>
-      <c r="AI5" s="203"/>
+      <c r="AF5" s="176"/>
+      <c r="AG5" s="176"/>
+      <c r="AH5" s="176"/>
+      <c r="AI5" s="176"/>
       <c r="AJ5" s="34"/>
-      <c r="AK5" s="206" t="s">
+      <c r="AK5" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="AL5" s="207"/>
-      <c r="AM5" s="207"/>
-      <c r="AN5" s="207"/>
-      <c r="AO5" s="207"/>
-      <c r="AP5" s="208"/>
+      <c r="AL5" s="180"/>
+      <c r="AM5" s="180"/>
+      <c r="AN5" s="180"/>
+      <c r="AO5" s="180"/>
+      <c r="AP5" s="181"/>
       <c r="AQ5" s="3"/>
     </row>
     <row r="6" spans="1:53" ht="21.75" customHeight="1">
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
       <c r="O6" s="69"/>
-      <c r="P6" s="196" t="s">
+      <c r="P6" s="187" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="196"/>
-      <c r="R6" s="196"/>
-      <c r="S6" s="196"/>
-      <c r="T6" s="197"/>
+      <c r="Q6" s="187"/>
+      <c r="R6" s="187"/>
+      <c r="S6" s="187"/>
+      <c r="T6" s="188"/>
       <c r="V6" s="68" t="s">
         <v>12</v>
       </c>
       <c r="W6" s="35"/>
-      <c r="X6" s="212"/>
-      <c r="Y6" s="212"/>
-      <c r="Z6" s="212"/>
-      <c r="AA6" s="212"/>
-      <c r="AB6" s="212"/>
-      <c r="AC6" s="212"/>
-      <c r="AD6" s="212"/>
-      <c r="AE6" s="212"/>
-      <c r="AF6" s="212"/>
-      <c r="AG6" s="212"/>
-      <c r="AH6" s="212"/>
-      <c r="AI6" s="212"/>
+      <c r="X6" s="185"/>
+      <c r="Y6" s="185"/>
+      <c r="Z6" s="185"/>
+      <c r="AA6" s="185"/>
+      <c r="AB6" s="185"/>
+      <c r="AC6" s="185"/>
+      <c r="AD6" s="185"/>
+      <c r="AE6" s="185"/>
+      <c r="AF6" s="185"/>
+      <c r="AG6" s="185"/>
+      <c r="AH6" s="185"/>
+      <c r="AI6" s="185"/>
       <c r="AJ6" s="34"/>
-      <c r="AK6" s="209"/>
-      <c r="AL6" s="210"/>
-      <c r="AM6" s="210"/>
-      <c r="AN6" s="210"/>
-      <c r="AO6" s="210"/>
-      <c r="AP6" s="211"/>
+      <c r="AK6" s="182"/>
+      <c r="AL6" s="183"/>
+      <c r="AM6" s="183"/>
+      <c r="AN6" s="183"/>
+      <c r="AO6" s="183"/>
+      <c r="AP6" s="184"/>
       <c r="AQ6" s="3"/>
     </row>
     <row r="7" spans="1:53" ht="24" customHeight="1">
@@ -2557,11 +2557,11 @@
       <c r="M7" s="57"/>
       <c r="N7" s="57"/>
       <c r="O7" s="69"/>
-      <c r="P7" s="198"/>
-      <c r="Q7" s="198"/>
-      <c r="R7" s="198"/>
-      <c r="S7" s="198"/>
-      <c r="T7" s="199"/>
+      <c r="P7" s="189"/>
+      <c r="Q7" s="189"/>
+      <c r="R7" s="189"/>
+      <c r="S7" s="189"/>
+      <c r="T7" s="190"/>
       <c r="V7" s="66" t="s">
         <v>13</v>
       </c>
@@ -2569,23 +2569,23 @@
       <c r="X7" s="77"/>
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
-      <c r="AA7" s="213"/>
-      <c r="AB7" s="213"/>
-      <c r="AC7" s="213"/>
-      <c r="AD7" s="213"/>
-      <c r="AE7" s="213"/>
-      <c r="AF7" s="213"/>
-      <c r="AG7" s="213"/>
-      <c r="AH7" s="213"/>
-      <c r="AI7" s="213"/>
-      <c r="AK7" s="203" t="s">
+      <c r="AA7" s="186"/>
+      <c r="AB7" s="186"/>
+      <c r="AC7" s="186"/>
+      <c r="AD7" s="186"/>
+      <c r="AE7" s="186"/>
+      <c r="AF7" s="186"/>
+      <c r="AG7" s="186"/>
+      <c r="AH7" s="186"/>
+      <c r="AI7" s="186"/>
+      <c r="AK7" s="176" t="s">
         <v>14</v>
       </c>
-      <c r="AL7" s="203"/>
-      <c r="AM7" s="203"/>
-      <c r="AN7" s="203"/>
-      <c r="AO7" s="203"/>
-      <c r="AP7" s="203"/>
+      <c r="AL7" s="176"/>
+      <c r="AM7" s="176"/>
+      <c r="AN7" s="176"/>
+      <c r="AO7" s="176"/>
+      <c r="AP7" s="176"/>
       <c r="AQ7" s="3"/>
     </row>
     <row r="8" spans="1:53" ht="10.5" customHeight="1" thickBot="1">
@@ -2615,62 +2615,62 @@
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
-      <c r="G9" s="193"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="195"/>
-      <c r="J9" s="178" t="s">
+      <c r="G9" s="197"/>
+      <c r="H9" s="198"/>
+      <c r="I9" s="199"/>
+      <c r="J9" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="178"/>
-      <c r="L9" s="178"/>
-      <c r="M9" s="178" t="s">
+      <c r="K9" s="173"/>
+      <c r="L9" s="173"/>
+      <c r="M9" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="178"/>
-      <c r="O9" s="178"/>
-      <c r="P9" s="178" t="s">
+      <c r="N9" s="173"/>
+      <c r="O9" s="173"/>
+      <c r="P9" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="178"/>
-      <c r="R9" s="178"/>
-      <c r="S9" s="200" t="s">
+      <c r="Q9" s="173"/>
+      <c r="R9" s="173"/>
+      <c r="S9" s="191" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="201"/>
-      <c r="U9" s="202"/>
-      <c r="V9" s="178" t="s">
+      <c r="T9" s="192"/>
+      <c r="U9" s="193"/>
+      <c r="V9" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="W9" s="178"/>
-      <c r="X9" s="178"/>
-      <c r="Y9" s="215"/>
-      <c r="Z9" s="215"/>
-      <c r="AA9" s="215"/>
-      <c r="AB9" s="178" t="s">
+      <c r="W9" s="173"/>
+      <c r="X9" s="173"/>
+      <c r="Y9" s="175"/>
+      <c r="Z9" s="175"/>
+      <c r="AA9" s="175"/>
+      <c r="AB9" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="AC9" s="178"/>
-      <c r="AD9" s="178"/>
-      <c r="AE9" s="214" t="s">
+      <c r="AC9" s="173"/>
+      <c r="AD9" s="173"/>
+      <c r="AE9" s="174" t="s">
         <v>19</v>
       </c>
-      <c r="AF9" s="214"/>
-      <c r="AG9" s="214"/>
-      <c r="AH9" s="178" t="s">
+      <c r="AF9" s="174"/>
+      <c r="AG9" s="174"/>
+      <c r="AH9" s="173" t="s">
         <v>18</v>
       </c>
-      <c r="AI9" s="178"/>
-      <c r="AJ9" s="178"/>
-      <c r="AK9" s="178" t="s">
+      <c r="AI9" s="173"/>
+      <c r="AJ9" s="173"/>
+      <c r="AK9" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="AL9" s="178"/>
-      <c r="AM9" s="178"/>
-      <c r="AN9" s="178" t="s">
+      <c r="AL9" s="173"/>
+      <c r="AM9" s="173"/>
+      <c r="AN9" s="173" t="s">
         <v>20</v>
       </c>
-      <c r="AO9" s="178"/>
-      <c r="AP9" s="178"/>
+      <c r="AO9" s="173"/>
+      <c r="AP9" s="173"/>
       <c r="AQ9" s="21" t="s">
         <v>40</v>
       </c>
@@ -2710,52 +2710,52 @@
       <c r="D10" s="82"/>
       <c r="E10" s="82"/>
       <c r="F10" s="83"/>
-      <c r="G10" s="178" t="s">
+      <c r="G10" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="178"/>
-      <c r="I10" s="178"/>
-      <c r="J10" s="177"/>
-      <c r="K10" s="177"/>
-      <c r="L10" s="177"/>
-      <c r="M10" s="177"/>
-      <c r="N10" s="177"/>
-      <c r="O10" s="177"/>
-      <c r="P10" s="177"/>
-      <c r="Q10" s="177"/>
-      <c r="R10" s="177"/>
-      <c r="S10" s="177"/>
-      <c r="T10" s="177"/>
-      <c r="U10" s="177"/>
-      <c r="V10" s="159">
+      <c r="H10" s="173"/>
+      <c r="I10" s="173"/>
+      <c r="J10" s="158"/>
+      <c r="K10" s="158"/>
+      <c r="L10" s="158"/>
+      <c r="M10" s="158"/>
+      <c r="N10" s="158"/>
+      <c r="O10" s="158"/>
+      <c r="P10" s="158"/>
+      <c r="Q10" s="158"/>
+      <c r="R10" s="158"/>
+      <c r="S10" s="158"/>
+      <c r="T10" s="158"/>
+      <c r="U10" s="158"/>
+      <c r="V10" s="172">
         <f>((M10-J10)+(S10-P10))</f>
         <v>0</v>
       </c>
-      <c r="W10" s="159"/>
-      <c r="X10" s="159"/>
-      <c r="Y10" s="178" t="s">
+      <c r="W10" s="172"/>
+      <c r="X10" s="172"/>
+      <c r="Y10" s="173" t="s">
         <v>4</v>
       </c>
-      <c r="Z10" s="178"/>
-      <c r="AA10" s="178"/>
-      <c r="AB10" s="177"/>
-      <c r="AC10" s="177"/>
-      <c r="AD10" s="177"/>
-      <c r="AE10" s="177"/>
-      <c r="AF10" s="177"/>
-      <c r="AG10" s="177"/>
-      <c r="AH10" s="177"/>
-      <c r="AI10" s="177"/>
-      <c r="AJ10" s="177"/>
-      <c r="AK10" s="177"/>
-      <c r="AL10" s="177"/>
-      <c r="AM10" s="177"/>
-      <c r="AN10" s="159">
+      <c r="Z10" s="173"/>
+      <c r="AA10" s="173"/>
+      <c r="AB10" s="158"/>
+      <c r="AC10" s="158"/>
+      <c r="AD10" s="158"/>
+      <c r="AE10" s="158"/>
+      <c r="AF10" s="158"/>
+      <c r="AG10" s="158"/>
+      <c r="AH10" s="158"/>
+      <c r="AI10" s="158"/>
+      <c r="AJ10" s="158"/>
+      <c r="AK10" s="158"/>
+      <c r="AL10" s="158"/>
+      <c r="AM10" s="158"/>
+      <c r="AN10" s="172">
         <f t="shared" ref="AN10:AN16" si="0">((AE10-AB10)+(AK10-AH10))</f>
         <v>0</v>
       </c>
-      <c r="AO10" s="159"/>
-      <c r="AP10" s="159"/>
+      <c r="AO10" s="172"/>
+      <c r="AP10" s="172"/>
       <c r="AQ10" s="22">
         <f>MIN(8/24,V10)</f>
         <v>0</v>
@@ -2805,60 +2805,60 @@
       <c r="D11" s="82"/>
       <c r="E11" s="82"/>
       <c r="F11" s="83"/>
-      <c r="G11" s="178" t="s">
+      <c r="G11" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="178"/>
-      <c r="I11" s="178"/>
-      <c r="J11" s="177"/>
-      <c r="K11" s="177"/>
-      <c r="L11" s="177"/>
-      <c r="M11" s="177"/>
-      <c r="N11" s="177"/>
-      <c r="O11" s="177"/>
-      <c r="P11" s="177"/>
-      <c r="Q11" s="177"/>
-      <c r="R11" s="177"/>
-      <c r="S11" s="177"/>
-      <c r="T11" s="177"/>
-      <c r="U11" s="177"/>
-      <c r="V11" s="159">
+      <c r="H11" s="173"/>
+      <c r="I11" s="173"/>
+      <c r="J11" s="158"/>
+      <c r="K11" s="195"/>
+      <c r="L11" s="196"/>
+      <c r="M11" s="194"/>
+      <c r="N11" s="195"/>
+      <c r="O11" s="196"/>
+      <c r="P11" s="194"/>
+      <c r="Q11" s="195"/>
+      <c r="R11" s="196"/>
+      <c r="S11" s="194"/>
+      <c r="T11" s="195"/>
+      <c r="U11" s="196"/>
+      <c r="V11" s="172">
         <f t="shared" ref="V11:V16" si="7">((M11-J11)+(S11-P11))</f>
         <v>0</v>
       </c>
-      <c r="W11" s="159"/>
-      <c r="X11" s="159"/>
-      <c r="Y11" s="178" t="s">
+      <c r="W11" s="172"/>
+      <c r="X11" s="172"/>
+      <c r="Y11" s="173" t="s">
         <v>5</v>
       </c>
-      <c r="Z11" s="178"/>
-      <c r="AA11" s="178"/>
-      <c r="AB11" s="177">
+      <c r="Z11" s="173"/>
+      <c r="AA11" s="173"/>
+      <c r="AB11" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC11" s="177"/>
-      <c r="AD11" s="177"/>
-      <c r="AE11" s="180">
+      <c r="AC11" s="158"/>
+      <c r="AD11" s="158"/>
+      <c r="AE11" s="194">
         <v>0.5</v>
       </c>
-      <c r="AF11" s="181"/>
-      <c r="AG11" s="182"/>
-      <c r="AH11" s="177">
+      <c r="AF11" s="195"/>
+      <c r="AG11" s="196"/>
+      <c r="AH11" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI11" s="177"/>
-      <c r="AJ11" s="177"/>
-      <c r="AK11" s="177">
+      <c r="AI11" s="158"/>
+      <c r="AJ11" s="158"/>
+      <c r="AK11" s="158">
         <v>0.6875</v>
       </c>
-      <c r="AL11" s="177"/>
-      <c r="AM11" s="177"/>
-      <c r="AN11" s="159">
+      <c r="AL11" s="158"/>
+      <c r="AM11" s="158"/>
+      <c r="AN11" s="172">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO11" s="159"/>
-      <c r="AP11" s="159"/>
+      <c r="AO11" s="172"/>
+      <c r="AP11" s="172"/>
       <c r="AQ11" s="22">
         <f t="shared" ref="AQ11:AQ16" si="8">MIN(8/24,V11)</f>
         <v>0</v>
@@ -2908,68 +2908,68 @@
       <c r="D12" s="82"/>
       <c r="E12" s="82"/>
       <c r="F12" s="83"/>
-      <c r="G12" s="178" t="s">
+      <c r="G12" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="178"/>
-      <c r="I12" s="178"/>
-      <c r="J12" s="177">
+      <c r="H12" s="173"/>
+      <c r="I12" s="173"/>
+      <c r="J12" s="158">
         <v>0.375</v>
       </c>
-      <c r="K12" s="177"/>
-      <c r="L12" s="177"/>
-      <c r="M12" s="177">
+      <c r="K12" s="158"/>
+      <c r="L12" s="158"/>
+      <c r="M12" s="158">
         <v>0.5</v>
       </c>
-      <c r="N12" s="177"/>
-      <c r="O12" s="177"/>
-      <c r="P12" s="177">
+      <c r="N12" s="158"/>
+      <c r="O12" s="158"/>
+      <c r="P12" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q12" s="177"/>
-      <c r="R12" s="177"/>
-      <c r="S12" s="177">
+      <c r="Q12" s="158"/>
+      <c r="R12" s="158"/>
+      <c r="S12" s="158">
         <v>0.72916666666666663</v>
       </c>
-      <c r="T12" s="177"/>
-      <c r="U12" s="177"/>
-      <c r="V12" s="159">
+      <c r="T12" s="158"/>
+      <c r="U12" s="158"/>
+      <c r="V12" s="172">
         <f t="shared" si="7"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="W12" s="159"/>
-      <c r="X12" s="159"/>
-      <c r="Y12" s="178" t="s">
+      <c r="W12" s="172"/>
+      <c r="X12" s="172"/>
+      <c r="Y12" s="173" t="s">
         <v>6</v>
       </c>
-      <c r="Z12" s="178"/>
-      <c r="AA12" s="178"/>
-      <c r="AB12" s="177">
+      <c r="Z12" s="173"/>
+      <c r="AA12" s="173"/>
+      <c r="AB12" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC12" s="177"/>
-      <c r="AD12" s="177"/>
-      <c r="AE12" s="180">
+      <c r="AC12" s="158"/>
+      <c r="AD12" s="158"/>
+      <c r="AE12" s="194">
         <v>0.5</v>
       </c>
-      <c r="AF12" s="181"/>
-      <c r="AG12" s="182"/>
-      <c r="AH12" s="177">
+      <c r="AF12" s="195"/>
+      <c r="AG12" s="196"/>
+      <c r="AH12" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI12" s="177"/>
-      <c r="AJ12" s="177"/>
-      <c r="AK12" s="177">
+      <c r="AI12" s="158"/>
+      <c r="AJ12" s="158"/>
+      <c r="AK12" s="158">
         <v>0.6875</v>
       </c>
-      <c r="AL12" s="177"/>
-      <c r="AM12" s="177"/>
-      <c r="AN12" s="159">
+      <c r="AL12" s="158"/>
+      <c r="AM12" s="158"/>
+      <c r="AN12" s="172">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO12" s="159"/>
-      <c r="AP12" s="159"/>
+      <c r="AO12" s="172"/>
+      <c r="AP12" s="172"/>
       <c r="AQ12" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333326</v>
@@ -3019,68 +3019,68 @@
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
       <c r="F13" s="83"/>
-      <c r="G13" s="178" t="s">
+      <c r="G13" s="173" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="178"/>
-      <c r="I13" s="178"/>
-      <c r="J13" s="177">
+      <c r="H13" s="173"/>
+      <c r="I13" s="173"/>
+      <c r="J13" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K13" s="177"/>
-      <c r="L13" s="177"/>
-      <c r="M13" s="177">
+      <c r="K13" s="158"/>
+      <c r="L13" s="158"/>
+      <c r="M13" s="158">
         <v>0.5</v>
       </c>
-      <c r="N13" s="177"/>
-      <c r="O13" s="177"/>
-      <c r="P13" s="177">
+      <c r="N13" s="158"/>
+      <c r="O13" s="158"/>
+      <c r="P13" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q13" s="177"/>
-      <c r="R13" s="177"/>
-      <c r="S13" s="177">
+      <c r="Q13" s="158"/>
+      <c r="R13" s="158"/>
+      <c r="S13" s="158">
         <v>0.6875</v>
       </c>
-      <c r="T13" s="177"/>
-      <c r="U13" s="177"/>
-      <c r="V13" s="159">
+      <c r="T13" s="158"/>
+      <c r="U13" s="158"/>
+      <c r="V13" s="172">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W13" s="159"/>
-      <c r="X13" s="159"/>
-      <c r="Y13" s="178" t="s">
+      <c r="W13" s="172"/>
+      <c r="X13" s="172"/>
+      <c r="Y13" s="173" t="s">
         <v>7</v>
       </c>
-      <c r="Z13" s="178"/>
-      <c r="AA13" s="178"/>
-      <c r="AB13" s="177">
+      <c r="Z13" s="173"/>
+      <c r="AA13" s="173"/>
+      <c r="AB13" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC13" s="177"/>
-      <c r="AD13" s="177"/>
-      <c r="AE13" s="180">
+      <c r="AC13" s="158"/>
+      <c r="AD13" s="158"/>
+      <c r="AE13" s="194">
         <v>0.5</v>
       </c>
-      <c r="AF13" s="181"/>
-      <c r="AG13" s="182"/>
-      <c r="AH13" s="177">
+      <c r="AF13" s="195"/>
+      <c r="AG13" s="196"/>
+      <c r="AH13" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI13" s="177"/>
-      <c r="AJ13" s="177"/>
-      <c r="AK13" s="177">
+      <c r="AI13" s="158"/>
+      <c r="AJ13" s="158"/>
+      <c r="AK13" s="158">
         <v>0.6875</v>
       </c>
-      <c r="AL13" s="177"/>
-      <c r="AM13" s="177"/>
-      <c r="AN13" s="159">
+      <c r="AL13" s="158"/>
+      <c r="AM13" s="158"/>
+      <c r="AN13" s="172">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO13" s="159"/>
-      <c r="AP13" s="159"/>
+      <c r="AO13" s="172"/>
+      <c r="AP13" s="172"/>
       <c r="AQ13" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3130,68 +3130,68 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="56"/>
-      <c r="G14" s="178" t="s">
+      <c r="G14" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="178"/>
-      <c r="I14" s="178"/>
-      <c r="J14" s="177">
+      <c r="H14" s="173"/>
+      <c r="I14" s="173"/>
+      <c r="J14" s="158">
         <v>0.34375</v>
       </c>
-      <c r="K14" s="177"/>
-      <c r="L14" s="177"/>
-      <c r="M14" s="177">
+      <c r="K14" s="158"/>
+      <c r="L14" s="158"/>
+      <c r="M14" s="158">
         <v>0.5</v>
       </c>
-      <c r="N14" s="177"/>
-      <c r="O14" s="177"/>
-      <c r="P14" s="177">
+      <c r="N14" s="158"/>
+      <c r="O14" s="158"/>
+      <c r="P14" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q14" s="177"/>
-      <c r="R14" s="177"/>
-      <c r="S14" s="177">
+      <c r="Q14" s="158"/>
+      <c r="R14" s="158"/>
+      <c r="S14" s="158">
         <v>0.69791666666666663</v>
       </c>
-      <c r="T14" s="177"/>
-      <c r="U14" s="177"/>
-      <c r="V14" s="159">
+      <c r="T14" s="158"/>
+      <c r="U14" s="158"/>
+      <c r="V14" s="172">
         <f t="shared" si="7"/>
         <v>0.33333333333333326</v>
       </c>
-      <c r="W14" s="159"/>
-      <c r="X14" s="159"/>
-      <c r="Y14" s="178" t="s">
+      <c r="W14" s="172"/>
+      <c r="X14" s="172"/>
+      <c r="Y14" s="173" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="178"/>
-      <c r="AA14" s="178"/>
-      <c r="AB14" s="177">
+      <c r="Z14" s="173"/>
+      <c r="AA14" s="173"/>
+      <c r="AB14" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC14" s="177"/>
-      <c r="AD14" s="177"/>
-      <c r="AE14" s="180">
+      <c r="AC14" s="158"/>
+      <c r="AD14" s="158"/>
+      <c r="AE14" s="194">
         <v>0.5</v>
       </c>
-      <c r="AF14" s="181"/>
-      <c r="AG14" s="182"/>
-      <c r="AH14" s="177">
+      <c r="AF14" s="195"/>
+      <c r="AG14" s="196"/>
+      <c r="AH14" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI14" s="177"/>
-      <c r="AJ14" s="177"/>
-      <c r="AK14" s="177">
+      <c r="AI14" s="158"/>
+      <c r="AJ14" s="158"/>
+      <c r="AK14" s="158">
         <v>0.6875</v>
       </c>
-      <c r="AL14" s="177"/>
-      <c r="AM14" s="177"/>
-      <c r="AN14" s="159">
+      <c r="AL14" s="158"/>
+      <c r="AM14" s="158"/>
+      <c r="AN14" s="172">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO14" s="159"/>
-      <c r="AP14" s="159"/>
+      <c r="AO14" s="172"/>
+      <c r="AP14" s="172"/>
       <c r="AQ14" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333326</v>
@@ -3241,68 +3241,68 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="56"/>
-      <c r="G15" s="178" t="s">
+      <c r="G15" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="178"/>
-      <c r="I15" s="178"/>
-      <c r="J15" s="177">
+      <c r="H15" s="173"/>
+      <c r="I15" s="173"/>
+      <c r="J15" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K15" s="177"/>
-      <c r="L15" s="177"/>
-      <c r="M15" s="177">
+      <c r="K15" s="158"/>
+      <c r="L15" s="158"/>
+      <c r="M15" s="158">
         <v>0.5</v>
       </c>
-      <c r="N15" s="177"/>
-      <c r="O15" s="177"/>
-      <c r="P15" s="177">
+      <c r="N15" s="158"/>
+      <c r="O15" s="158"/>
+      <c r="P15" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q15" s="177"/>
-      <c r="R15" s="177"/>
-      <c r="S15" s="177">
+      <c r="Q15" s="158"/>
+      <c r="R15" s="158"/>
+      <c r="S15" s="158">
         <v>0.6875</v>
       </c>
-      <c r="T15" s="177"/>
-      <c r="U15" s="177"/>
-      <c r="V15" s="159">
+      <c r="T15" s="158"/>
+      <c r="U15" s="158"/>
+      <c r="V15" s="172">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W15" s="159"/>
-      <c r="X15" s="159"/>
-      <c r="Y15" s="178" t="s">
+      <c r="W15" s="172"/>
+      <c r="X15" s="172"/>
+      <c r="Y15" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="Z15" s="178"/>
-      <c r="AA15" s="178"/>
-      <c r="AB15" s="177">
+      <c r="Z15" s="173"/>
+      <c r="AA15" s="173"/>
+      <c r="AB15" s="158">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC15" s="177"/>
-      <c r="AD15" s="177"/>
-      <c r="AE15" s="180">
+      <c r="AC15" s="158"/>
+      <c r="AD15" s="158"/>
+      <c r="AE15" s="194">
         <v>0.5</v>
       </c>
-      <c r="AF15" s="181"/>
-      <c r="AG15" s="182"/>
-      <c r="AH15" s="177">
+      <c r="AF15" s="195"/>
+      <c r="AG15" s="196"/>
+      <c r="AH15" s="158">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI15" s="177"/>
-      <c r="AJ15" s="177"/>
-      <c r="AK15" s="177">
+      <c r="AI15" s="158"/>
+      <c r="AJ15" s="158"/>
+      <c r="AK15" s="158">
         <v>0.6875</v>
       </c>
-      <c r="AL15" s="177"/>
-      <c r="AM15" s="177"/>
-      <c r="AN15" s="159">
+      <c r="AL15" s="158"/>
+      <c r="AM15" s="158"/>
+      <c r="AN15" s="172">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO15" s="159"/>
-      <c r="AP15" s="159"/>
+      <c r="AO15" s="172"/>
+      <c r="AP15" s="172"/>
       <c r="AQ15" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3352,52 +3352,52 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="55"/>
-      <c r="G16" s="178" t="s">
+      <c r="G16" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="178"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="177"/>
-      <c r="K16" s="177"/>
-      <c r="L16" s="177"/>
-      <c r="M16" s="177"/>
-      <c r="N16" s="177"/>
-      <c r="O16" s="177"/>
-      <c r="P16" s="177"/>
-      <c r="Q16" s="177"/>
-      <c r="R16" s="177"/>
-      <c r="S16" s="177"/>
-      <c r="T16" s="177"/>
-      <c r="U16" s="177"/>
-      <c r="V16" s="159">
+      <c r="H16" s="173"/>
+      <c r="I16" s="173"/>
+      <c r="J16" s="158"/>
+      <c r="K16" s="158"/>
+      <c r="L16" s="158"/>
+      <c r="M16" s="158"/>
+      <c r="N16" s="158"/>
+      <c r="O16" s="158"/>
+      <c r="P16" s="158"/>
+      <c r="Q16" s="158"/>
+      <c r="R16" s="158"/>
+      <c r="S16" s="158"/>
+      <c r="T16" s="158"/>
+      <c r="U16" s="158"/>
+      <c r="V16" s="172">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W16" s="159"/>
-      <c r="X16" s="159"/>
-      <c r="Y16" s="178" t="s">
+      <c r="W16" s="172"/>
+      <c r="X16" s="172"/>
+      <c r="Y16" s="173" t="s">
         <v>10</v>
       </c>
-      <c r="Z16" s="178"/>
-      <c r="AA16" s="178"/>
-      <c r="AB16" s="177"/>
-      <c r="AC16" s="177"/>
-      <c r="AD16" s="177"/>
-      <c r="AE16" s="177"/>
-      <c r="AF16" s="177"/>
-      <c r="AG16" s="177"/>
-      <c r="AH16" s="177"/>
-      <c r="AI16" s="177"/>
-      <c r="AJ16" s="177"/>
-      <c r="AK16" s="177"/>
-      <c r="AL16" s="177"/>
-      <c r="AM16" s="177"/>
-      <c r="AN16" s="159">
+      <c r="Z16" s="173"/>
+      <c r="AA16" s="173"/>
+      <c r="AB16" s="158"/>
+      <c r="AC16" s="158"/>
+      <c r="AD16" s="158"/>
+      <c r="AE16" s="158"/>
+      <c r="AF16" s="158"/>
+      <c r="AG16" s="158"/>
+      <c r="AH16" s="158"/>
+      <c r="AI16" s="158"/>
+      <c r="AJ16" s="158"/>
+      <c r="AK16" s="158"/>
+      <c r="AL16" s="158"/>
+      <c r="AM16" s="158"/>
+      <c r="AN16" s="172">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="159"/>
-      <c r="AP16" s="159"/>
+      <c r="AO16" s="172"/>
+      <c r="AP16" s="172"/>
       <c r="AQ16" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3551,50 +3551,50 @@
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
-      <c r="G19" s="186"/>
-      <c r="H19" s="186"/>
-      <c r="I19" s="186"/>
-      <c r="J19" s="186"/>
-      <c r="K19" s="186"/>
-      <c r="L19" s="186"/>
-      <c r="M19" s="186"/>
-      <c r="N19" s="186"/>
-      <c r="O19" s="186"/>
-      <c r="P19" s="186"/>
-      <c r="Q19" s="186"/>
+      <c r="G19" s="201"/>
+      <c r="H19" s="201"/>
+      <c r="I19" s="201"/>
+      <c r="J19" s="201"/>
+      <c r="K19" s="201"/>
+      <c r="L19" s="201"/>
+      <c r="M19" s="201"/>
+      <c r="N19" s="201"/>
+      <c r="O19" s="201"/>
+      <c r="P19" s="201"/>
+      <c r="Q19" s="201"/>
       <c r="R19" s="62"/>
-      <c r="S19" s="184" t="s">
+      <c r="S19" s="206" t="s">
         <v>62</v>
       </c>
-      <c r="T19" s="184"/>
-      <c r="U19" s="184"/>
-      <c r="V19" s="184"/>
-      <c r="W19" s="184"/>
-      <c r="Y19" s="184">
+      <c r="T19" s="206"/>
+      <c r="U19" s="206"/>
+      <c r="V19" s="206"/>
+      <c r="W19" s="206"/>
+      <c r="Y19" s="206">
         <v>41862</v>
       </c>
-      <c r="Z19" s="188"/>
-      <c r="AA19" s="188"/>
-      <c r="AB19" s="188"/>
-      <c r="AD19" s="168" t="s">
+      <c r="Z19" s="207"/>
+      <c r="AA19" s="207"/>
+      <c r="AB19" s="207"/>
+      <c r="AD19" s="217" t="s">
         <v>33</v>
       </c>
-      <c r="AE19" s="169"/>
-      <c r="AF19" s="169"/>
-      <c r="AG19" s="169"/>
-      <c r="AH19" s="170"/>
-      <c r="AI19" s="166" t="s">
+      <c r="AE19" s="218"/>
+      <c r="AF19" s="218"/>
+      <c r="AG19" s="218"/>
+      <c r="AH19" s="219"/>
+      <c r="AI19" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="AJ19" s="167"/>
-      <c r="AK19" s="167"/>
-      <c r="AL19" s="167"/>
-      <c r="AM19" s="167"/>
-      <c r="AO19" s="162">
+      <c r="AJ19" s="157"/>
+      <c r="AK19" s="157"/>
+      <c r="AL19" s="157"/>
+      <c r="AM19" s="157"/>
+      <c r="AO19" s="210">
         <f>+AQ19+AW19</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="AP19" s="163"/>
+      <c r="AP19" s="211"/>
       <c r="AQ19" s="26">
         <f>MIN(SUM(AQ10:AQ16),40/24)</f>
         <v>1.333333333333333</v>
@@ -3620,33 +3620,33 @@
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
-      <c r="G20" s="187"/>
-      <c r="H20" s="187"/>
-      <c r="I20" s="187"/>
-      <c r="J20" s="187"/>
-      <c r="K20" s="187"/>
-      <c r="L20" s="187"/>
-      <c r="M20" s="187"/>
-      <c r="N20" s="187"/>
-      <c r="O20" s="187"/>
-      <c r="P20" s="187"/>
-      <c r="Q20" s="187"/>
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202"/>
+      <c r="J20" s="202"/>
+      <c r="K20" s="202"/>
+      <c r="L20" s="202"/>
+      <c r="M20" s="202"/>
+      <c r="N20" s="202"/>
+      <c r="O20" s="202"/>
+      <c r="P20" s="202"/>
+      <c r="Q20" s="202"/>
       <c r="R20" s="63"/>
-      <c r="S20" s="185"/>
-      <c r="T20" s="185"/>
-      <c r="U20" s="185"/>
-      <c r="V20" s="185"/>
-      <c r="W20" s="185"/>
-      <c r="Y20" s="189"/>
-      <c r="Z20" s="189"/>
-      <c r="AA20" s="189"/>
-      <c r="AB20" s="189"/>
+      <c r="S20" s="205"/>
+      <c r="T20" s="205"/>
+      <c r="U20" s="205"/>
+      <c r="V20" s="205"/>
+      <c r="W20" s="205"/>
+      <c r="Y20" s="160"/>
+      <c r="Z20" s="160"/>
+      <c r="AA20" s="160"/>
+      <c r="AB20" s="160"/>
       <c r="AC20" s="48"/>
-      <c r="AD20" s="171"/>
-      <c r="AE20" s="172"/>
-      <c r="AF20" s="172"/>
-      <c r="AG20" s="172"/>
-      <c r="AH20" s="173"/>
+      <c r="AD20" s="220"/>
+      <c r="AE20" s="221"/>
+      <c r="AF20" s="221"/>
+      <c r="AG20" s="221"/>
+      <c r="AH20" s="222"/>
       <c r="AM20" s="66"/>
       <c r="AO20" s="65"/>
       <c r="AP20" s="65"/>
@@ -3683,35 +3683,35 @@
       <c r="P21" s="35"/>
       <c r="Q21" s="50"/>
       <c r="R21" s="35"/>
-      <c r="S21" s="183" t="s">
+      <c r="S21" s="208" t="s">
         <v>28</v>
       </c>
-      <c r="T21" s="183"/>
-      <c r="U21" s="183"/>
-      <c r="V21" s="183"/>
-      <c r="W21" s="183"/>
-      <c r="Y21" s="228" t="s">
+      <c r="T21" s="208"/>
+      <c r="U21" s="208"/>
+      <c r="V21" s="208"/>
+      <c r="W21" s="208"/>
+      <c r="Y21" s="171" t="s">
         <v>26</v>
       </c>
-      <c r="Z21" s="228"/>
-      <c r="AA21" s="228"/>
-      <c r="AD21" s="171"/>
-      <c r="AE21" s="172"/>
-      <c r="AF21" s="172"/>
-      <c r="AG21" s="172"/>
-      <c r="AH21" s="173"/>
-      <c r="AI21" s="166" t="s">
+      <c r="Z21" s="171"/>
+      <c r="AA21" s="171"/>
+      <c r="AD21" s="220"/>
+      <c r="AE21" s="221"/>
+      <c r="AF21" s="221"/>
+      <c r="AG21" s="221"/>
+      <c r="AH21" s="222"/>
+      <c r="AI21" s="156" t="s">
         <v>24</v>
       </c>
-      <c r="AJ21" s="167"/>
-      <c r="AK21" s="167"/>
-      <c r="AL21" s="167"/>
-      <c r="AM21" s="167"/>
-      <c r="AO21" s="162">
+      <c r="AJ21" s="157"/>
+      <c r="AK21" s="157"/>
+      <c r="AL21" s="157"/>
+      <c r="AM21" s="157"/>
+      <c r="AO21" s="210">
         <f>+AR21+AX21</f>
         <v>0</v>
       </c>
-      <c r="AP21" s="163"/>
+      <c r="AP21" s="211"/>
       <c r="AQ21" s="19"/>
       <c r="AR21" s="20">
         <f>SUM(AR10:AR16)+MAX(0,SUM(AQ10:AQ16)-40/24)</f>
@@ -3757,11 +3757,11 @@
       <c r="Y22" s="51"/>
       <c r="Z22" s="51"/>
       <c r="AA22" s="51"/>
-      <c r="AD22" s="171"/>
-      <c r="AE22" s="172"/>
-      <c r="AF22" s="172"/>
-      <c r="AG22" s="172"/>
-      <c r="AH22" s="173"/>
+      <c r="AD22" s="220"/>
+      <c r="AE22" s="221"/>
+      <c r="AF22" s="221"/>
+      <c r="AG22" s="221"/>
+      <c r="AH22" s="222"/>
       <c r="AL22" s="28"/>
       <c r="AM22" s="66"/>
       <c r="AN22" s="23"/>
@@ -3780,32 +3780,32 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:59" ht="3.75" customHeight="1" thickBot="1">
-      <c r="G23" s="190" t="s">
+      <c r="G23" s="203" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="190"/>
-      <c r="I23" s="190"/>
-      <c r="J23" s="190"/>
-      <c r="K23" s="190"/>
-      <c r="L23" s="190"/>
-      <c r="M23" s="190"/>
-      <c r="N23" s="190"/>
-      <c r="O23" s="190"/>
-      <c r="P23" s="190"/>
-      <c r="Q23" s="190"/>
-      <c r="R23" s="190"/>
-      <c r="S23" s="190"/>
-      <c r="T23" s="190"/>
-      <c r="U23" s="190"/>
-      <c r="V23" s="190"/>
-      <c r="W23" s="190"/>
-      <c r="X23" s="190"/>
+      <c r="H23" s="203"/>
+      <c r="I23" s="203"/>
+      <c r="J23" s="203"/>
+      <c r="K23" s="203"/>
+      <c r="L23" s="203"/>
+      <c r="M23" s="203"/>
+      <c r="N23" s="203"/>
+      <c r="O23" s="203"/>
+      <c r="P23" s="203"/>
+      <c r="Q23" s="203"/>
+      <c r="R23" s="203"/>
+      <c r="S23" s="203"/>
+      <c r="T23" s="203"/>
+      <c r="U23" s="203"/>
+      <c r="V23" s="203"/>
+      <c r="W23" s="203"/>
+      <c r="X23" s="203"/>
       <c r="AC23" s="48"/>
-      <c r="AD23" s="171"/>
-      <c r="AE23" s="172"/>
-      <c r="AF23" s="172"/>
-      <c r="AG23" s="172"/>
-      <c r="AH23" s="173"/>
+      <c r="AD23" s="220"/>
+      <c r="AE23" s="221"/>
+      <c r="AF23" s="221"/>
+      <c r="AG23" s="221"/>
+      <c r="AH23" s="222"/>
       <c r="AM23" s="66"/>
       <c r="AO23" s="65"/>
       <c r="AP23" s="65"/>
@@ -3822,41 +3822,41 @@
       <c r="BA23" s="6"/>
     </row>
     <row r="24" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
-      <c r="G24" s="190"/>
-      <c r="H24" s="190"/>
-      <c r="I24" s="190"/>
-      <c r="J24" s="190"/>
-      <c r="K24" s="190"/>
-      <c r="L24" s="190"/>
-      <c r="M24" s="190"/>
-      <c r="N24" s="190"/>
-      <c r="O24" s="190"/>
-      <c r="P24" s="190"/>
-      <c r="Q24" s="190"/>
-      <c r="R24" s="190"/>
-      <c r="S24" s="190"/>
-      <c r="T24" s="190"/>
-      <c r="U24" s="190"/>
-      <c r="V24" s="190"/>
-      <c r="W24" s="190"/>
-      <c r="X24" s="190"/>
-      <c r="AD24" s="171"/>
-      <c r="AE24" s="172"/>
-      <c r="AF24" s="172"/>
-      <c r="AG24" s="172"/>
-      <c r="AH24" s="173"/>
-      <c r="AI24" s="166" t="s">
+      <c r="G24" s="203"/>
+      <c r="H24" s="203"/>
+      <c r="I24" s="203"/>
+      <c r="J24" s="203"/>
+      <c r="K24" s="203"/>
+      <c r="L24" s="203"/>
+      <c r="M24" s="203"/>
+      <c r="N24" s="203"/>
+      <c r="O24" s="203"/>
+      <c r="P24" s="203"/>
+      <c r="Q24" s="203"/>
+      <c r="R24" s="203"/>
+      <c r="S24" s="203"/>
+      <c r="T24" s="203"/>
+      <c r="U24" s="203"/>
+      <c r="V24" s="203"/>
+      <c r="W24" s="203"/>
+      <c r="X24" s="203"/>
+      <c r="AD24" s="220"/>
+      <c r="AE24" s="221"/>
+      <c r="AF24" s="221"/>
+      <c r="AG24" s="221"/>
+      <c r="AH24" s="222"/>
+      <c r="AI24" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="AJ24" s="167"/>
-      <c r="AK24" s="167"/>
-      <c r="AL24" s="167"/>
-      <c r="AM24" s="167"/>
-      <c r="AO24" s="162">
+      <c r="AJ24" s="157"/>
+      <c r="AK24" s="157"/>
+      <c r="AL24" s="157"/>
+      <c r="AM24" s="157"/>
+      <c r="AO24" s="210">
         <f>+AS24+AY24</f>
         <v>0</v>
       </c>
-      <c r="AP24" s="163"/>
+      <c r="AP24" s="211"/>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="19"/>
       <c r="AS24" s="20">
@@ -3876,30 +3876,30 @@
       <c r="BA24" s="6"/>
     </row>
     <row r="25" spans="1:59" ht="6.75" customHeight="1" thickBot="1">
-      <c r="G25" s="190"/>
-      <c r="H25" s="190"/>
-      <c r="I25" s="190"/>
-      <c r="J25" s="190"/>
-      <c r="K25" s="190"/>
-      <c r="L25" s="190"/>
-      <c r="M25" s="190"/>
-      <c r="N25" s="190"/>
-      <c r="O25" s="190"/>
-      <c r="P25" s="190"/>
-      <c r="Q25" s="190"/>
-      <c r="R25" s="190"/>
-      <c r="S25" s="190"/>
-      <c r="T25" s="190"/>
-      <c r="U25" s="190"/>
-      <c r="V25" s="190"/>
-      <c r="W25" s="190"/>
-      <c r="X25" s="190"/>
+      <c r="G25" s="203"/>
+      <c r="H25" s="203"/>
+      <c r="I25" s="203"/>
+      <c r="J25" s="203"/>
+      <c r="K25" s="203"/>
+      <c r="L25" s="203"/>
+      <c r="M25" s="203"/>
+      <c r="N25" s="203"/>
+      <c r="O25" s="203"/>
+      <c r="P25" s="203"/>
+      <c r="Q25" s="203"/>
+      <c r="R25" s="203"/>
+      <c r="S25" s="203"/>
+      <c r="T25" s="203"/>
+      <c r="U25" s="203"/>
+      <c r="V25" s="203"/>
+      <c r="W25" s="203"/>
+      <c r="X25" s="203"/>
       <c r="AC25" s="48"/>
-      <c r="AD25" s="171"/>
-      <c r="AE25" s="172"/>
-      <c r="AF25" s="172"/>
-      <c r="AG25" s="172"/>
-      <c r="AH25" s="173"/>
+      <c r="AD25" s="220"/>
+      <c r="AE25" s="221"/>
+      <c r="AF25" s="221"/>
+      <c r="AG25" s="221"/>
+      <c r="AH25" s="222"/>
       <c r="AM25" s="66"/>
       <c r="AO25" s="65"/>
       <c r="AP25" s="65"/>
@@ -3922,45 +3922,45 @@
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
-      <c r="G26" s="186"/>
-      <c r="H26" s="186"/>
-      <c r="I26" s="186"/>
-      <c r="J26" s="186"/>
-      <c r="K26" s="186"/>
-      <c r="L26" s="186"/>
-      <c r="M26" s="186"/>
-      <c r="N26" s="186"/>
-      <c r="O26" s="186"/>
-      <c r="P26" s="186"/>
-      <c r="Q26" s="186"/>
+      <c r="G26" s="201"/>
+      <c r="H26" s="201"/>
+      <c r="I26" s="201"/>
+      <c r="J26" s="201"/>
+      <c r="K26" s="201"/>
+      <c r="L26" s="201"/>
+      <c r="M26" s="201"/>
+      <c r="N26" s="201"/>
+      <c r="O26" s="201"/>
+      <c r="P26" s="201"/>
+      <c r="Q26" s="201"/>
       <c r="R26" s="64"/>
-      <c r="S26" s="191"/>
-      <c r="T26" s="191"/>
-      <c r="U26" s="191"/>
-      <c r="V26" s="191"/>
-      <c r="W26" s="191"/>
+      <c r="S26" s="204"/>
+      <c r="T26" s="204"/>
+      <c r="U26" s="204"/>
+      <c r="V26" s="204"/>
+      <c r="W26" s="204"/>
       <c r="X26" s="35"/>
-      <c r="Y26" s="219"/>
-      <c r="Z26" s="219"/>
-      <c r="AA26" s="219"/>
-      <c r="AB26" s="219"/>
-      <c r="AD26" s="171"/>
-      <c r="AE26" s="172"/>
-      <c r="AF26" s="172"/>
-      <c r="AG26" s="172"/>
-      <c r="AH26" s="173"/>
-      <c r="AI26" s="166" t="s">
+      <c r="Y26" s="159"/>
+      <c r="Z26" s="159"/>
+      <c r="AA26" s="159"/>
+      <c r="AB26" s="159"/>
+      <c r="AD26" s="220"/>
+      <c r="AE26" s="221"/>
+      <c r="AF26" s="221"/>
+      <c r="AG26" s="221"/>
+      <c r="AH26" s="222"/>
+      <c r="AI26" s="156" t="s">
         <v>22</v>
       </c>
-      <c r="AJ26" s="167"/>
-      <c r="AK26" s="167"/>
-      <c r="AL26" s="167"/>
-      <c r="AM26" s="167"/>
-      <c r="AO26" s="160">
+      <c r="AJ26" s="157"/>
+      <c r="AK26" s="157"/>
+      <c r="AL26" s="157"/>
+      <c r="AM26" s="157"/>
+      <c r="AO26" s="213">
         <f>AT26+AZ26</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="AP26" s="161"/>
+      <c r="AP26" s="214"/>
       <c r="AQ26" s="19"/>
       <c r="AR26" s="19"/>
       <c r="AS26" s="19"/>
@@ -3986,33 +3986,33 @@
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
-      <c r="G27" s="186"/>
-      <c r="H27" s="186"/>
-      <c r="I27" s="186"/>
-      <c r="J27" s="186"/>
-      <c r="K27" s="186"/>
-      <c r="L27" s="186"/>
-      <c r="M27" s="186"/>
-      <c r="N27" s="186"/>
-      <c r="O27" s="186"/>
-      <c r="P27" s="186"/>
-      <c r="Q27" s="186"/>
+      <c r="G27" s="201"/>
+      <c r="H27" s="201"/>
+      <c r="I27" s="201"/>
+      <c r="J27" s="201"/>
+      <c r="K27" s="201"/>
+      <c r="L27" s="201"/>
+      <c r="M27" s="201"/>
+      <c r="N27" s="201"/>
+      <c r="O27" s="201"/>
+      <c r="P27" s="201"/>
+      <c r="Q27" s="201"/>
       <c r="R27" s="64"/>
-      <c r="S27" s="191"/>
-      <c r="T27" s="191"/>
-      <c r="U27" s="191"/>
-      <c r="V27" s="191"/>
-      <c r="W27" s="191"/>
+      <c r="S27" s="204"/>
+      <c r="T27" s="204"/>
+      <c r="U27" s="204"/>
+      <c r="V27" s="204"/>
+      <c r="W27" s="204"/>
       <c r="X27" s="35"/>
-      <c r="Y27" s="219"/>
-      <c r="Z27" s="219"/>
-      <c r="AA27" s="219"/>
-      <c r="AB27" s="219"/>
-      <c r="AD27" s="171"/>
-      <c r="AE27" s="172"/>
-      <c r="AF27" s="172"/>
-      <c r="AG27" s="172"/>
-      <c r="AH27" s="173"/>
+      <c r="Y27" s="159"/>
+      <c r="Z27" s="159"/>
+      <c r="AA27" s="159"/>
+      <c r="AB27" s="159"/>
+      <c r="AD27" s="220"/>
+      <c r="AE27" s="221"/>
+      <c r="AF27" s="221"/>
+      <c r="AG27" s="221"/>
+      <c r="AH27" s="222"/>
       <c r="AM27" s="74"/>
       <c r="AO27" s="76"/>
       <c r="AP27" s="76"/>
@@ -4029,43 +4029,43 @@
       <c r="BA27" s="6"/>
     </row>
     <row r="28" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
-      <c r="G28" s="187"/>
-      <c r="H28" s="187"/>
-      <c r="I28" s="187"/>
-      <c r="J28" s="187"/>
-      <c r="K28" s="187"/>
-      <c r="L28" s="187"/>
-      <c r="M28" s="187"/>
-      <c r="N28" s="187"/>
-      <c r="O28" s="187"/>
-      <c r="P28" s="187"/>
-      <c r="Q28" s="187"/>
+      <c r="G28" s="202"/>
+      <c r="H28" s="202"/>
+      <c r="I28" s="202"/>
+      <c r="J28" s="202"/>
+      <c r="K28" s="202"/>
+      <c r="L28" s="202"/>
+      <c r="M28" s="202"/>
+      <c r="N28" s="202"/>
+      <c r="O28" s="202"/>
+      <c r="P28" s="202"/>
+      <c r="Q28" s="202"/>
       <c r="R28" s="35"/>
-      <c r="S28" s="185"/>
-      <c r="T28" s="185"/>
-      <c r="U28" s="185"/>
-      <c r="V28" s="185"/>
-      <c r="W28" s="185"/>
+      <c r="S28" s="205"/>
+      <c r="T28" s="205"/>
+      <c r="U28" s="205"/>
+      <c r="V28" s="205"/>
+      <c r="W28" s="205"/>
       <c r="X28" s="35"/>
-      <c r="Y28" s="189"/>
-      <c r="Z28" s="189"/>
-      <c r="AA28" s="189"/>
-      <c r="AB28" s="189"/>
+      <c r="Y28" s="160"/>
+      <c r="Z28" s="160"/>
+      <c r="AA28" s="160"/>
+      <c r="AB28" s="160"/>
       <c r="AC28" s="52"/>
-      <c r="AD28" s="171"/>
-      <c r="AE28" s="172"/>
-      <c r="AF28" s="172"/>
-      <c r="AG28" s="172"/>
-      <c r="AH28" s="173"/>
-      <c r="AI28" s="166" t="s">
+      <c r="AD28" s="220"/>
+      <c r="AE28" s="221"/>
+      <c r="AF28" s="221"/>
+      <c r="AG28" s="221"/>
+      <c r="AH28" s="222"/>
+      <c r="AI28" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="AJ28" s="167"/>
-      <c r="AK28" s="167"/>
-      <c r="AL28" s="167"/>
-      <c r="AM28" s="167"/>
-      <c r="AO28" s="164"/>
-      <c r="AP28" s="165"/>
+      <c r="AJ28" s="157"/>
+      <c r="AK28" s="157"/>
+      <c r="AL28" s="157"/>
+      <c r="AM28" s="157"/>
+      <c r="AO28" s="215"/>
+      <c r="AP28" s="216"/>
       <c r="AQ28" s="19"/>
       <c r="AR28" s="19"/>
       <c r="AS28" s="19"/>
@@ -4093,25 +4093,25 @@
       <c r="O29" s="35"/>
       <c r="P29" s="35"/>
       <c r="R29" s="35"/>
-      <c r="S29" s="158" t="s">
+      <c r="S29" s="212" t="s">
         <v>29</v>
       </c>
-      <c r="T29" s="158"/>
-      <c r="U29" s="158"/>
-      <c r="V29" s="158"/>
-      <c r="W29" s="158"/>
+      <c r="T29" s="212"/>
+      <c r="U29" s="212"/>
+      <c r="V29" s="212"/>
+      <c r="W29" s="212"/>
       <c r="X29" s="35"/>
-      <c r="Y29" s="179" t="s">
+      <c r="Y29" s="209" t="s">
         <v>26</v>
       </c>
-      <c r="Z29" s="179"/>
-      <c r="AA29" s="179"/>
+      <c r="Z29" s="209"/>
+      <c r="AA29" s="209"/>
       <c r="AC29" s="52"/>
-      <c r="AD29" s="174"/>
-      <c r="AE29" s="175"/>
-      <c r="AF29" s="175"/>
-      <c r="AG29" s="175"/>
-      <c r="AH29" s="176"/>
+      <c r="AD29" s="223"/>
+      <c r="AE29" s="224"/>
+      <c r="AF29" s="224"/>
+      <c r="AG29" s="224"/>
+      <c r="AH29" s="225"/>
       <c r="AO29" s="27"/>
       <c r="AP29" s="27"/>
       <c r="AQ29" s="19"/>
@@ -4182,88 +4182,88 @@
       <c r="BA31" s="102"/>
       <c r="BB31" s="102"/>
       <c r="BC31" s="92"/>
-      <c r="BD31" s="222" t="s">
+      <c r="BD31" s="163" t="s">
         <v>45</v>
       </c>
-      <c r="BE31" s="223"/>
-      <c r="BF31" s="229" t="s">
+      <c r="BE31" s="164"/>
+      <c r="BF31" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="BG31" s="230"/>
+      <c r="BG31" s="144"/>
     </row>
     <row r="32" spans="1:59" s="2" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B32" s="216" t="s">
+      <c r="B32" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="217"/>
-      <c r="D32" s="217"/>
-      <c r="E32" s="217"/>
-      <c r="F32" s="217"/>
-      <c r="G32" s="217"/>
-      <c r="H32" s="217"/>
-      <c r="I32" s="217"/>
-      <c r="J32" s="217"/>
-      <c r="K32" s="217"/>
-      <c r="L32" s="217"/>
-      <c r="M32" s="217"/>
-      <c r="N32" s="218"/>
-      <c r="O32" s="216" t="s">
+      <c r="C32" s="149"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="149"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="149"/>
+      <c r="I32" s="149"/>
+      <c r="J32" s="149"/>
+      <c r="K32" s="149"/>
+      <c r="L32" s="149"/>
+      <c r="M32" s="149"/>
+      <c r="N32" s="148"/>
+      <c r="O32" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="P32" s="218"/>
-      <c r="Q32" s="216" t="s">
+      <c r="P32" s="148"/>
+      <c r="Q32" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="R32" s="218"/>
-      <c r="S32" s="216" t="s">
+      <c r="R32" s="148"/>
+      <c r="S32" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="T32" s="217"/>
-      <c r="U32" s="217"/>
-      <c r="V32" s="218"/>
-      <c r="W32" s="216" t="s">
+      <c r="T32" s="149"/>
+      <c r="U32" s="149"/>
+      <c r="V32" s="148"/>
+      <c r="W32" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="X32" s="217"/>
-      <c r="Y32" s="217"/>
-      <c r="Z32" s="217"/>
-      <c r="AA32" s="217"/>
-      <c r="AB32" s="217"/>
-      <c r="AC32" s="217"/>
-      <c r="AD32" s="218"/>
-      <c r="AE32" s="233" t="s">
+      <c r="X32" s="149"/>
+      <c r="Y32" s="149"/>
+      <c r="Z32" s="149"/>
+      <c r="AA32" s="149"/>
+      <c r="AB32" s="149"/>
+      <c r="AC32" s="149"/>
+      <c r="AD32" s="148"/>
+      <c r="AE32" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="AF32" s="234"/>
-      <c r="AG32" s="234"/>
-      <c r="AH32" s="234"/>
-      <c r="AI32" s="234"/>
-      <c r="AJ32" s="234"/>
-      <c r="AK32" s="234"/>
-      <c r="AL32" s="234"/>
-      <c r="AM32" s="234"/>
-      <c r="AN32" s="235"/>
-      <c r="AO32" s="236" t="s">
+      <c r="AF32" s="151"/>
+      <c r="AG32" s="151"/>
+      <c r="AH32" s="151"/>
+      <c r="AI32" s="151"/>
+      <c r="AJ32" s="151"/>
+      <c r="AK32" s="151"/>
+      <c r="AL32" s="151"/>
+      <c r="AM32" s="151"/>
+      <c r="AN32" s="152"/>
+      <c r="AO32" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="AP32" s="237"/>
-      <c r="AQ32" s="237"/>
-      <c r="AR32" s="237"/>
-      <c r="AS32" s="237"/>
-      <c r="AT32" s="237"/>
-      <c r="AU32" s="237"/>
-      <c r="AV32" s="237"/>
-      <c r="AW32" s="237"/>
-      <c r="AX32" s="237"/>
-      <c r="AY32" s="237"/>
-      <c r="AZ32" s="237"/>
-      <c r="BA32" s="237"/>
-      <c r="BB32" s="237"/>
-      <c r="BC32" s="238"/>
-      <c r="BD32" s="224"/>
-      <c r="BE32" s="225"/>
-      <c r="BF32" s="231"/>
-      <c r="BG32" s="232"/>
+      <c r="AP32" s="154"/>
+      <c r="AQ32" s="154"/>
+      <c r="AR32" s="154"/>
+      <c r="AS32" s="154"/>
+      <c r="AT32" s="154"/>
+      <c r="AU32" s="154"/>
+      <c r="AV32" s="154"/>
+      <c r="AW32" s="154"/>
+      <c r="AX32" s="154"/>
+      <c r="AY32" s="154"/>
+      <c r="AZ32" s="154"/>
+      <c r="BA32" s="154"/>
+      <c r="BB32" s="154"/>
+      <c r="BC32" s="155"/>
+      <c r="BD32" s="165"/>
+      <c r="BE32" s="166"/>
+      <c r="BF32" s="145"/>
+      <c r="BG32" s="146"/>
     </row>
     <row r="33" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B33" s="104"/>
@@ -4316,12 +4316,12 @@
       <c r="AW33" s="120"/>
       <c r="AX33" s="120"/>
       <c r="AY33" s="120"/>
-      <c r="AZ33" s="148"/>
-      <c r="BA33" s="149"/>
+      <c r="AZ33" s="237"/>
+      <c r="BA33" s="238"/>
       <c r="BB33" s="120"/>
       <c r="BC33" s="121"/>
-      <c r="BD33" s="226"/>
-      <c r="BE33" s="227"/>
+      <c r="BD33" s="169"/>
+      <c r="BE33" s="170"/>
       <c r="BF33" s="122"/>
       <c r="BG33" s="123"/>
     </row>
@@ -4376,12 +4376,12 @@
       <c r="AW34" s="126"/>
       <c r="AX34" s="126"/>
       <c r="AY34" s="126"/>
-      <c r="AZ34" s="150"/>
-      <c r="BA34" s="151"/>
+      <c r="AZ34" s="167"/>
+      <c r="BA34" s="168"/>
       <c r="BB34" s="126"/>
       <c r="BC34" s="127"/>
-      <c r="BD34" s="152"/>
-      <c r="BE34" s="153"/>
+      <c r="BD34" s="226"/>
+      <c r="BE34" s="227"/>
       <c r="BF34" s="128"/>
       <c r="BG34" s="129"/>
     </row>
@@ -4436,12 +4436,12 @@
       <c r="AW35" s="126"/>
       <c r="AX35" s="126"/>
       <c r="AY35" s="126"/>
-      <c r="AZ35" s="150"/>
-      <c r="BA35" s="151"/>
+      <c r="AZ35" s="167"/>
+      <c r="BA35" s="168"/>
       <c r="BB35" s="126"/>
       <c r="BC35" s="127"/>
-      <c r="BD35" s="152"/>
-      <c r="BE35" s="153"/>
+      <c r="BD35" s="226"/>
+      <c r="BE35" s="227"/>
       <c r="BF35" s="128"/>
       <c r="BG35" s="129"/>
     </row>
@@ -4496,12 +4496,12 @@
       <c r="AW36" s="126"/>
       <c r="AX36" s="126"/>
       <c r="AY36" s="126"/>
-      <c r="AZ36" s="150"/>
-      <c r="BA36" s="151"/>
+      <c r="AZ36" s="167"/>
+      <c r="BA36" s="168"/>
       <c r="BB36" s="126"/>
       <c r="BC36" s="127"/>
-      <c r="BD36" s="152"/>
-      <c r="BE36" s="153"/>
+      <c r="BD36" s="226"/>
+      <c r="BE36" s="227"/>
       <c r="BF36" s="128"/>
       <c r="BG36" s="129"/>
     </row>
@@ -4556,12 +4556,12 @@
       <c r="AW37" s="126"/>
       <c r="AX37" s="126"/>
       <c r="AY37" s="126"/>
-      <c r="AZ37" s="150"/>
-      <c r="BA37" s="151"/>
+      <c r="AZ37" s="167"/>
+      <c r="BA37" s="168"/>
       <c r="BB37" s="126"/>
       <c r="BC37" s="127"/>
-      <c r="BD37" s="154"/>
-      <c r="BE37" s="155"/>
+      <c r="BD37" s="228"/>
+      <c r="BE37" s="229"/>
       <c r="BF37" s="130"/>
       <c r="BG37" s="131"/>
     </row>
@@ -4616,12 +4616,12 @@
       <c r="AW38" s="126"/>
       <c r="AX38" s="126"/>
       <c r="AY38" s="126"/>
-      <c r="AZ38" s="150"/>
-      <c r="BA38" s="151"/>
+      <c r="AZ38" s="167"/>
+      <c r="BA38" s="168"/>
       <c r="BB38" s="126"/>
       <c r="BC38" s="127"/>
-      <c r="BD38" s="152"/>
-      <c r="BE38" s="153"/>
+      <c r="BD38" s="226"/>
+      <c r="BE38" s="227"/>
       <c r="BF38" s="128"/>
       <c r="BG38" s="129"/>
     </row>
@@ -4676,57 +4676,57 @@
       <c r="AW39" s="139"/>
       <c r="AX39" s="139"/>
       <c r="AY39" s="139"/>
-      <c r="AZ39" s="156"/>
-      <c r="BA39" s="157"/>
+      <c r="AZ39" s="230"/>
+      <c r="BA39" s="231"/>
       <c r="BB39" s="139"/>
       <c r="BC39" s="140"/>
-      <c r="BD39" s="220"/>
-      <c r="BE39" s="221"/>
+      <c r="BD39" s="161"/>
+      <c r="BE39" s="162"/>
       <c r="BF39" s="141"/>
       <c r="BG39" s="142"/>
     </row>
     <row r="40" spans="2:59" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B40" s="145" t="s">
+      <c r="B40" s="234" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="145"/>
-      <c r="D40" s="145"/>
-      <c r="E40" s="145"/>
-      <c r="F40" s="145"/>
-      <c r="G40" s="145"/>
-      <c r="H40" s="145"/>
-      <c r="I40" s="145"/>
+      <c r="C40" s="234"/>
+      <c r="D40" s="234"/>
+      <c r="E40" s="234"/>
+      <c r="F40" s="234"/>
+      <c r="G40" s="234"/>
+      <c r="H40" s="234"/>
+      <c r="I40" s="234"/>
       <c r="AC40" s="66"/>
       <c r="AD40" s="66"/>
       <c r="AE40" s="66"/>
       <c r="AF40" s="66"/>
       <c r="AG40" s="81"/>
-      <c r="AH40" s="147" t="s">
+      <c r="AH40" s="236" t="s">
         <v>37</v>
       </c>
-      <c r="AI40" s="147"/>
-      <c r="AJ40" s="147"/>
-      <c r="AK40" s="147"/>
-      <c r="AL40" s="147"/>
+      <c r="AI40" s="236"/>
+      <c r="AJ40" s="236"/>
+      <c r="AK40" s="236"/>
+      <c r="AL40" s="236"/>
       <c r="AM40" s="103"/>
       <c r="AO40" s="87"/>
-      <c r="BD40" s="143" t="str">
+      <c r="BD40" s="232" t="str">
         <f>IF(SUM(BD33:BD39)=0,"",SUM(BD33:BD39))</f>
         <v/>
       </c>
-      <c r="BE40" s="144"/>
+      <c r="BE40" s="233"/>
     </row>
     <row r="41" spans="2:59" ht="14.25">
-      <c r="B41" s="146" t="s">
+      <c r="B41" s="235" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="146"/>
-      <c r="D41" s="146"/>
-      <c r="E41" s="146"/>
-      <c r="F41" s="146"/>
-      <c r="G41" s="146"/>
-      <c r="H41" s="146"/>
-      <c r="I41" s="146"/>
+      <c r="C41" s="235"/>
+      <c r="D41" s="235"/>
+      <c r="E41" s="235"/>
+      <c r="F41" s="235"/>
+      <c r="G41" s="235"/>
+      <c r="H41" s="235"/>
+      <c r="I41" s="235"/>
       <c r="AC41" s="66"/>
       <c r="AD41" s="66"/>
       <c r="AE41" s="66"/>
@@ -4739,16 +4739,16 @@
       </c>
     </row>
     <row r="42" spans="2:59" ht="14.25">
-      <c r="B42" s="146" t="s">
+      <c r="B42" s="235" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="146"/>
-      <c r="D42" s="146"/>
-      <c r="E42" s="146"/>
-      <c r="F42" s="146"/>
-      <c r="G42" s="146"/>
-      <c r="H42" s="146"/>
-      <c r="I42" s="146"/>
+      <c r="C42" s="235"/>
+      <c r="D42" s="235"/>
+      <c r="E42" s="235"/>
+      <c r="F42" s="235"/>
+      <c r="G42" s="235"/>
+      <c r="H42" s="235"/>
+      <c r="I42" s="235"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="54"/>
@@ -4762,15 +4762,119 @@
     <protectedRange password="EB2E" sqref="AN10:AO17 V10:W17" name="Range1"/>
   </protectedRanges>
   <mergeCells count="156">
-    <mergeCell ref="BF31:BG32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:AD32"/>
-    <mergeCell ref="AE32:AN32"/>
-    <mergeCell ref="AO32:BC32"/>
-    <mergeCell ref="AI19:AM19"/>
-    <mergeCell ref="AI24:AM24"/>
-    <mergeCell ref="AI26:AM26"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="AH40:AL40"/>
+    <mergeCell ref="AZ33:BA33"/>
+    <mergeCell ref="AZ34:BA34"/>
+    <mergeCell ref="AZ35:BA35"/>
+    <mergeCell ref="AZ36:BA36"/>
+    <mergeCell ref="AZ37:BA37"/>
+    <mergeCell ref="AN16:AP16"/>
+    <mergeCell ref="AN15:AP15"/>
+    <mergeCell ref="BD34:BE34"/>
+    <mergeCell ref="BD35:BE35"/>
+    <mergeCell ref="BD36:BE36"/>
+    <mergeCell ref="BD37:BE37"/>
+    <mergeCell ref="BD38:BE38"/>
+    <mergeCell ref="AZ39:BA39"/>
+    <mergeCell ref="BD40:BE40"/>
+    <mergeCell ref="AN14:AP14"/>
+    <mergeCell ref="Y29:AA29"/>
+    <mergeCell ref="Y15:AA15"/>
+    <mergeCell ref="AE15:AG15"/>
+    <mergeCell ref="AH15:AJ15"/>
+    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="AE11:AG11"/>
+    <mergeCell ref="AE12:AG12"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="AB15:AD15"/>
+    <mergeCell ref="AI21:AM21"/>
+    <mergeCell ref="AH16:AJ16"/>
+    <mergeCell ref="AN12:AP12"/>
+    <mergeCell ref="AK10:AM10"/>
+    <mergeCell ref="AN11:AP11"/>
+    <mergeCell ref="AH13:AJ13"/>
+    <mergeCell ref="AH14:AJ14"/>
+    <mergeCell ref="AO19:AP19"/>
+    <mergeCell ref="AN13:AP13"/>
+    <mergeCell ref="AN10:AP10"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AO21:AP21"/>
+    <mergeCell ref="AO28:AP28"/>
+    <mergeCell ref="AI28:AM28"/>
+    <mergeCell ref="G1:AJ1"/>
+    <mergeCell ref="AK11:AM11"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="AK12:AM12"/>
+    <mergeCell ref="AK13:AM13"/>
+    <mergeCell ref="AK14:AM14"/>
+    <mergeCell ref="AK15:AM15"/>
+    <mergeCell ref="AK16:AM16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AH12:AJ12"/>
+    <mergeCell ref="AB14:AD14"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="Y4:AC4"/>
+    <mergeCell ref="AK5:AP6"/>
+    <mergeCell ref="X6:AI6"/>
+    <mergeCell ref="AA7:AI7"/>
+    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="AE5:AI5"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="P6:T7"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="AB12:AD12"/>
+    <mergeCell ref="AN9:AP9"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="Y12:AA12"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE13:AG13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="AB13:AD13"/>
+    <mergeCell ref="Y14:AA14"/>
     <mergeCell ref="AB16:AD16"/>
     <mergeCell ref="Y26:AB28"/>
     <mergeCell ref="BD39:BE39"/>
@@ -4795,129 +4899,25 @@
     <mergeCell ref="P12:R12"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="AK9:AM9"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="AB10:AD10"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="AK5:AP6"/>
-    <mergeCell ref="X6:AI6"/>
-    <mergeCell ref="AA7:AI7"/>
-    <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="AE5:AI5"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="P6:T7"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AE13:AG13"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G1:AJ1"/>
-    <mergeCell ref="AK11:AM11"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="AK12:AM12"/>
-    <mergeCell ref="AK13:AM13"/>
-    <mergeCell ref="AK14:AM14"/>
-    <mergeCell ref="AK15:AM15"/>
-    <mergeCell ref="AK16:AM16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="BF31:BG32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:AD32"/>
+    <mergeCell ref="AE32:AN32"/>
+    <mergeCell ref="AO32:BC32"/>
+    <mergeCell ref="AI19:AM19"/>
+    <mergeCell ref="AI24:AM24"/>
+    <mergeCell ref="AI26:AM26"/>
     <mergeCell ref="G26:Q28"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="M16:O16"/>
     <mergeCell ref="G23:X25"/>
     <mergeCell ref="S26:W28"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="Y16:AA16"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="S15:U15"/>
     <mergeCell ref="S19:W20"/>
     <mergeCell ref="G19:Q20"/>
     <mergeCell ref="Y19:AB20"/>
-    <mergeCell ref="AH9:AJ9"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AH12:AJ12"/>
-    <mergeCell ref="AB14:AD14"/>
-    <mergeCell ref="AB13:AD13"/>
     <mergeCell ref="S21:W21"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="AB12:AD12"/>
-    <mergeCell ref="AN14:AP14"/>
-    <mergeCell ref="Y29:AA29"/>
-    <mergeCell ref="Y15:AA15"/>
-    <mergeCell ref="AE15:AG15"/>
-    <mergeCell ref="AH15:AJ15"/>
-    <mergeCell ref="AH10:AJ10"/>
-    <mergeCell ref="AE11:AG11"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB15:AD15"/>
-    <mergeCell ref="AI21:AM21"/>
-    <mergeCell ref="AH16:AJ16"/>
-    <mergeCell ref="AN9:AP9"/>
-    <mergeCell ref="AN12:AP12"/>
-    <mergeCell ref="AK10:AM10"/>
-    <mergeCell ref="AN11:AP11"/>
-    <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="AH14:AJ14"/>
-    <mergeCell ref="AO19:AP19"/>
-    <mergeCell ref="AN13:AP13"/>
     <mergeCell ref="S29:W29"/>
-    <mergeCell ref="AN10:AP10"/>
-    <mergeCell ref="AO26:AP26"/>
-    <mergeCell ref="AO21:AP21"/>
-    <mergeCell ref="AO28:AP28"/>
-    <mergeCell ref="AI28:AM28"/>
     <mergeCell ref="AD19:AH29"/>
     <mergeCell ref="AO24:AP24"/>
-    <mergeCell ref="AN16:AP16"/>
-    <mergeCell ref="AN15:AP15"/>
-    <mergeCell ref="BD34:BE34"/>
-    <mergeCell ref="BD35:BE35"/>
-    <mergeCell ref="BD36:BE36"/>
-    <mergeCell ref="BD37:BE37"/>
-    <mergeCell ref="BD38:BE38"/>
-    <mergeCell ref="AZ39:BA39"/>
-    <mergeCell ref="BD40:BE40"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="AH40:AL40"/>
-    <mergeCell ref="AZ33:BA33"/>
-    <mergeCell ref="AZ34:BA34"/>
-    <mergeCell ref="AZ35:BA35"/>
-    <mergeCell ref="AZ36:BA36"/>
-    <mergeCell ref="AZ37:BA37"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations xWindow="252" yWindow="215" count="4">

</xml_diff>

<commit_message>
Normalization 3 is working as expected
add some exported tables.
</commit_message>
<xml_diff>
--- a/2012 CALTRANS TIMESHEET 0727-0809.xlsx
+++ b/2012 CALTRANS TIMESHEET 0727-0809.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shq153\Desktop\Caltrans\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView showSheetTabs="0" xWindow="360" yWindow="15" windowWidth="9720" windowHeight="6540"/>
   </bookViews>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Caltrans Student Timesheet'!$A$1:$BH$43</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -215,14 +220,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="[h]:mm"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -988,7 +993,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="238">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1423,6 +1428,235 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1435,15 +1669,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1462,162 +1687,6 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0" hidden="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -1648,36 +1717,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1704,47 +1746,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1753,6 +1754,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2254,7 +2263,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -2296,7 +2305,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -2315,14 +2324,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BG51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4:AC4"/>
+      <selection activeCell="BE21" sqref="BE21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="0.85546875" style="27" customWidth="1"/>
     <col min="2" max="6" width="4" style="27"/>
@@ -2352,39 +2361,39 @@
     <col min="55" max="16384" width="4" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" ht="24.75" customHeight="1">
-      <c r="G1" s="200" t="s">
+    <row r="1" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="G1" s="173" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="200"/>
-      <c r="I1" s="200"/>
-      <c r="J1" s="200"/>
-      <c r="K1" s="200"/>
-      <c r="L1" s="200"/>
-      <c r="M1" s="200"/>
-      <c r="N1" s="200"/>
-      <c r="O1" s="200"/>
-      <c r="P1" s="200"/>
-      <c r="Q1" s="200"/>
-      <c r="R1" s="200"/>
-      <c r="S1" s="200"/>
-      <c r="T1" s="200"/>
-      <c r="U1" s="200"/>
-      <c r="V1" s="200"/>
-      <c r="W1" s="200"/>
-      <c r="X1" s="200"/>
-      <c r="Y1" s="200"/>
-      <c r="Z1" s="200"/>
-      <c r="AA1" s="200"/>
-      <c r="AB1" s="200"/>
-      <c r="AC1" s="200"/>
-      <c r="AD1" s="200"/>
-      <c r="AE1" s="200"/>
-      <c r="AF1" s="200"/>
-      <c r="AG1" s="200"/>
-      <c r="AH1" s="200"/>
-      <c r="AI1" s="200"/>
-      <c r="AJ1" s="200"/>
+      <c r="H1" s="173"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="173"/>
+      <c r="K1" s="173"/>
+      <c r="L1" s="173"/>
+      <c r="M1" s="173"/>
+      <c r="N1" s="173"/>
+      <c r="O1" s="173"/>
+      <c r="P1" s="173"/>
+      <c r="Q1" s="173"/>
+      <c r="R1" s="173"/>
+      <c r="S1" s="173"/>
+      <c r="T1" s="173"/>
+      <c r="U1" s="173"/>
+      <c r="V1" s="173"/>
+      <c r="W1" s="173"/>
+      <c r="X1" s="173"/>
+      <c r="Y1" s="173"/>
+      <c r="Z1" s="173"/>
+      <c r="AA1" s="173"/>
+      <c r="AB1" s="173"/>
+      <c r="AC1" s="173"/>
+      <c r="AD1" s="173"/>
+      <c r="AE1" s="173"/>
+      <c r="AF1" s="173"/>
+      <c r="AG1" s="173"/>
+      <c r="AH1" s="173"/>
+      <c r="AI1" s="173"/>
+      <c r="AJ1" s="173"/>
       <c r="AK1" s="71" t="s">
         <v>15</v>
       </c>
@@ -2392,7 +2401,7 @@
       <c r="AP1" s="27"/>
       <c r="AQ1" s="3"/>
     </row>
-    <row r="2" spans="1:53" ht="14.25">
+    <row r="2" spans="1:53" ht="14.25" x14ac:dyDescent="0.2">
       <c r="K2" s="29"/>
       <c r="L2" s="29"/>
       <c r="M2" s="29"/>
@@ -2412,7 +2421,7 @@
       <c r="AP2" s="30"/>
       <c r="AQ2" s="3"/>
     </row>
-    <row r="3" spans="1:53" ht="14.25" customHeight="1">
+    <row r="3" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G3" s="84"/>
       <c r="H3" s="85"/>
       <c r="I3" s="85"/>
@@ -2434,7 +2443,7 @@
       <c r="AP3" s="30"/>
       <c r="AQ3" s="3"/>
     </row>
-    <row r="4" spans="1:53" ht="15.75">
+    <row r="4" spans="1:53" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G4" s="86" t="s">
         <v>58</v>
       </c>
@@ -2456,28 +2465,28 @@
       <c r="V4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="178">
-        <v>41847</v>
-      </c>
-      <c r="Z4" s="178"/>
-      <c r="AA4" s="178"/>
-      <c r="AB4" s="178"/>
-      <c r="AC4" s="178"/>
+      <c r="Y4" s="175">
+        <v>41875</v>
+      </c>
+      <c r="Z4" s="175"/>
+      <c r="AA4" s="175"/>
+      <c r="AB4" s="175"/>
+      <c r="AC4" s="175"/>
       <c r="AD4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="AE4" s="177">
-        <v>41860</v>
-      </c>
-      <c r="AF4" s="177"/>
-      <c r="AG4" s="177"/>
-      <c r="AH4" s="177"/>
-      <c r="AI4" s="177"/>
+      <c r="AE4" s="175">
+        <v>41888</v>
+      </c>
+      <c r="AF4" s="175"/>
+      <c r="AG4" s="175"/>
+      <c r="AH4" s="175"/>
+      <c r="AI4" s="175"/>
       <c r="AO4" s="27"/>
       <c r="AP4" s="27"/>
       <c r="AQ4" s="3"/>
     </row>
-    <row r="5" spans="1:53" ht="14.25" customHeight="1">
+    <row r="5" spans="1:53" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G5" s="27" t="s">
         <v>1</v>
       </c>
@@ -2488,80 +2497,80 @@
       <c r="R5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="Y5" s="176" t="s">
+      <c r="Y5" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="176"/>
-      <c r="AA5" s="176"/>
-      <c r="AB5" s="176"/>
-      <c r="AC5" s="176"/>
+      <c r="Z5" s="174"/>
+      <c r="AA5" s="174"/>
+      <c r="AB5" s="174"/>
+      <c r="AC5" s="174"/>
       <c r="AD5" s="33"/>
-      <c r="AE5" s="176" t="s">
+      <c r="AE5" s="174" t="s">
         <v>25</v>
       </c>
-      <c r="AF5" s="176"/>
-      <c r="AG5" s="176"/>
-      <c r="AH5" s="176"/>
-      <c r="AI5" s="176"/>
+      <c r="AF5" s="174"/>
+      <c r="AG5" s="174"/>
+      <c r="AH5" s="174"/>
+      <c r="AI5" s="174"/>
       <c r="AJ5" s="34"/>
-      <c r="AK5" s="179" t="s">
+      <c r="AK5" s="176" t="s">
         <v>61</v>
       </c>
-      <c r="AL5" s="180"/>
-      <c r="AM5" s="180"/>
-      <c r="AN5" s="180"/>
-      <c r="AO5" s="180"/>
-      <c r="AP5" s="181"/>
+      <c r="AL5" s="177"/>
+      <c r="AM5" s="177"/>
+      <c r="AN5" s="177"/>
+      <c r="AO5" s="177"/>
+      <c r="AP5" s="178"/>
       <c r="AQ5" s="3"/>
     </row>
-    <row r="6" spans="1:53" ht="21.75" customHeight="1">
+    <row r="6" spans="1:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
       <c r="O6" s="69"/>
-      <c r="P6" s="187" t="s">
+      <c r="P6" s="184" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="187"/>
-      <c r="R6" s="187"/>
-      <c r="S6" s="187"/>
-      <c r="T6" s="188"/>
+      <c r="Q6" s="184"/>
+      <c r="R6" s="184"/>
+      <c r="S6" s="184"/>
+      <c r="T6" s="185"/>
       <c r="V6" s="68" t="s">
         <v>12</v>
       </c>
       <c r="W6" s="35"/>
-      <c r="X6" s="185"/>
-      <c r="Y6" s="185"/>
-      <c r="Z6" s="185"/>
-      <c r="AA6" s="185"/>
-      <c r="AB6" s="185"/>
-      <c r="AC6" s="185"/>
-      <c r="AD6" s="185"/>
-      <c r="AE6" s="185"/>
-      <c r="AF6" s="185"/>
-      <c r="AG6" s="185"/>
-      <c r="AH6" s="185"/>
-      <c r="AI6" s="185"/>
+      <c r="X6" s="182"/>
+      <c r="Y6" s="182"/>
+      <c r="Z6" s="182"/>
+      <c r="AA6" s="182"/>
+      <c r="AB6" s="182"/>
+      <c r="AC6" s="182"/>
+      <c r="AD6" s="182"/>
+      <c r="AE6" s="182"/>
+      <c r="AF6" s="182"/>
+      <c r="AG6" s="182"/>
+      <c r="AH6" s="182"/>
+      <c r="AI6" s="182"/>
       <c r="AJ6" s="34"/>
-      <c r="AK6" s="182"/>
-      <c r="AL6" s="183"/>
-      <c r="AM6" s="183"/>
-      <c r="AN6" s="183"/>
-      <c r="AO6" s="183"/>
-      <c r="AP6" s="184"/>
+      <c r="AK6" s="179"/>
+      <c r="AL6" s="180"/>
+      <c r="AM6" s="180"/>
+      <c r="AN6" s="180"/>
+      <c r="AO6" s="180"/>
+      <c r="AP6" s="181"/>
       <c r="AQ6" s="3"/>
     </row>
-    <row r="7" spans="1:53" ht="24" customHeight="1">
+    <row r="7" spans="1:53" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" s="66" t="s">
         <v>0</v>
       </c>
       <c r="M7" s="57"/>
       <c r="N7" s="57"/>
       <c r="O7" s="69"/>
-      <c r="P7" s="189"/>
-      <c r="Q7" s="189"/>
-      <c r="R7" s="189"/>
-      <c r="S7" s="189"/>
-      <c r="T7" s="190"/>
+      <c r="P7" s="186"/>
+      <c r="Q7" s="186"/>
+      <c r="R7" s="186"/>
+      <c r="S7" s="186"/>
+      <c r="T7" s="187"/>
       <c r="V7" s="66" t="s">
         <v>13</v>
       </c>
@@ -2569,26 +2578,26 @@
       <c r="X7" s="77"/>
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
-      <c r="AA7" s="186"/>
-      <c r="AB7" s="186"/>
-      <c r="AC7" s="186"/>
-      <c r="AD7" s="186"/>
-      <c r="AE7" s="186"/>
-      <c r="AF7" s="186"/>
-      <c r="AG7" s="186"/>
-      <c r="AH7" s="186"/>
-      <c r="AI7" s="186"/>
-      <c r="AK7" s="176" t="s">
+      <c r="AA7" s="183"/>
+      <c r="AB7" s="183"/>
+      <c r="AC7" s="183"/>
+      <c r="AD7" s="183"/>
+      <c r="AE7" s="183"/>
+      <c r="AF7" s="183"/>
+      <c r="AG7" s="183"/>
+      <c r="AH7" s="183"/>
+      <c r="AI7" s="183"/>
+      <c r="AK7" s="174" t="s">
         <v>14</v>
       </c>
-      <c r="AL7" s="176"/>
-      <c r="AM7" s="176"/>
-      <c r="AN7" s="176"/>
-      <c r="AO7" s="176"/>
-      <c r="AP7" s="176"/>
+      <c r="AL7" s="174"/>
+      <c r="AM7" s="174"/>
+      <c r="AN7" s="174"/>
+      <c r="AO7" s="174"/>
+      <c r="AP7" s="174"/>
       <c r="AQ7" s="3"/>
     </row>
-    <row r="8" spans="1:53" ht="10.5" customHeight="1" thickBot="1">
+    <row r="8" spans="1:53" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AG8" s="36"/>
       <c r="AO8" s="27"/>
       <c r="AP8" s="27"/>
@@ -2608,69 +2617,69 @@
       <c r="AZ8" s="6"/>
       <c r="BA8" s="6"/>
     </row>
-    <row r="9" spans="1:53" s="2" customFormat="1" ht="24.75" customHeight="1" thickBot="1">
+    <row r="9" spans="1:53" s="2" customFormat="1" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
-      <c r="G9" s="197"/>
-      <c r="H9" s="198"/>
-      <c r="I9" s="199"/>
-      <c r="J9" s="173" t="s">
+      <c r="G9" s="191"/>
+      <c r="H9" s="192"/>
+      <c r="I9" s="193"/>
+      <c r="J9" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="173"/>
-      <c r="L9" s="173"/>
-      <c r="M9" s="173" t="s">
+      <c r="K9" s="160"/>
+      <c r="L9" s="160"/>
+      <c r="M9" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="173"/>
-      <c r="O9" s="173"/>
-      <c r="P9" s="173" t="s">
+      <c r="N9" s="160"/>
+      <c r="O9" s="160"/>
+      <c r="P9" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="173"/>
-      <c r="R9" s="173"/>
-      <c r="S9" s="191" t="s">
+      <c r="Q9" s="160"/>
+      <c r="R9" s="160"/>
+      <c r="S9" s="188" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="192"/>
-      <c r="U9" s="193"/>
-      <c r="V9" s="173" t="s">
+      <c r="T9" s="189"/>
+      <c r="U9" s="190"/>
+      <c r="V9" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="W9" s="173"/>
-      <c r="X9" s="173"/>
-      <c r="Y9" s="175"/>
-      <c r="Z9" s="175"/>
-      <c r="AA9" s="175"/>
-      <c r="AB9" s="173" t="s">
+      <c r="W9" s="160"/>
+      <c r="X9" s="160"/>
+      <c r="Y9" s="195"/>
+      <c r="Z9" s="195"/>
+      <c r="AA9" s="195"/>
+      <c r="AB9" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="AC9" s="173"/>
-      <c r="AD9" s="173"/>
-      <c r="AE9" s="174" t="s">
+      <c r="AC9" s="160"/>
+      <c r="AD9" s="160"/>
+      <c r="AE9" s="194" t="s">
         <v>19</v>
       </c>
-      <c r="AF9" s="174"/>
-      <c r="AG9" s="174"/>
-      <c r="AH9" s="173" t="s">
+      <c r="AF9" s="194"/>
+      <c r="AG9" s="194"/>
+      <c r="AH9" s="160" t="s">
         <v>18</v>
       </c>
-      <c r="AI9" s="173"/>
-      <c r="AJ9" s="173"/>
-      <c r="AK9" s="173" t="s">
+      <c r="AI9" s="160"/>
+      <c r="AJ9" s="160"/>
+      <c r="AK9" s="160" t="s">
         <v>19</v>
       </c>
-      <c r="AL9" s="173"/>
-      <c r="AM9" s="173"/>
-      <c r="AN9" s="173" t="s">
+      <c r="AL9" s="160"/>
+      <c r="AM9" s="160"/>
+      <c r="AN9" s="160" t="s">
         <v>20</v>
       </c>
-      <c r="AO9" s="173"/>
-      <c r="AP9" s="173"/>
+      <c r="AO9" s="160"/>
+      <c r="AP9" s="160"/>
       <c r="AQ9" s="21" t="s">
         <v>40</v>
       </c>
@@ -2703,59 +2712,59 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="10" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82"/>
       <c r="B10" s="82"/>
       <c r="C10" s="82"/>
       <c r="D10" s="82"/>
       <c r="E10" s="82"/>
       <c r="F10" s="83"/>
-      <c r="G10" s="173" t="s">
+      <c r="G10" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="173"/>
-      <c r="I10" s="173"/>
-      <c r="J10" s="158"/>
-      <c r="K10" s="158"/>
-      <c r="L10" s="158"/>
-      <c r="M10" s="158"/>
-      <c r="N10" s="158"/>
-      <c r="O10" s="158"/>
-      <c r="P10" s="158"/>
-      <c r="Q10" s="158"/>
-      <c r="R10" s="158"/>
-      <c r="S10" s="158"/>
-      <c r="T10" s="158"/>
-      <c r="U10" s="158"/>
-      <c r="V10" s="172">
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="164"/>
+      <c r="K10" s="164"/>
+      <c r="L10" s="164"/>
+      <c r="M10" s="164"/>
+      <c r="N10" s="164"/>
+      <c r="O10" s="164"/>
+      <c r="P10" s="164"/>
+      <c r="Q10" s="164"/>
+      <c r="R10" s="164"/>
+      <c r="S10" s="164"/>
+      <c r="T10" s="164"/>
+      <c r="U10" s="164"/>
+      <c r="V10" s="150">
         <f>((M10-J10)+(S10-P10))</f>
         <v>0</v>
       </c>
-      <c r="W10" s="172"/>
-      <c r="X10" s="172"/>
-      <c r="Y10" s="173" t="s">
+      <c r="W10" s="150"/>
+      <c r="X10" s="150"/>
+      <c r="Y10" s="160" t="s">
         <v>4</v>
       </c>
-      <c r="Z10" s="173"/>
-      <c r="AA10" s="173"/>
-      <c r="AB10" s="158"/>
-      <c r="AC10" s="158"/>
-      <c r="AD10" s="158"/>
-      <c r="AE10" s="158"/>
-      <c r="AF10" s="158"/>
-      <c r="AG10" s="158"/>
-      <c r="AH10" s="158"/>
-      <c r="AI10" s="158"/>
-      <c r="AJ10" s="158"/>
-      <c r="AK10" s="158"/>
-      <c r="AL10" s="158"/>
-      <c r="AM10" s="158"/>
-      <c r="AN10" s="172">
+      <c r="Z10" s="160"/>
+      <c r="AA10" s="160"/>
+      <c r="AB10" s="164"/>
+      <c r="AC10" s="164"/>
+      <c r="AD10" s="164"/>
+      <c r="AE10" s="164"/>
+      <c r="AF10" s="164"/>
+      <c r="AG10" s="164"/>
+      <c r="AH10" s="164"/>
+      <c r="AI10" s="164"/>
+      <c r="AJ10" s="164"/>
+      <c r="AK10" s="164"/>
+      <c r="AL10" s="164"/>
+      <c r="AM10" s="164"/>
+      <c r="AN10" s="150">
         <f t="shared" ref="AN10:AN16" si="0">((AE10-AB10)+(AK10-AH10))</f>
         <v>0</v>
       </c>
-      <c r="AO10" s="172"/>
-      <c r="AP10" s="172"/>
+      <c r="AO10" s="150"/>
+      <c r="AP10" s="150"/>
       <c r="AQ10" s="22">
         <f>MIN(8/24,V10)</f>
         <v>0</v>
@@ -2798,70 +2807,78 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="11" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="82"/>
       <c r="B11" s="82"/>
       <c r="C11" s="82"/>
       <c r="D11" s="82"/>
       <c r="E11" s="82"/>
       <c r="F11" s="83"/>
-      <c r="G11" s="173" t="s">
+      <c r="G11" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="173"/>
-      <c r="I11" s="173"/>
-      <c r="J11" s="158"/>
-      <c r="K11" s="195"/>
-      <c r="L11" s="196"/>
-      <c r="M11" s="194"/>
-      <c r="N11" s="195"/>
-      <c r="O11" s="196"/>
-      <c r="P11" s="194"/>
-      <c r="Q11" s="195"/>
-      <c r="R11" s="196"/>
-      <c r="S11" s="194"/>
-      <c r="T11" s="195"/>
-      <c r="U11" s="196"/>
-      <c r="V11" s="172">
+      <c r="H11" s="160"/>
+      <c r="I11" s="160"/>
+      <c r="J11" s="164">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K11" s="164"/>
+      <c r="L11" s="164"/>
+      <c r="M11" s="164">
+        <v>0.5</v>
+      </c>
+      <c r="N11" s="164"/>
+      <c r="O11" s="164"/>
+      <c r="P11" s="164">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="Q11" s="164"/>
+      <c r="R11" s="164"/>
+      <c r="S11" s="164">
+        <v>0.6875</v>
+      </c>
+      <c r="T11" s="164"/>
+      <c r="U11" s="164"/>
+      <c r="V11" s="150">
         <f t="shared" ref="V11:V16" si="7">((M11-J11)+(S11-P11))</f>
-        <v>0</v>
-      </c>
-      <c r="W11" s="172"/>
-      <c r="X11" s="172"/>
-      <c r="Y11" s="173" t="s">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="W11" s="150"/>
+      <c r="X11" s="150"/>
+      <c r="Y11" s="160" t="s">
         <v>5</v>
       </c>
-      <c r="Z11" s="173"/>
-      <c r="AA11" s="173"/>
-      <c r="AB11" s="158">
+      <c r="Z11" s="160"/>
+      <c r="AA11" s="160"/>
+      <c r="AB11" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC11" s="158"/>
-      <c r="AD11" s="158"/>
-      <c r="AE11" s="194">
+      <c r="AC11" s="164"/>
+      <c r="AD11" s="164"/>
+      <c r="AE11" s="161">
         <v>0.5</v>
       </c>
-      <c r="AF11" s="195"/>
-      <c r="AG11" s="196"/>
-      <c r="AH11" s="158">
+      <c r="AF11" s="162"/>
+      <c r="AG11" s="163"/>
+      <c r="AH11" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI11" s="158"/>
-      <c r="AJ11" s="158"/>
-      <c r="AK11" s="158">
+      <c r="AI11" s="164"/>
+      <c r="AJ11" s="164"/>
+      <c r="AK11" s="164">
         <v>0.6875</v>
       </c>
-      <c r="AL11" s="158"/>
-      <c r="AM11" s="158"/>
-      <c r="AN11" s="172">
+      <c r="AL11" s="164"/>
+      <c r="AM11" s="164"/>
+      <c r="AN11" s="150">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO11" s="172"/>
-      <c r="AP11" s="172"/>
+      <c r="AO11" s="150"/>
+      <c r="AP11" s="150"/>
       <c r="AQ11" s="22">
         <f t="shared" ref="AQ11:AQ16" si="8">MIN(8/24,V11)</f>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AR11" s="10">
         <f t="shared" ref="AR11:AR18" si="9">MIN(MAX(V11-8/24,0),4/24)</f>
@@ -2873,11 +2890,11 @@
       </c>
       <c r="AT11" s="10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AU11" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV11" s="12"/>
       <c r="AW11" s="10">
@@ -2901,78 +2918,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="12" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="82"/>
       <c r="B12" s="82"/>
       <c r="C12" s="82"/>
       <c r="D12" s="82"/>
       <c r="E12" s="82"/>
       <c r="F12" s="83"/>
-      <c r="G12" s="173" t="s">
+      <c r="G12" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="173"/>
-      <c r="I12" s="173"/>
-      <c r="J12" s="158">
-        <v>0.375</v>
-      </c>
-      <c r="K12" s="158"/>
-      <c r="L12" s="158"/>
-      <c r="M12" s="158">
+      <c r="H12" s="160"/>
+      <c r="I12" s="160"/>
+      <c r="J12" s="164">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K12" s="164"/>
+      <c r="L12" s="164"/>
+      <c r="M12" s="164">
         <v>0.5</v>
       </c>
-      <c r="N12" s="158"/>
-      <c r="O12" s="158"/>
-      <c r="P12" s="158">
+      <c r="N12" s="164"/>
+      <c r="O12" s="164"/>
+      <c r="P12" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q12" s="158"/>
-      <c r="R12" s="158"/>
-      <c r="S12" s="158">
-        <v>0.72916666666666663</v>
-      </c>
-      <c r="T12" s="158"/>
-      <c r="U12" s="158"/>
-      <c r="V12" s="172">
+      <c r="Q12" s="164"/>
+      <c r="R12" s="164"/>
+      <c r="S12" s="164">
+        <v>0.6875</v>
+      </c>
+      <c r="T12" s="164"/>
+      <c r="U12" s="164"/>
+      <c r="V12" s="150">
         <f t="shared" si="7"/>
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="W12" s="172"/>
-      <c r="X12" s="172"/>
-      <c r="Y12" s="173" t="s">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="W12" s="150"/>
+      <c r="X12" s="150"/>
+      <c r="Y12" s="160" t="s">
         <v>6</v>
       </c>
-      <c r="Z12" s="173"/>
-      <c r="AA12" s="173"/>
-      <c r="AB12" s="158">
+      <c r="Z12" s="160"/>
+      <c r="AA12" s="160"/>
+      <c r="AB12" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC12" s="158"/>
-      <c r="AD12" s="158"/>
-      <c r="AE12" s="194">
+      <c r="AC12" s="164"/>
+      <c r="AD12" s="164"/>
+      <c r="AE12" s="161">
         <v>0.5</v>
       </c>
-      <c r="AF12" s="195"/>
-      <c r="AG12" s="196"/>
-      <c r="AH12" s="158">
+      <c r="AF12" s="162"/>
+      <c r="AG12" s="163"/>
+      <c r="AH12" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI12" s="158"/>
-      <c r="AJ12" s="158"/>
-      <c r="AK12" s="158">
+      <c r="AI12" s="164"/>
+      <c r="AJ12" s="164"/>
+      <c r="AK12" s="164">
         <v>0.6875</v>
       </c>
-      <c r="AL12" s="158"/>
-      <c r="AM12" s="158"/>
-      <c r="AN12" s="172">
+      <c r="AL12" s="164"/>
+      <c r="AM12" s="164"/>
+      <c r="AN12" s="150">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO12" s="172"/>
-      <c r="AP12" s="172"/>
+      <c r="AO12" s="150"/>
+      <c r="AP12" s="150"/>
       <c r="AQ12" s="22">
         <f t="shared" si="8"/>
-        <v>0.33333333333333326</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AR12" s="10">
         <f t="shared" si="9"/>
@@ -2984,7 +3001,7 @@
       </c>
       <c r="AT12" s="10">
         <f t="shared" si="1"/>
-        <v>0.33333333333333326</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AU12" s="11">
         <f t="shared" si="2"/>
@@ -3012,75 +3029,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="13" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="82"/>
       <c r="B13" s="82"/>
       <c r="C13" s="82"/>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
       <c r="F13" s="83"/>
-      <c r="G13" s="173" t="s">
+      <c r="G13" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="173"/>
-      <c r="I13" s="173"/>
-      <c r="J13" s="158">
+      <c r="H13" s="160"/>
+      <c r="I13" s="160"/>
+      <c r="J13" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K13" s="158"/>
-      <c r="L13" s="158"/>
-      <c r="M13" s="158">
+      <c r="K13" s="164"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="164">
         <v>0.5</v>
       </c>
-      <c r="N13" s="158"/>
-      <c r="O13" s="158"/>
-      <c r="P13" s="158">
+      <c r="N13" s="164"/>
+      <c r="O13" s="164"/>
+      <c r="P13" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q13" s="158"/>
-      <c r="R13" s="158"/>
-      <c r="S13" s="158">
+      <c r="Q13" s="164"/>
+      <c r="R13" s="164"/>
+      <c r="S13" s="164">
         <v>0.6875</v>
       </c>
-      <c r="T13" s="158"/>
-      <c r="U13" s="158"/>
-      <c r="V13" s="172">
+      <c r="T13" s="164"/>
+      <c r="U13" s="164"/>
+      <c r="V13" s="150">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W13" s="172"/>
-      <c r="X13" s="172"/>
-      <c r="Y13" s="173" t="s">
+      <c r="W13" s="150"/>
+      <c r="X13" s="150"/>
+      <c r="Y13" s="160" t="s">
         <v>7</v>
       </c>
-      <c r="Z13" s="173"/>
-      <c r="AA13" s="173"/>
-      <c r="AB13" s="158">
+      <c r="Z13" s="160"/>
+      <c r="AA13" s="160"/>
+      <c r="AB13" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC13" s="158"/>
-      <c r="AD13" s="158"/>
-      <c r="AE13" s="194">
+      <c r="AC13" s="164"/>
+      <c r="AD13" s="164"/>
+      <c r="AE13" s="161">
         <v>0.5</v>
       </c>
-      <c r="AF13" s="195"/>
-      <c r="AG13" s="196"/>
-      <c r="AH13" s="158">
+      <c r="AF13" s="162"/>
+      <c r="AG13" s="163"/>
+      <c r="AH13" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI13" s="158"/>
-      <c r="AJ13" s="158"/>
-      <c r="AK13" s="158">
+      <c r="AI13" s="164"/>
+      <c r="AJ13" s="164"/>
+      <c r="AK13" s="164">
         <v>0.6875</v>
       </c>
-      <c r="AL13" s="158"/>
-      <c r="AM13" s="158"/>
-      <c r="AN13" s="172">
+      <c r="AL13" s="164"/>
+      <c r="AM13" s="164"/>
+      <c r="AN13" s="150">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO13" s="172"/>
-      <c r="AP13" s="172"/>
+      <c r="AO13" s="150"/>
+      <c r="AP13" s="150"/>
       <c r="AQ13" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3123,78 +3140,78 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="14" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="56"/>
-      <c r="G14" s="173" t="s">
+      <c r="G14" s="160" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="173"/>
-      <c r="I14" s="173"/>
-      <c r="J14" s="158">
-        <v>0.34375</v>
-      </c>
-      <c r="K14" s="158"/>
-      <c r="L14" s="158"/>
-      <c r="M14" s="158">
+      <c r="H14" s="160"/>
+      <c r="I14" s="160"/>
+      <c r="J14" s="164">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="K14" s="164"/>
+      <c r="L14" s="164"/>
+      <c r="M14" s="164">
         <v>0.5</v>
       </c>
-      <c r="N14" s="158"/>
-      <c r="O14" s="158"/>
-      <c r="P14" s="158">
+      <c r="N14" s="164"/>
+      <c r="O14" s="164"/>
+      <c r="P14" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q14" s="158"/>
-      <c r="R14" s="158"/>
-      <c r="S14" s="158">
-        <v>0.69791666666666663</v>
-      </c>
-      <c r="T14" s="158"/>
-      <c r="U14" s="158"/>
-      <c r="V14" s="172">
+      <c r="Q14" s="164"/>
+      <c r="R14" s="164"/>
+      <c r="S14" s="164">
+        <v>0.6875</v>
+      </c>
+      <c r="T14" s="164"/>
+      <c r="U14" s="164"/>
+      <c r="V14" s="150">
         <f t="shared" si="7"/>
-        <v>0.33333333333333326</v>
-      </c>
-      <c r="W14" s="172"/>
-      <c r="X14" s="172"/>
-      <c r="Y14" s="173" t="s">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="W14" s="150"/>
+      <c r="X14" s="150"/>
+      <c r="Y14" s="160" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="173"/>
-      <c r="AA14" s="173"/>
-      <c r="AB14" s="158">
+      <c r="Z14" s="160"/>
+      <c r="AA14" s="160"/>
+      <c r="AB14" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC14" s="158"/>
-      <c r="AD14" s="158"/>
-      <c r="AE14" s="194">
+      <c r="AC14" s="164"/>
+      <c r="AD14" s="164"/>
+      <c r="AE14" s="161">
         <v>0.5</v>
       </c>
-      <c r="AF14" s="195"/>
-      <c r="AG14" s="196"/>
-      <c r="AH14" s="158">
+      <c r="AF14" s="162"/>
+      <c r="AG14" s="163"/>
+      <c r="AH14" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI14" s="158"/>
-      <c r="AJ14" s="158"/>
-      <c r="AK14" s="158">
+      <c r="AI14" s="164"/>
+      <c r="AJ14" s="164"/>
+      <c r="AK14" s="164">
         <v>0.6875</v>
       </c>
-      <c r="AL14" s="158"/>
-      <c r="AM14" s="158"/>
-      <c r="AN14" s="172">
+      <c r="AL14" s="164"/>
+      <c r="AM14" s="164"/>
+      <c r="AN14" s="150">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO14" s="172"/>
-      <c r="AP14" s="172"/>
+      <c r="AO14" s="150"/>
+      <c r="AP14" s="150"/>
       <c r="AQ14" s="22">
         <f t="shared" si="8"/>
-        <v>0.33333333333333326</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AR14" s="10">
         <f t="shared" si="9"/>
@@ -3206,7 +3223,7 @@
       </c>
       <c r="AT14" s="10">
         <f t="shared" si="1"/>
-        <v>0.33333333333333326</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="AU14" s="11">
         <f t="shared" si="2"/>
@@ -3234,75 +3251,75 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="15" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="56"/>
-      <c r="G15" s="173" t="s">
+      <c r="G15" s="160" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="173"/>
-      <c r="I15" s="173"/>
-      <c r="J15" s="158">
+      <c r="H15" s="160"/>
+      <c r="I15" s="160"/>
+      <c r="J15" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
-      <c r="M15" s="158">
+      <c r="K15" s="164"/>
+      <c r="L15" s="164"/>
+      <c r="M15" s="164">
         <v>0.5</v>
       </c>
-      <c r="N15" s="158"/>
-      <c r="O15" s="158"/>
-      <c r="P15" s="158">
+      <c r="N15" s="164"/>
+      <c r="O15" s="164"/>
+      <c r="P15" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q15" s="158"/>
-      <c r="R15" s="158"/>
-      <c r="S15" s="158">
+      <c r="Q15" s="164"/>
+      <c r="R15" s="164"/>
+      <c r="S15" s="164">
         <v>0.6875</v>
       </c>
-      <c r="T15" s="158"/>
-      <c r="U15" s="158"/>
-      <c r="V15" s="172">
+      <c r="T15" s="164"/>
+      <c r="U15" s="164"/>
+      <c r="V15" s="150">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W15" s="172"/>
-      <c r="X15" s="172"/>
-      <c r="Y15" s="173" t="s">
+      <c r="W15" s="150"/>
+      <c r="X15" s="150"/>
+      <c r="Y15" s="160" t="s">
         <v>9</v>
       </c>
-      <c r="Z15" s="173"/>
-      <c r="AA15" s="173"/>
-      <c r="AB15" s="158">
+      <c r="Z15" s="160"/>
+      <c r="AA15" s="160"/>
+      <c r="AB15" s="164">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC15" s="158"/>
-      <c r="AD15" s="158"/>
-      <c r="AE15" s="194">
+      <c r="AC15" s="164"/>
+      <c r="AD15" s="164"/>
+      <c r="AE15" s="161">
         <v>0.5</v>
       </c>
-      <c r="AF15" s="195"/>
-      <c r="AG15" s="196"/>
-      <c r="AH15" s="158">
+      <c r="AF15" s="162"/>
+      <c r="AG15" s="163"/>
+      <c r="AH15" s="164">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI15" s="158"/>
-      <c r="AJ15" s="158"/>
-      <c r="AK15" s="158">
+      <c r="AI15" s="164"/>
+      <c r="AJ15" s="164"/>
+      <c r="AK15" s="164">
         <v>0.6875</v>
       </c>
-      <c r="AL15" s="158"/>
-      <c r="AM15" s="158"/>
-      <c r="AN15" s="172">
+      <c r="AL15" s="164"/>
+      <c r="AM15" s="164"/>
+      <c r="AN15" s="150">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO15" s="172"/>
-      <c r="AP15" s="172"/>
+      <c r="AO15" s="150"/>
+      <c r="AP15" s="150"/>
       <c r="AQ15" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3345,59 +3362,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1">
+    <row r="16" spans="1:53" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="55"/>
-      <c r="G16" s="173" t="s">
+      <c r="G16" s="160" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="173"/>
-      <c r="I16" s="173"/>
-      <c r="J16" s="158"/>
-      <c r="K16" s="158"/>
-      <c r="L16" s="158"/>
-      <c r="M16" s="158"/>
-      <c r="N16" s="158"/>
-      <c r="O16" s="158"/>
-      <c r="P16" s="158"/>
-      <c r="Q16" s="158"/>
-      <c r="R16" s="158"/>
-      <c r="S16" s="158"/>
-      <c r="T16" s="158"/>
-      <c r="U16" s="158"/>
-      <c r="V16" s="172">
+      <c r="H16" s="160"/>
+      <c r="I16" s="160"/>
+      <c r="J16" s="164"/>
+      <c r="K16" s="164"/>
+      <c r="L16" s="164"/>
+      <c r="M16" s="164"/>
+      <c r="N16" s="164"/>
+      <c r="O16" s="164"/>
+      <c r="P16" s="164"/>
+      <c r="Q16" s="164"/>
+      <c r="R16" s="164"/>
+      <c r="S16" s="164"/>
+      <c r="T16" s="164"/>
+      <c r="U16" s="164"/>
+      <c r="V16" s="150">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W16" s="172"/>
-      <c r="X16" s="172"/>
-      <c r="Y16" s="173" t="s">
+      <c r="W16" s="150"/>
+      <c r="X16" s="150"/>
+      <c r="Y16" s="160" t="s">
         <v>10</v>
       </c>
-      <c r="Z16" s="173"/>
-      <c r="AA16" s="173"/>
-      <c r="AB16" s="158"/>
-      <c r="AC16" s="158"/>
-      <c r="AD16" s="158"/>
-      <c r="AE16" s="158"/>
-      <c r="AF16" s="158"/>
-      <c r="AG16" s="158"/>
-      <c r="AH16" s="158"/>
-      <c r="AI16" s="158"/>
-      <c r="AJ16" s="158"/>
-      <c r="AK16" s="158"/>
-      <c r="AL16" s="158"/>
-      <c r="AM16" s="158"/>
-      <c r="AN16" s="172">
+      <c r="Z16" s="160"/>
+      <c r="AA16" s="160"/>
+      <c r="AB16" s="164"/>
+      <c r="AC16" s="164"/>
+      <c r="AD16" s="164"/>
+      <c r="AE16" s="164"/>
+      <c r="AF16" s="164"/>
+      <c r="AG16" s="164"/>
+      <c r="AH16" s="164"/>
+      <c r="AI16" s="164"/>
+      <c r="AJ16" s="164"/>
+      <c r="AK16" s="164"/>
+      <c r="AL16" s="164"/>
+      <c r="AM16" s="164"/>
+      <c r="AN16" s="150">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="172"/>
-      <c r="AP16" s="172"/>
+      <c r="AO16" s="150"/>
+      <c r="AP16" s="150"/>
       <c r="AQ16" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3440,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:59" s="2" customFormat="1" ht="17.45" customHeight="1" thickBot="1">
+    <row r="17" spans="1:59" s="2" customFormat="1" ht="17.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -3495,7 +3512,7 @@
       <c r="AZ17" s="13"/>
       <c r="BA17" s="11"/>
     </row>
-    <row r="18" spans="1:59" ht="13.5" thickBot="1">
+    <row r="18" spans="1:59" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="AD18" s="44"/>
       <c r="AE18" s="44"/>
       <c r="AF18" s="31"/>
@@ -3504,7 +3521,7 @@
       <c r="AP18" s="27"/>
       <c r="AQ18" s="15">
         <f>SUM(AQ10:AQ16)</f>
-        <v>1.333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="AR18" s="10">
         <f t="shared" si="9"/>
@@ -3516,11 +3533,11 @@
       </c>
       <c r="AT18" s="15">
         <f>SUM(AT10:AT16)</f>
-        <v>1.333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="AU18" s="16">
         <f>SUM(AU10:AU16)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AV18" s="6"/>
       <c r="AW18" s="15">
@@ -3544,60 +3561,60 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
+    <row r="19" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="46"/>
       <c r="B19" s="46"/>
       <c r="C19" s="46"/>
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
-      <c r="G19" s="201"/>
-      <c r="H19" s="201"/>
-      <c r="I19" s="201"/>
-      <c r="J19" s="201"/>
-      <c r="K19" s="201"/>
-      <c r="L19" s="201"/>
-      <c r="M19" s="201"/>
-      <c r="N19" s="201"/>
-      <c r="O19" s="201"/>
-      <c r="P19" s="201"/>
-      <c r="Q19" s="201"/>
+      <c r="G19" s="220"/>
+      <c r="H19" s="220"/>
+      <c r="I19" s="220"/>
+      <c r="J19" s="220"/>
+      <c r="K19" s="220"/>
+      <c r="L19" s="220"/>
+      <c r="M19" s="220"/>
+      <c r="N19" s="220"/>
+      <c r="O19" s="220"/>
+      <c r="P19" s="220"/>
+      <c r="Q19" s="220"/>
       <c r="R19" s="62"/>
-      <c r="S19" s="206" t="s">
+      <c r="S19" s="225" t="s">
         <v>62</v>
       </c>
-      <c r="T19" s="206"/>
-      <c r="U19" s="206"/>
-      <c r="V19" s="206"/>
-      <c r="W19" s="206"/>
-      <c r="Y19" s="206">
-        <v>41862</v>
-      </c>
-      <c r="Z19" s="207"/>
-      <c r="AA19" s="207"/>
-      <c r="AB19" s="207"/>
-      <c r="AD19" s="217" t="s">
+      <c r="T19" s="225"/>
+      <c r="U19" s="225"/>
+      <c r="V19" s="225"/>
+      <c r="W19" s="225"/>
+      <c r="Y19" s="225">
+        <v>41887</v>
+      </c>
+      <c r="Z19" s="226"/>
+      <c r="AA19" s="226"/>
+      <c r="AB19" s="226"/>
+      <c r="AD19" s="229" t="s">
         <v>33</v>
       </c>
-      <c r="AE19" s="218"/>
-      <c r="AF19" s="218"/>
-      <c r="AG19" s="218"/>
-      <c r="AH19" s="219"/>
-      <c r="AI19" s="156" t="s">
+      <c r="AE19" s="230"/>
+      <c r="AF19" s="230"/>
+      <c r="AG19" s="230"/>
+      <c r="AH19" s="231"/>
+      <c r="AI19" s="165" t="s">
         <v>21</v>
       </c>
-      <c r="AJ19" s="157"/>
-      <c r="AK19" s="157"/>
-      <c r="AL19" s="157"/>
-      <c r="AM19" s="157"/>
-      <c r="AO19" s="210">
+      <c r="AJ19" s="166"/>
+      <c r="AK19" s="166"/>
+      <c r="AL19" s="166"/>
+      <c r="AM19" s="166"/>
+      <c r="AO19" s="167">
         <f>+AQ19+AW19</f>
-        <v>2.9999999999999996</v>
-      </c>
-      <c r="AP19" s="211"/>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="AP19" s="168"/>
       <c r="AQ19" s="26">
         <f>MIN(SUM(AQ10:AQ16),40/24)</f>
-        <v>1.333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="AR19" s="19"/>
       <c r="AS19" s="19"/>
@@ -3613,40 +3630,40 @@
       <c r="AZ19" s="19"/>
       <c r="BA19" s="6"/>
     </row>
-    <row r="20" spans="1:59" ht="6" customHeight="1" thickBot="1">
+    <row r="20" spans="1:59" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="47"/>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
-      <c r="G20" s="202"/>
-      <c r="H20" s="202"/>
-      <c r="I20" s="202"/>
-      <c r="J20" s="202"/>
-      <c r="K20" s="202"/>
-      <c r="L20" s="202"/>
-      <c r="M20" s="202"/>
-      <c r="N20" s="202"/>
-      <c r="O20" s="202"/>
-      <c r="P20" s="202"/>
-      <c r="Q20" s="202"/>
+      <c r="G20" s="221"/>
+      <c r="H20" s="221"/>
+      <c r="I20" s="221"/>
+      <c r="J20" s="221"/>
+      <c r="K20" s="221"/>
+      <c r="L20" s="221"/>
+      <c r="M20" s="221"/>
+      <c r="N20" s="221"/>
+      <c r="O20" s="221"/>
+      <c r="P20" s="221"/>
+      <c r="Q20" s="221"/>
       <c r="R20" s="63"/>
-      <c r="S20" s="205"/>
-      <c r="T20" s="205"/>
-      <c r="U20" s="205"/>
-      <c r="V20" s="205"/>
-      <c r="W20" s="205"/>
-      <c r="Y20" s="160"/>
-      <c r="Z20" s="160"/>
-      <c r="AA20" s="160"/>
-      <c r="AB20" s="160"/>
+      <c r="S20" s="224"/>
+      <c r="T20" s="224"/>
+      <c r="U20" s="224"/>
+      <c r="V20" s="224"/>
+      <c r="W20" s="224"/>
+      <c r="Y20" s="197"/>
+      <c r="Z20" s="197"/>
+      <c r="AA20" s="197"/>
+      <c r="AB20" s="197"/>
       <c r="AC20" s="48"/>
-      <c r="AD20" s="220"/>
-      <c r="AE20" s="221"/>
-      <c r="AF20" s="221"/>
-      <c r="AG20" s="221"/>
-      <c r="AH20" s="222"/>
+      <c r="AD20" s="232"/>
+      <c r="AE20" s="233"/>
+      <c r="AF20" s="233"/>
+      <c r="AG20" s="233"/>
+      <c r="AH20" s="234"/>
       <c r="AM20" s="66"/>
       <c r="AO20" s="65"/>
       <c r="AP20" s="65"/>
@@ -3662,7 +3679,7 @@
       <c r="AZ20" s="19"/>
       <c r="BA20" s="6"/>
     </row>
-    <row r="21" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
+    <row r="21" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -3683,35 +3700,35 @@
       <c r="P21" s="35"/>
       <c r="Q21" s="50"/>
       <c r="R21" s="35"/>
-      <c r="S21" s="208" t="s">
+      <c r="S21" s="227" t="s">
         <v>28</v>
       </c>
-      <c r="T21" s="208"/>
-      <c r="U21" s="208"/>
-      <c r="V21" s="208"/>
-      <c r="W21" s="208"/>
-      <c r="Y21" s="171" t="s">
+      <c r="T21" s="227"/>
+      <c r="U21" s="227"/>
+      <c r="V21" s="227"/>
+      <c r="W21" s="227"/>
+      <c r="Y21" s="206" t="s">
         <v>26</v>
       </c>
-      <c r="Z21" s="171"/>
-      <c r="AA21" s="171"/>
-      <c r="AD21" s="220"/>
-      <c r="AE21" s="221"/>
-      <c r="AF21" s="221"/>
-      <c r="AG21" s="221"/>
-      <c r="AH21" s="222"/>
-      <c r="AI21" s="156" t="s">
+      <c r="Z21" s="206"/>
+      <c r="AA21" s="206"/>
+      <c r="AD21" s="232"/>
+      <c r="AE21" s="233"/>
+      <c r="AF21" s="233"/>
+      <c r="AG21" s="233"/>
+      <c r="AH21" s="234"/>
+      <c r="AI21" s="165" t="s">
         <v>24</v>
       </c>
-      <c r="AJ21" s="157"/>
-      <c r="AK21" s="157"/>
-      <c r="AL21" s="157"/>
-      <c r="AM21" s="157"/>
-      <c r="AO21" s="210">
+      <c r="AJ21" s="166"/>
+      <c r="AK21" s="166"/>
+      <c r="AL21" s="166"/>
+      <c r="AM21" s="166"/>
+      <c r="AO21" s="167">
         <f>+AR21+AX21</f>
         <v>0</v>
       </c>
-      <c r="AP21" s="211"/>
+      <c r="AP21" s="168"/>
       <c r="AQ21" s="19"/>
       <c r="AR21" s="20">
         <f>SUM(AR10:AR16)+MAX(0,SUM(AQ10:AQ16)-40/24)</f>
@@ -3730,7 +3747,7 @@
       <c r="AZ21" s="19"/>
       <c r="BA21" s="6"/>
     </row>
-    <row r="22" spans="1:59" ht="6" customHeight="1">
+    <row r="22" spans="1:59" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="35"/>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
@@ -3757,11 +3774,11 @@
       <c r="Y22" s="51"/>
       <c r="Z22" s="51"/>
       <c r="AA22" s="51"/>
-      <c r="AD22" s="220"/>
-      <c r="AE22" s="221"/>
-      <c r="AF22" s="221"/>
-      <c r="AG22" s="221"/>
-      <c r="AH22" s="222"/>
+      <c r="AD22" s="232"/>
+      <c r="AE22" s="233"/>
+      <c r="AF22" s="233"/>
+      <c r="AG22" s="233"/>
+      <c r="AH22" s="234"/>
       <c r="AL22" s="28"/>
       <c r="AM22" s="66"/>
       <c r="AN22" s="23"/>
@@ -3779,33 +3796,33 @@
       <c r="AZ22" s="19"/>
       <c r="BA22" s="6"/>
     </row>
-    <row r="23" spans="1:59" ht="3.75" customHeight="1" thickBot="1">
-      <c r="G23" s="203" t="s">
+    <row r="23" spans="1:59" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="222" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="203"/>
-      <c r="I23" s="203"/>
-      <c r="J23" s="203"/>
-      <c r="K23" s="203"/>
-      <c r="L23" s="203"/>
-      <c r="M23" s="203"/>
-      <c r="N23" s="203"/>
-      <c r="O23" s="203"/>
-      <c r="P23" s="203"/>
-      <c r="Q23" s="203"/>
-      <c r="R23" s="203"/>
-      <c r="S23" s="203"/>
-      <c r="T23" s="203"/>
-      <c r="U23" s="203"/>
-      <c r="V23" s="203"/>
-      <c r="W23" s="203"/>
-      <c r="X23" s="203"/>
+      <c r="H23" s="222"/>
+      <c r="I23" s="222"/>
+      <c r="J23" s="222"/>
+      <c r="K23" s="222"/>
+      <c r="L23" s="222"/>
+      <c r="M23" s="222"/>
+      <c r="N23" s="222"/>
+      <c r="O23" s="222"/>
+      <c r="P23" s="222"/>
+      <c r="Q23" s="222"/>
+      <c r="R23" s="222"/>
+      <c r="S23" s="222"/>
+      <c r="T23" s="222"/>
+      <c r="U23" s="222"/>
+      <c r="V23" s="222"/>
+      <c r="W23" s="222"/>
+      <c r="X23" s="222"/>
       <c r="AC23" s="48"/>
-      <c r="AD23" s="220"/>
-      <c r="AE23" s="221"/>
-      <c r="AF23" s="221"/>
-      <c r="AG23" s="221"/>
-      <c r="AH23" s="222"/>
+      <c r="AD23" s="232"/>
+      <c r="AE23" s="233"/>
+      <c r="AF23" s="233"/>
+      <c r="AG23" s="233"/>
+      <c r="AH23" s="234"/>
       <c r="AM23" s="66"/>
       <c r="AO23" s="65"/>
       <c r="AP23" s="65"/>
@@ -3821,42 +3838,42 @@
       <c r="AZ23" s="19"/>
       <c r="BA23" s="6"/>
     </row>
-    <row r="24" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
-      <c r="G24" s="203"/>
-      <c r="H24" s="203"/>
-      <c r="I24" s="203"/>
-      <c r="J24" s="203"/>
-      <c r="K24" s="203"/>
-      <c r="L24" s="203"/>
-      <c r="M24" s="203"/>
-      <c r="N24" s="203"/>
-      <c r="O24" s="203"/>
-      <c r="P24" s="203"/>
-      <c r="Q24" s="203"/>
-      <c r="R24" s="203"/>
-      <c r="S24" s="203"/>
-      <c r="T24" s="203"/>
-      <c r="U24" s="203"/>
-      <c r="V24" s="203"/>
-      <c r="W24" s="203"/>
-      <c r="X24" s="203"/>
-      <c r="AD24" s="220"/>
-      <c r="AE24" s="221"/>
-      <c r="AF24" s="221"/>
-      <c r="AG24" s="221"/>
-      <c r="AH24" s="222"/>
-      <c r="AI24" s="156" t="s">
+    <row r="24" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="222"/>
+      <c r="H24" s="222"/>
+      <c r="I24" s="222"/>
+      <c r="J24" s="222"/>
+      <c r="K24" s="222"/>
+      <c r="L24" s="222"/>
+      <c r="M24" s="222"/>
+      <c r="N24" s="222"/>
+      <c r="O24" s="222"/>
+      <c r="P24" s="222"/>
+      <c r="Q24" s="222"/>
+      <c r="R24" s="222"/>
+      <c r="S24" s="222"/>
+      <c r="T24" s="222"/>
+      <c r="U24" s="222"/>
+      <c r="V24" s="222"/>
+      <c r="W24" s="222"/>
+      <c r="X24" s="222"/>
+      <c r="AD24" s="232"/>
+      <c r="AE24" s="233"/>
+      <c r="AF24" s="233"/>
+      <c r="AG24" s="233"/>
+      <c r="AH24" s="234"/>
+      <c r="AI24" s="165" t="s">
         <v>23</v>
       </c>
-      <c r="AJ24" s="157"/>
-      <c r="AK24" s="157"/>
-      <c r="AL24" s="157"/>
-      <c r="AM24" s="157"/>
-      <c r="AO24" s="210">
+      <c r="AJ24" s="166"/>
+      <c r="AK24" s="166"/>
+      <c r="AL24" s="166"/>
+      <c r="AM24" s="166"/>
+      <c r="AO24" s="167">
         <f>+AS24+AY24</f>
         <v>0</v>
       </c>
-      <c r="AP24" s="211"/>
+      <c r="AP24" s="168"/>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="19"/>
       <c r="AS24" s="20">
@@ -3875,31 +3892,31 @@
       <c r="AZ24" s="19"/>
       <c r="BA24" s="6"/>
     </row>
-    <row r="25" spans="1:59" ht="6.75" customHeight="1" thickBot="1">
-      <c r="G25" s="203"/>
-      <c r="H25" s="203"/>
-      <c r="I25" s="203"/>
-      <c r="J25" s="203"/>
-      <c r="K25" s="203"/>
-      <c r="L25" s="203"/>
-      <c r="M25" s="203"/>
-      <c r="N25" s="203"/>
-      <c r="O25" s="203"/>
-      <c r="P25" s="203"/>
-      <c r="Q25" s="203"/>
-      <c r="R25" s="203"/>
-      <c r="S25" s="203"/>
-      <c r="T25" s="203"/>
-      <c r="U25" s="203"/>
-      <c r="V25" s="203"/>
-      <c r="W25" s="203"/>
-      <c r="X25" s="203"/>
+    <row r="25" spans="1:59" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="222"/>
+      <c r="H25" s="222"/>
+      <c r="I25" s="222"/>
+      <c r="J25" s="222"/>
+      <c r="K25" s="222"/>
+      <c r="L25" s="222"/>
+      <c r="M25" s="222"/>
+      <c r="N25" s="222"/>
+      <c r="O25" s="222"/>
+      <c r="P25" s="222"/>
+      <c r="Q25" s="222"/>
+      <c r="R25" s="222"/>
+      <c r="S25" s="222"/>
+      <c r="T25" s="222"/>
+      <c r="U25" s="222"/>
+      <c r="V25" s="222"/>
+      <c r="W25" s="222"/>
+      <c r="X25" s="222"/>
       <c r="AC25" s="48"/>
-      <c r="AD25" s="220"/>
-      <c r="AE25" s="221"/>
-      <c r="AF25" s="221"/>
-      <c r="AG25" s="221"/>
-      <c r="AH25" s="222"/>
+      <c r="AD25" s="232"/>
+      <c r="AE25" s="233"/>
+      <c r="AF25" s="233"/>
+      <c r="AG25" s="233"/>
+      <c r="AH25" s="234"/>
       <c r="AM25" s="66"/>
       <c r="AO25" s="65"/>
       <c r="AP25" s="65"/>
@@ -3915,58 +3932,58 @@
       <c r="AZ25" s="19"/>
       <c r="BA25" s="6"/>
     </row>
-    <row r="26" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
+    <row r="26" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
       <c r="B26" s="47"/>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
-      <c r="G26" s="201"/>
-      <c r="H26" s="201"/>
-      <c r="I26" s="201"/>
-      <c r="J26" s="201"/>
-      <c r="K26" s="201"/>
-      <c r="L26" s="201"/>
-      <c r="M26" s="201"/>
-      <c r="N26" s="201"/>
-      <c r="O26" s="201"/>
-      <c r="P26" s="201"/>
-      <c r="Q26" s="201"/>
+      <c r="G26" s="220"/>
+      <c r="H26" s="220"/>
+      <c r="I26" s="220"/>
+      <c r="J26" s="220"/>
+      <c r="K26" s="220"/>
+      <c r="L26" s="220"/>
+      <c r="M26" s="220"/>
+      <c r="N26" s="220"/>
+      <c r="O26" s="220"/>
+      <c r="P26" s="220"/>
+      <c r="Q26" s="220"/>
       <c r="R26" s="64"/>
-      <c r="S26" s="204"/>
-      <c r="T26" s="204"/>
-      <c r="U26" s="204"/>
-      <c r="V26" s="204"/>
-      <c r="W26" s="204"/>
+      <c r="S26" s="223"/>
+      <c r="T26" s="223"/>
+      <c r="U26" s="223"/>
+      <c r="V26" s="223"/>
+      <c r="W26" s="223"/>
       <c r="X26" s="35"/>
-      <c r="Y26" s="159"/>
-      <c r="Z26" s="159"/>
-      <c r="AA26" s="159"/>
-      <c r="AB26" s="159"/>
-      <c r="AD26" s="220"/>
-      <c r="AE26" s="221"/>
-      <c r="AF26" s="221"/>
-      <c r="AG26" s="221"/>
-      <c r="AH26" s="222"/>
-      <c r="AI26" s="156" t="s">
+      <c r="Y26" s="196"/>
+      <c r="Z26" s="196"/>
+      <c r="AA26" s="196"/>
+      <c r="AB26" s="196"/>
+      <c r="AD26" s="232"/>
+      <c r="AE26" s="233"/>
+      <c r="AF26" s="233"/>
+      <c r="AG26" s="233"/>
+      <c r="AH26" s="234"/>
+      <c r="AI26" s="165" t="s">
         <v>22</v>
       </c>
-      <c r="AJ26" s="157"/>
-      <c r="AK26" s="157"/>
-      <c r="AL26" s="157"/>
-      <c r="AM26" s="157"/>
-      <c r="AO26" s="213">
+      <c r="AJ26" s="166"/>
+      <c r="AK26" s="166"/>
+      <c r="AL26" s="166"/>
+      <c r="AM26" s="166"/>
+      <c r="AO26" s="169">
         <f>AT26+AZ26</f>
-        <v>2.9999999999999996</v>
-      </c>
-      <c r="AP26" s="214"/>
+        <v>3.333333333333333</v>
+      </c>
+      <c r="AP26" s="170"/>
       <c r="AQ26" s="19"/>
       <c r="AR26" s="19"/>
       <c r="AS26" s="19"/>
       <c r="AT26" s="20">
         <f>SUM(AT10:AT16)</f>
-        <v>1.333333333333333</v>
+        <v>1.6666666666666665</v>
       </c>
       <c r="AU26" s="6"/>
       <c r="AV26" s="6"/>
@@ -3979,40 +3996,40 @@
       </c>
       <c r="BA26" s="6"/>
     </row>
-    <row r="27" spans="1:59" ht="16.5" customHeight="1" thickBot="1">
+    <row r="27" spans="1:59" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="47"/>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
-      <c r="G27" s="201"/>
-      <c r="H27" s="201"/>
-      <c r="I27" s="201"/>
-      <c r="J27" s="201"/>
-      <c r="K27" s="201"/>
-      <c r="L27" s="201"/>
-      <c r="M27" s="201"/>
-      <c r="N27" s="201"/>
-      <c r="O27" s="201"/>
-      <c r="P27" s="201"/>
-      <c r="Q27" s="201"/>
+      <c r="G27" s="220"/>
+      <c r="H27" s="220"/>
+      <c r="I27" s="220"/>
+      <c r="J27" s="220"/>
+      <c r="K27" s="220"/>
+      <c r="L27" s="220"/>
+      <c r="M27" s="220"/>
+      <c r="N27" s="220"/>
+      <c r="O27" s="220"/>
+      <c r="P27" s="220"/>
+      <c r="Q27" s="220"/>
       <c r="R27" s="64"/>
-      <c r="S27" s="204"/>
-      <c r="T27" s="204"/>
-      <c r="U27" s="204"/>
-      <c r="V27" s="204"/>
-      <c r="W27" s="204"/>
+      <c r="S27" s="223"/>
+      <c r="T27" s="223"/>
+      <c r="U27" s="223"/>
+      <c r="V27" s="223"/>
+      <c r="W27" s="223"/>
       <c r="X27" s="35"/>
-      <c r="Y27" s="159"/>
-      <c r="Z27" s="159"/>
-      <c r="AA27" s="159"/>
-      <c r="AB27" s="159"/>
-      <c r="AD27" s="220"/>
-      <c r="AE27" s="221"/>
-      <c r="AF27" s="221"/>
-      <c r="AG27" s="221"/>
-      <c r="AH27" s="222"/>
+      <c r="Y27" s="196"/>
+      <c r="Z27" s="196"/>
+      <c r="AA27" s="196"/>
+      <c r="AB27" s="196"/>
+      <c r="AD27" s="232"/>
+      <c r="AE27" s="233"/>
+      <c r="AF27" s="233"/>
+      <c r="AG27" s="233"/>
+      <c r="AH27" s="234"/>
       <c r="AM27" s="74"/>
       <c r="AO27" s="76"/>
       <c r="AP27" s="76"/>
@@ -4028,50 +4045,50 @@
       <c r="AZ27" s="20"/>
       <c r="BA27" s="6"/>
     </row>
-    <row r="28" spans="1:59" ht="18.95" customHeight="1" thickBot="1">
-      <c r="G28" s="202"/>
-      <c r="H28" s="202"/>
-      <c r="I28" s="202"/>
-      <c r="J28" s="202"/>
-      <c r="K28" s="202"/>
-      <c r="L28" s="202"/>
-      <c r="M28" s="202"/>
-      <c r="N28" s="202"/>
-      <c r="O28" s="202"/>
-      <c r="P28" s="202"/>
-      <c r="Q28" s="202"/>
+    <row r="28" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="G28" s="221"/>
+      <c r="H28" s="221"/>
+      <c r="I28" s="221"/>
+      <c r="J28" s="221"/>
+      <c r="K28" s="221"/>
+      <c r="L28" s="221"/>
+      <c r="M28" s="221"/>
+      <c r="N28" s="221"/>
+      <c r="O28" s="221"/>
+      <c r="P28" s="221"/>
+      <c r="Q28" s="221"/>
       <c r="R28" s="35"/>
-      <c r="S28" s="205"/>
-      <c r="T28" s="205"/>
-      <c r="U28" s="205"/>
-      <c r="V28" s="205"/>
-      <c r="W28" s="205"/>
+      <c r="S28" s="224"/>
+      <c r="T28" s="224"/>
+      <c r="U28" s="224"/>
+      <c r="V28" s="224"/>
+      <c r="W28" s="224"/>
       <c r="X28" s="35"/>
-      <c r="Y28" s="160"/>
-      <c r="Z28" s="160"/>
-      <c r="AA28" s="160"/>
-      <c r="AB28" s="160"/>
+      <c r="Y28" s="197"/>
+      <c r="Z28" s="197"/>
+      <c r="AA28" s="197"/>
+      <c r="AB28" s="197"/>
       <c r="AC28" s="52"/>
-      <c r="AD28" s="220"/>
-      <c r="AE28" s="221"/>
-      <c r="AF28" s="221"/>
-      <c r="AG28" s="221"/>
-      <c r="AH28" s="222"/>
-      <c r="AI28" s="156" t="s">
+      <c r="AD28" s="232"/>
+      <c r="AE28" s="233"/>
+      <c r="AF28" s="233"/>
+      <c r="AG28" s="233"/>
+      <c r="AH28" s="234"/>
+      <c r="AI28" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="AJ28" s="157"/>
-      <c r="AK28" s="157"/>
-      <c r="AL28" s="157"/>
-      <c r="AM28" s="157"/>
-      <c r="AO28" s="215"/>
-      <c r="AP28" s="216"/>
+      <c r="AJ28" s="166"/>
+      <c r="AK28" s="166"/>
+      <c r="AL28" s="166"/>
+      <c r="AM28" s="166"/>
+      <c r="AO28" s="171"/>
+      <c r="AP28" s="172"/>
       <c r="AQ28" s="19"/>
       <c r="AR28" s="19"/>
       <c r="AS28" s="19"/>
       <c r="AT28" s="20">
         <f>SUM(AT11:AT18)</f>
-        <v>2.6666666666666661</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="AU28" s="6"/>
       <c r="AV28" s="6"/>
@@ -4084,7 +4101,7 @@
       </c>
       <c r="BA28" s="6"/>
     </row>
-    <row r="29" spans="1:59" ht="14.25" customHeight="1">
+    <row r="29" spans="1:59" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H29" s="66" t="s">
         <v>39</v>
       </c>
@@ -4093,25 +4110,25 @@
       <c r="O29" s="35"/>
       <c r="P29" s="35"/>
       <c r="R29" s="35"/>
-      <c r="S29" s="212" t="s">
+      <c r="S29" s="228" t="s">
         <v>29</v>
       </c>
-      <c r="T29" s="212"/>
-      <c r="U29" s="212"/>
-      <c r="V29" s="212"/>
-      <c r="W29" s="212"/>
+      <c r="T29" s="228"/>
+      <c r="U29" s="228"/>
+      <c r="V29" s="228"/>
+      <c r="W29" s="228"/>
       <c r="X29" s="35"/>
-      <c r="Y29" s="209" t="s">
+      <c r="Y29" s="159" t="s">
         <v>26</v>
       </c>
-      <c r="Z29" s="209"/>
-      <c r="AA29" s="209"/>
+      <c r="Z29" s="159"/>
+      <c r="AA29" s="159"/>
       <c r="AC29" s="52"/>
-      <c r="AD29" s="223"/>
-      <c r="AE29" s="224"/>
-      <c r="AF29" s="224"/>
-      <c r="AG29" s="224"/>
-      <c r="AH29" s="225"/>
+      <c r="AD29" s="235"/>
+      <c r="AE29" s="236"/>
+      <c r="AF29" s="236"/>
+      <c r="AG29" s="236"/>
+      <c r="AH29" s="237"/>
       <c r="AO29" s="27"/>
       <c r="AP29" s="27"/>
       <c r="AQ29" s="19"/>
@@ -4126,8 +4143,8 @@
       <c r="AZ29" s="24"/>
       <c r="BA29" s="6"/>
     </row>
-    <row r="30" spans="1:59" ht="12.75" customHeight="1" thickBot="1"/>
-    <row r="31" spans="1:59" s="2" customFormat="1" ht="14.25" customHeight="1" thickBot="1">
+    <row r="30" spans="1:59" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:59" s="2" customFormat="1" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B31" s="58"/>
       <c r="C31" s="59"/>
       <c r="D31" s="60"/>
@@ -4182,90 +4199,90 @@
       <c r="BA31" s="102"/>
       <c r="BB31" s="102"/>
       <c r="BC31" s="92"/>
-      <c r="BD31" s="163" t="s">
+      <c r="BD31" s="200" t="s">
         <v>45</v>
       </c>
-      <c r="BE31" s="164"/>
-      <c r="BF31" s="143" t="s">
+      <c r="BE31" s="201"/>
+      <c r="BF31" s="210" t="s">
         <v>46</v>
       </c>
-      <c r="BG31" s="144"/>
+      <c r="BG31" s="211"/>
     </row>
-    <row r="32" spans="1:59" s="2" customFormat="1" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B32" s="147" t="s">
+    <row r="32" spans="1:59" s="2" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="207" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="149"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="149"/>
-      <c r="F32" s="149"/>
-      <c r="G32" s="149"/>
-      <c r="H32" s="149"/>
-      <c r="I32" s="149"/>
-      <c r="J32" s="149"/>
-      <c r="K32" s="149"/>
-      <c r="L32" s="149"/>
-      <c r="M32" s="149"/>
-      <c r="N32" s="148"/>
-      <c r="O32" s="147" t="s">
+      <c r="C32" s="208"/>
+      <c r="D32" s="208"/>
+      <c r="E32" s="208"/>
+      <c r="F32" s="208"/>
+      <c r="G32" s="208"/>
+      <c r="H32" s="208"/>
+      <c r="I32" s="208"/>
+      <c r="J32" s="208"/>
+      <c r="K32" s="208"/>
+      <c r="L32" s="208"/>
+      <c r="M32" s="208"/>
+      <c r="N32" s="209"/>
+      <c r="O32" s="207" t="s">
         <v>49</v>
       </c>
-      <c r="P32" s="148"/>
-      <c r="Q32" s="147" t="s">
+      <c r="P32" s="209"/>
+      <c r="Q32" s="207" t="s">
         <v>50</v>
       </c>
-      <c r="R32" s="148"/>
-      <c r="S32" s="147" t="s">
+      <c r="R32" s="209"/>
+      <c r="S32" s="207" t="s">
         <v>51</v>
       </c>
-      <c r="T32" s="149"/>
-      <c r="U32" s="149"/>
-      <c r="V32" s="148"/>
-      <c r="W32" s="147" t="s">
+      <c r="T32" s="208"/>
+      <c r="U32" s="208"/>
+      <c r="V32" s="209"/>
+      <c r="W32" s="207" t="s">
         <v>53</v>
       </c>
-      <c r="X32" s="149"/>
-      <c r="Y32" s="149"/>
-      <c r="Z32" s="149"/>
-      <c r="AA32" s="149"/>
-      <c r="AB32" s="149"/>
-      <c r="AC32" s="149"/>
-      <c r="AD32" s="148"/>
-      <c r="AE32" s="150" t="s">
+      <c r="X32" s="208"/>
+      <c r="Y32" s="208"/>
+      <c r="Z32" s="208"/>
+      <c r="AA32" s="208"/>
+      <c r="AB32" s="208"/>
+      <c r="AC32" s="208"/>
+      <c r="AD32" s="209"/>
+      <c r="AE32" s="214" t="s">
         <v>52</v>
       </c>
-      <c r="AF32" s="151"/>
-      <c r="AG32" s="151"/>
-      <c r="AH32" s="151"/>
-      <c r="AI32" s="151"/>
-      <c r="AJ32" s="151"/>
-      <c r="AK32" s="151"/>
-      <c r="AL32" s="151"/>
-      <c r="AM32" s="151"/>
-      <c r="AN32" s="152"/>
-      <c r="AO32" s="153" t="s">
+      <c r="AF32" s="215"/>
+      <c r="AG32" s="215"/>
+      <c r="AH32" s="215"/>
+      <c r="AI32" s="215"/>
+      <c r="AJ32" s="215"/>
+      <c r="AK32" s="215"/>
+      <c r="AL32" s="215"/>
+      <c r="AM32" s="215"/>
+      <c r="AN32" s="216"/>
+      <c r="AO32" s="217" t="s">
         <v>54</v>
       </c>
-      <c r="AP32" s="154"/>
-      <c r="AQ32" s="154"/>
-      <c r="AR32" s="154"/>
-      <c r="AS32" s="154"/>
-      <c r="AT32" s="154"/>
-      <c r="AU32" s="154"/>
-      <c r="AV32" s="154"/>
-      <c r="AW32" s="154"/>
-      <c r="AX32" s="154"/>
-      <c r="AY32" s="154"/>
-      <c r="AZ32" s="154"/>
-      <c r="BA32" s="154"/>
-      <c r="BB32" s="154"/>
-      <c r="BC32" s="155"/>
-      <c r="BD32" s="165"/>
-      <c r="BE32" s="166"/>
-      <c r="BF32" s="145"/>
-      <c r="BG32" s="146"/>
+      <c r="AP32" s="218"/>
+      <c r="AQ32" s="218"/>
+      <c r="AR32" s="218"/>
+      <c r="AS32" s="218"/>
+      <c r="AT32" s="218"/>
+      <c r="AU32" s="218"/>
+      <c r="AV32" s="218"/>
+      <c r="AW32" s="218"/>
+      <c r="AX32" s="218"/>
+      <c r="AY32" s="218"/>
+      <c r="AZ32" s="218"/>
+      <c r="BA32" s="218"/>
+      <c r="BB32" s="218"/>
+      <c r="BC32" s="219"/>
+      <c r="BD32" s="202"/>
+      <c r="BE32" s="203"/>
+      <c r="BF32" s="212"/>
+      <c r="BG32" s="213"/>
     </row>
-    <row r="33" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="33" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="104"/>
       <c r="C33" s="105"/>
       <c r="D33" s="106"/>
@@ -4316,16 +4333,16 @@
       <c r="AW33" s="120"/>
       <c r="AX33" s="120"/>
       <c r="AY33" s="120"/>
-      <c r="AZ33" s="237"/>
-      <c r="BA33" s="238"/>
+      <c r="AZ33" s="146"/>
+      <c r="BA33" s="147"/>
       <c r="BB33" s="120"/>
       <c r="BC33" s="121"/>
-      <c r="BD33" s="169"/>
-      <c r="BE33" s="170"/>
+      <c r="BD33" s="204"/>
+      <c r="BE33" s="205"/>
       <c r="BF33" s="122"/>
       <c r="BG33" s="123"/>
     </row>
-    <row r="34" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="34" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B34" s="114"/>
       <c r="C34" s="112"/>
       <c r="D34" s="110"/>
@@ -4376,16 +4393,16 @@
       <c r="AW34" s="126"/>
       <c r="AX34" s="126"/>
       <c r="AY34" s="126"/>
-      <c r="AZ34" s="167"/>
-      <c r="BA34" s="168"/>
+      <c r="AZ34" s="148"/>
+      <c r="BA34" s="149"/>
       <c r="BB34" s="126"/>
       <c r="BC34" s="127"/>
-      <c r="BD34" s="226"/>
-      <c r="BE34" s="227"/>
+      <c r="BD34" s="151"/>
+      <c r="BE34" s="152"/>
       <c r="BF34" s="128"/>
       <c r="BG34" s="129"/>
     </row>
-    <row r="35" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="35" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B35" s="114"/>
       <c r="C35" s="112"/>
       <c r="D35" s="110"/>
@@ -4436,16 +4453,16 @@
       <c r="AW35" s="126"/>
       <c r="AX35" s="126"/>
       <c r="AY35" s="126"/>
-      <c r="AZ35" s="167"/>
-      <c r="BA35" s="168"/>
+      <c r="AZ35" s="148"/>
+      <c r="BA35" s="149"/>
       <c r="BB35" s="126"/>
       <c r="BC35" s="127"/>
-      <c r="BD35" s="226"/>
-      <c r="BE35" s="227"/>
+      <c r="BD35" s="151"/>
+      <c r="BE35" s="152"/>
       <c r="BF35" s="128"/>
       <c r="BG35" s="129"/>
     </row>
-    <row r="36" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="36" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B36" s="114"/>
       <c r="C36" s="112"/>
       <c r="D36" s="110"/>
@@ -4496,16 +4513,16 @@
       <c r="AW36" s="126"/>
       <c r="AX36" s="126"/>
       <c r="AY36" s="126"/>
-      <c r="AZ36" s="167"/>
-      <c r="BA36" s="168"/>
+      <c r="AZ36" s="148"/>
+      <c r="BA36" s="149"/>
       <c r="BB36" s="126"/>
       <c r="BC36" s="127"/>
-      <c r="BD36" s="226"/>
-      <c r="BE36" s="227"/>
+      <c r="BD36" s="151"/>
+      <c r="BE36" s="152"/>
       <c r="BF36" s="128"/>
       <c r="BG36" s="129"/>
     </row>
-    <row r="37" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="37" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B37" s="114"/>
       <c r="C37" s="112"/>
       <c r="D37" s="110"/>
@@ -4556,16 +4573,16 @@
       <c r="AW37" s="126"/>
       <c r="AX37" s="126"/>
       <c r="AY37" s="126"/>
-      <c r="AZ37" s="167"/>
-      <c r="BA37" s="168"/>
+      <c r="AZ37" s="148"/>
+      <c r="BA37" s="149"/>
       <c r="BB37" s="126"/>
       <c r="BC37" s="127"/>
-      <c r="BD37" s="228"/>
-      <c r="BE37" s="229"/>
+      <c r="BD37" s="153"/>
+      <c r="BE37" s="154"/>
       <c r="BF37" s="130"/>
       <c r="BG37" s="131"/>
     </row>
-    <row r="38" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1">
+    <row r="38" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B38" s="114"/>
       <c r="C38" s="112"/>
       <c r="D38" s="110"/>
@@ -4616,16 +4633,16 @@
       <c r="AW38" s="126"/>
       <c r="AX38" s="126"/>
       <c r="AY38" s="126"/>
-      <c r="AZ38" s="167"/>
-      <c r="BA38" s="168"/>
+      <c r="AZ38" s="148"/>
+      <c r="BA38" s="149"/>
       <c r="BB38" s="126"/>
       <c r="BC38" s="127"/>
-      <c r="BD38" s="226"/>
-      <c r="BE38" s="227"/>
+      <c r="BD38" s="151"/>
+      <c r="BE38" s="152"/>
       <c r="BF38" s="128"/>
       <c r="BG38" s="129"/>
     </row>
-    <row r="39" spans="2:59" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+    <row r="39" spans="2:59" s="2" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B39" s="132"/>
       <c r="C39" s="133"/>
       <c r="D39" s="134"/>
@@ -4676,57 +4693,57 @@
       <c r="AW39" s="139"/>
       <c r="AX39" s="139"/>
       <c r="AY39" s="139"/>
-      <c r="AZ39" s="230"/>
-      <c r="BA39" s="231"/>
+      <c r="AZ39" s="155"/>
+      <c r="BA39" s="156"/>
       <c r="BB39" s="139"/>
       <c r="BC39" s="140"/>
-      <c r="BD39" s="161"/>
-      <c r="BE39" s="162"/>
+      <c r="BD39" s="198"/>
+      <c r="BE39" s="199"/>
       <c r="BF39" s="141"/>
       <c r="BG39" s="142"/>
     </row>
-    <row r="40" spans="2:59" ht="30.75" customHeight="1" thickBot="1">
-      <c r="B40" s="234" t="s">
+    <row r="40" spans="2:59" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="143" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="234"/>
-      <c r="D40" s="234"/>
-      <c r="E40" s="234"/>
-      <c r="F40" s="234"/>
-      <c r="G40" s="234"/>
-      <c r="H40" s="234"/>
-      <c r="I40" s="234"/>
+      <c r="C40" s="143"/>
+      <c r="D40" s="143"/>
+      <c r="E40" s="143"/>
+      <c r="F40" s="143"/>
+      <c r="G40" s="143"/>
+      <c r="H40" s="143"/>
+      <c r="I40" s="143"/>
       <c r="AC40" s="66"/>
       <c r="AD40" s="66"/>
       <c r="AE40" s="66"/>
       <c r="AF40" s="66"/>
       <c r="AG40" s="81"/>
-      <c r="AH40" s="236" t="s">
+      <c r="AH40" s="145" t="s">
         <v>37</v>
       </c>
-      <c r="AI40" s="236"/>
-      <c r="AJ40" s="236"/>
-      <c r="AK40" s="236"/>
-      <c r="AL40" s="236"/>
+      <c r="AI40" s="145"/>
+      <c r="AJ40" s="145"/>
+      <c r="AK40" s="145"/>
+      <c r="AL40" s="145"/>
       <c r="AM40" s="103"/>
       <c r="AO40" s="87"/>
-      <c r="BD40" s="232" t="str">
+      <c r="BD40" s="157" t="str">
         <f>IF(SUM(BD33:BD39)=0,"",SUM(BD33:BD39))</f>
         <v/>
       </c>
-      <c r="BE40" s="233"/>
+      <c r="BE40" s="158"/>
     </row>
-    <row r="41" spans="2:59" ht="14.25">
-      <c r="B41" s="235" t="s">
+    <row r="41" spans="2:59" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B41" s="144" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="235"/>
-      <c r="D41" s="235"/>
-      <c r="E41" s="235"/>
-      <c r="F41" s="235"/>
-      <c r="G41" s="235"/>
-      <c r="H41" s="235"/>
-      <c r="I41" s="235"/>
+      <c r="C41" s="144"/>
+      <c r="D41" s="144"/>
+      <c r="E41" s="144"/>
+      <c r="F41" s="144"/>
+      <c r="G41" s="144"/>
+      <c r="H41" s="144"/>
+      <c r="I41" s="144"/>
       <c r="AC41" s="66"/>
       <c r="AD41" s="66"/>
       <c r="AE41" s="66"/>
@@ -4738,19 +4755,19 @@
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="2:59" ht="14.25">
-      <c r="B42" s="235" t="s">
+    <row r="42" spans="2:59" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="B42" s="144" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="235"/>
-      <c r="D42" s="235"/>
-      <c r="E42" s="235"/>
-      <c r="F42" s="235"/>
-      <c r="G42" s="235"/>
-      <c r="H42" s="235"/>
-      <c r="I42" s="235"/>
+      <c r="C42" s="144"/>
+      <c r="D42" s="144"/>
+      <c r="E42" s="144"/>
+      <c r="F42" s="144"/>
+      <c r="G42" s="144"/>
+      <c r="H42" s="144"/>
+      <c r="I42" s="144"/>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="54"/>
       <c r="B51" s="54"/>
       <c r="C51" s="54"/>
@@ -4762,24 +4779,120 @@
     <protectedRange password="EB2E" sqref="AN10:AO17 V10:W17" name="Range1"/>
   </protectedRanges>
   <mergeCells count="156">
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="AH40:AL40"/>
-    <mergeCell ref="AZ33:BA33"/>
-    <mergeCell ref="AZ34:BA34"/>
-    <mergeCell ref="AZ35:BA35"/>
-    <mergeCell ref="AZ36:BA36"/>
-    <mergeCell ref="AZ37:BA37"/>
-    <mergeCell ref="AN16:AP16"/>
-    <mergeCell ref="AN15:AP15"/>
-    <mergeCell ref="BD34:BE34"/>
-    <mergeCell ref="BD35:BE35"/>
-    <mergeCell ref="BD36:BE36"/>
-    <mergeCell ref="BD37:BE37"/>
-    <mergeCell ref="BD38:BE38"/>
-    <mergeCell ref="AZ39:BA39"/>
-    <mergeCell ref="BD40:BE40"/>
+    <mergeCell ref="BF31:BG32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:AD32"/>
+    <mergeCell ref="AE32:AN32"/>
+    <mergeCell ref="AO32:BC32"/>
+    <mergeCell ref="AI19:AM19"/>
+    <mergeCell ref="AI24:AM24"/>
+    <mergeCell ref="AI26:AM26"/>
+    <mergeCell ref="G26:Q28"/>
+    <mergeCell ref="G23:X25"/>
+    <mergeCell ref="S26:W28"/>
+    <mergeCell ref="S19:W20"/>
+    <mergeCell ref="G19:Q20"/>
+    <mergeCell ref="Y19:AB20"/>
+    <mergeCell ref="S21:W21"/>
+    <mergeCell ref="S29:W29"/>
+    <mergeCell ref="AD19:AH29"/>
+    <mergeCell ref="AO24:AP24"/>
+    <mergeCell ref="AB16:AD16"/>
+    <mergeCell ref="Y26:AB28"/>
+    <mergeCell ref="BD39:BE39"/>
+    <mergeCell ref="BD31:BE32"/>
+    <mergeCell ref="AZ38:BA38"/>
+    <mergeCell ref="BD33:BE33"/>
+    <mergeCell ref="Y21:AA21"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="S10:U10"/>
+    <mergeCell ref="S11:U11"/>
+    <mergeCell ref="S12:U12"/>
+    <mergeCell ref="S13:U13"/>
+    <mergeCell ref="AE16:AG16"/>
+    <mergeCell ref="V16:X16"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="B32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="V10:X10"/>
+    <mergeCell ref="P12:R12"/>
+    <mergeCell ref="P13:R13"/>
+    <mergeCell ref="P11:R11"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="Y12:AA12"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE13:AG13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="AB13:AD13"/>
+    <mergeCell ref="Y14:AA14"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="Y4:AC4"/>
+    <mergeCell ref="AK5:AP6"/>
+    <mergeCell ref="X6:AI6"/>
+    <mergeCell ref="AA7:AI7"/>
+    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="AE5:AI5"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="P6:T7"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="AB12:AD12"/>
+    <mergeCell ref="AN9:AP9"/>
+    <mergeCell ref="G1:AJ1"/>
+    <mergeCell ref="AK11:AM11"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="AK12:AM12"/>
+    <mergeCell ref="AK13:AM13"/>
+    <mergeCell ref="AK14:AM14"/>
+    <mergeCell ref="AK15:AM15"/>
+    <mergeCell ref="AK16:AM16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AH12:AJ12"/>
+    <mergeCell ref="AB14:AD14"/>
     <mergeCell ref="AN14:AP14"/>
     <mergeCell ref="Y29:AA29"/>
     <mergeCell ref="Y15:AA15"/>
@@ -4804,120 +4917,24 @@
     <mergeCell ref="AO21:AP21"/>
     <mergeCell ref="AO28:AP28"/>
     <mergeCell ref="AI28:AM28"/>
-    <mergeCell ref="G1:AJ1"/>
-    <mergeCell ref="AK11:AM11"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="AK12:AM12"/>
-    <mergeCell ref="AK13:AM13"/>
-    <mergeCell ref="AK14:AM14"/>
-    <mergeCell ref="AK15:AM15"/>
-    <mergeCell ref="AK16:AM16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="Y16:AA16"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="AH9:AJ9"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AH12:AJ12"/>
-    <mergeCell ref="AB14:AD14"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="AK5:AP6"/>
-    <mergeCell ref="X6:AI6"/>
-    <mergeCell ref="AA7:AI7"/>
-    <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="AE5:AI5"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="P6:T7"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="AB12:AD12"/>
-    <mergeCell ref="AN9:AP9"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="AK9:AM9"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="AB10:AD10"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AE13:AG13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="AB13:AD13"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="AB16:AD16"/>
-    <mergeCell ref="Y26:AB28"/>
-    <mergeCell ref="BD39:BE39"/>
-    <mergeCell ref="BD31:BE32"/>
-    <mergeCell ref="AZ38:BA38"/>
-    <mergeCell ref="BD33:BE33"/>
-    <mergeCell ref="Y21:AA21"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="S10:U10"/>
-    <mergeCell ref="S11:U11"/>
-    <mergeCell ref="S12:U12"/>
-    <mergeCell ref="S13:U13"/>
-    <mergeCell ref="AE16:AG16"/>
-    <mergeCell ref="V16:X16"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="B32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="P10:R10"/>
-    <mergeCell ref="V10:X10"/>
-    <mergeCell ref="P12:R12"/>
-    <mergeCell ref="P13:R13"/>
-    <mergeCell ref="P11:R11"/>
-    <mergeCell ref="BF31:BG32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:AD32"/>
-    <mergeCell ref="AE32:AN32"/>
-    <mergeCell ref="AO32:BC32"/>
-    <mergeCell ref="AI19:AM19"/>
-    <mergeCell ref="AI24:AM24"/>
-    <mergeCell ref="AI26:AM26"/>
-    <mergeCell ref="G26:Q28"/>
-    <mergeCell ref="G23:X25"/>
-    <mergeCell ref="S26:W28"/>
-    <mergeCell ref="S19:W20"/>
-    <mergeCell ref="G19:Q20"/>
-    <mergeCell ref="Y19:AB20"/>
-    <mergeCell ref="S21:W21"/>
-    <mergeCell ref="S29:W29"/>
-    <mergeCell ref="AD19:AH29"/>
-    <mergeCell ref="AO24:AP24"/>
+    <mergeCell ref="AN16:AP16"/>
+    <mergeCell ref="AN15:AP15"/>
+    <mergeCell ref="BD34:BE34"/>
+    <mergeCell ref="BD35:BE35"/>
+    <mergeCell ref="BD36:BE36"/>
+    <mergeCell ref="BD37:BE37"/>
+    <mergeCell ref="BD38:BE38"/>
+    <mergeCell ref="AZ39:BA39"/>
+    <mergeCell ref="BD40:BE40"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="AH40:AL40"/>
+    <mergeCell ref="AZ33:BA33"/>
+    <mergeCell ref="AZ34:BA34"/>
+    <mergeCell ref="AZ35:BA35"/>
+    <mergeCell ref="AZ36:BA36"/>
+    <mergeCell ref="AZ37:BA37"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations xWindow="252" yWindow="215" count="4">

</xml_diff>

<commit_message>
start to finalize everything
</commit_message>
<xml_diff>
--- a/2012 CALTRANS TIMESHEET 0727-0809.xlsx
+++ b/2012 CALTRANS TIMESHEET 0727-0809.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView showSheetTabs="0" xWindow="360" yWindow="15" windowWidth="9720" windowHeight="6540"/>
+    <workbookView showSheetTabs="0" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Caltrans Student Timesheet" sheetId="1" r:id="rId1"/>
@@ -1428,6 +1428,310 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="18" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1442,310 +1746,6 @@
     </xf>
     <xf numFmtId="165" fontId="23" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="24" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="18" fontId="14" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="43" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="44" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="18" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2328,7 +2328,7 @@
   <dimension ref="A1:BG51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="BE21" sqref="BE21"/>
+      <selection activeCell="G19" sqref="G19:Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2362,38 +2362,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:53" ht="24.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="G1" s="173" t="s">
+      <c r="G1" s="219" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="173"/>
-      <c r="I1" s="173"/>
-      <c r="J1" s="173"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="173"/>
-      <c r="AD1" s="173"/>
-      <c r="AE1" s="173"/>
-      <c r="AF1" s="173"/>
-      <c r="AG1" s="173"/>
-      <c r="AH1" s="173"/>
-      <c r="AI1" s="173"/>
-      <c r="AJ1" s="173"/>
+      <c r="H1" s="219"/>
+      <c r="I1" s="219"/>
+      <c r="J1" s="219"/>
+      <c r="K1" s="219"/>
+      <c r="L1" s="219"/>
+      <c r="M1" s="219"/>
+      <c r="N1" s="219"/>
+      <c r="O1" s="219"/>
+      <c r="P1" s="219"/>
+      <c r="Q1" s="219"/>
+      <c r="R1" s="219"/>
+      <c r="S1" s="219"/>
+      <c r="T1" s="219"/>
+      <c r="U1" s="219"/>
+      <c r="V1" s="219"/>
+      <c r="W1" s="219"/>
+      <c r="X1" s="219"/>
+      <c r="Y1" s="219"/>
+      <c r="Z1" s="219"/>
+      <c r="AA1" s="219"/>
+      <c r="AB1" s="219"/>
+      <c r="AC1" s="219"/>
+      <c r="AD1" s="219"/>
+      <c r="AE1" s="219"/>
+      <c r="AF1" s="219"/>
+      <c r="AG1" s="219"/>
+      <c r="AH1" s="219"/>
+      <c r="AI1" s="219"/>
+      <c r="AJ1" s="219"/>
       <c r="AK1" s="71" t="s">
         <v>15</v>
       </c>
@@ -2465,23 +2465,23 @@
       <c r="V4" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="Y4" s="175">
-        <v>41875</v>
-      </c>
-      <c r="Z4" s="175"/>
-      <c r="AA4" s="175"/>
-      <c r="AB4" s="175"/>
-      <c r="AC4" s="175"/>
+      <c r="Y4" s="200">
+        <v>41889</v>
+      </c>
+      <c r="Z4" s="200"/>
+      <c r="AA4" s="200"/>
+      <c r="AB4" s="200"/>
+      <c r="AC4" s="200"/>
       <c r="AD4" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="AE4" s="175">
-        <v>41888</v>
-      </c>
-      <c r="AF4" s="175"/>
-      <c r="AG4" s="175"/>
-      <c r="AH4" s="175"/>
-      <c r="AI4" s="175"/>
+      <c r="AE4" s="200">
+        <v>41902</v>
+      </c>
+      <c r="AF4" s="200"/>
+      <c r="AG4" s="200"/>
+      <c r="AH4" s="200"/>
+      <c r="AI4" s="200"/>
       <c r="AO4" s="27"/>
       <c r="AP4" s="27"/>
       <c r="AQ4" s="3"/>
@@ -2497,66 +2497,66 @@
       <c r="R5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="Y5" s="174" t="s">
+      <c r="Y5" s="199" t="s">
         <v>25</v>
       </c>
-      <c r="Z5" s="174"/>
-      <c r="AA5" s="174"/>
-      <c r="AB5" s="174"/>
-      <c r="AC5" s="174"/>
+      <c r="Z5" s="199"/>
+      <c r="AA5" s="199"/>
+      <c r="AB5" s="199"/>
+      <c r="AC5" s="199"/>
       <c r="AD5" s="33"/>
-      <c r="AE5" s="174" t="s">
+      <c r="AE5" s="199" t="s">
         <v>25</v>
       </c>
-      <c r="AF5" s="174"/>
-      <c r="AG5" s="174"/>
-      <c r="AH5" s="174"/>
-      <c r="AI5" s="174"/>
+      <c r="AF5" s="199"/>
+      <c r="AG5" s="199"/>
+      <c r="AH5" s="199"/>
+      <c r="AI5" s="199"/>
       <c r="AJ5" s="34"/>
-      <c r="AK5" s="176" t="s">
+      <c r="AK5" s="201" t="s">
         <v>61</v>
       </c>
-      <c r="AL5" s="177"/>
-      <c r="AM5" s="177"/>
-      <c r="AN5" s="177"/>
-      <c r="AO5" s="177"/>
-      <c r="AP5" s="178"/>
+      <c r="AL5" s="202"/>
+      <c r="AM5" s="202"/>
+      <c r="AN5" s="202"/>
+      <c r="AO5" s="202"/>
+      <c r="AP5" s="203"/>
       <c r="AQ5" s="3"/>
     </row>
     <row r="6" spans="1:53" ht="21.75" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="M6" s="57"/>
       <c r="N6" s="57"/>
       <c r="O6" s="69"/>
-      <c r="P6" s="184" t="s">
+      <c r="P6" s="209" t="s">
         <v>60</v>
       </c>
-      <c r="Q6" s="184"/>
-      <c r="R6" s="184"/>
-      <c r="S6" s="184"/>
-      <c r="T6" s="185"/>
+      <c r="Q6" s="209"/>
+      <c r="R6" s="209"/>
+      <c r="S6" s="209"/>
+      <c r="T6" s="210"/>
       <c r="V6" s="68" t="s">
         <v>12</v>
       </c>
       <c r="W6" s="35"/>
-      <c r="X6" s="182"/>
-      <c r="Y6" s="182"/>
-      <c r="Z6" s="182"/>
-      <c r="AA6" s="182"/>
-      <c r="AB6" s="182"/>
-      <c r="AC6" s="182"/>
-      <c r="AD6" s="182"/>
-      <c r="AE6" s="182"/>
-      <c r="AF6" s="182"/>
-      <c r="AG6" s="182"/>
-      <c r="AH6" s="182"/>
-      <c r="AI6" s="182"/>
+      <c r="X6" s="207"/>
+      <c r="Y6" s="207"/>
+      <c r="Z6" s="207"/>
+      <c r="AA6" s="207"/>
+      <c r="AB6" s="207"/>
+      <c r="AC6" s="207"/>
+      <c r="AD6" s="207"/>
+      <c r="AE6" s="207"/>
+      <c r="AF6" s="207"/>
+      <c r="AG6" s="207"/>
+      <c r="AH6" s="207"/>
+      <c r="AI6" s="207"/>
       <c r="AJ6" s="34"/>
-      <c r="AK6" s="179"/>
-      <c r="AL6" s="180"/>
-      <c r="AM6" s="180"/>
-      <c r="AN6" s="180"/>
-      <c r="AO6" s="180"/>
-      <c r="AP6" s="181"/>
+      <c r="AK6" s="204"/>
+      <c r="AL6" s="205"/>
+      <c r="AM6" s="205"/>
+      <c r="AN6" s="205"/>
+      <c r="AO6" s="205"/>
+      <c r="AP6" s="206"/>
       <c r="AQ6" s="3"/>
     </row>
     <row r="7" spans="1:53" ht="24" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -2566,11 +2566,11 @@
       <c r="M7" s="57"/>
       <c r="N7" s="57"/>
       <c r="O7" s="69"/>
-      <c r="P7" s="186"/>
-      <c r="Q7" s="186"/>
-      <c r="R7" s="186"/>
-      <c r="S7" s="186"/>
-      <c r="T7" s="187"/>
+      <c r="P7" s="211"/>
+      <c r="Q7" s="211"/>
+      <c r="R7" s="211"/>
+      <c r="S7" s="211"/>
+      <c r="T7" s="212"/>
       <c r="V7" s="66" t="s">
         <v>13</v>
       </c>
@@ -2578,23 +2578,23 @@
       <c r="X7" s="77"/>
       <c r="Y7" s="78"/>
       <c r="Z7" s="78"/>
-      <c r="AA7" s="183"/>
-      <c r="AB7" s="183"/>
-      <c r="AC7" s="183"/>
-      <c r="AD7" s="183"/>
-      <c r="AE7" s="183"/>
-      <c r="AF7" s="183"/>
-      <c r="AG7" s="183"/>
-      <c r="AH7" s="183"/>
-      <c r="AI7" s="183"/>
-      <c r="AK7" s="174" t="s">
+      <c r="AA7" s="208"/>
+      <c r="AB7" s="208"/>
+      <c r="AC7" s="208"/>
+      <c r="AD7" s="208"/>
+      <c r="AE7" s="208"/>
+      <c r="AF7" s="208"/>
+      <c r="AG7" s="208"/>
+      <c r="AH7" s="208"/>
+      <c r="AI7" s="208"/>
+      <c r="AK7" s="199" t="s">
         <v>14</v>
       </c>
-      <c r="AL7" s="174"/>
-      <c r="AM7" s="174"/>
-      <c r="AN7" s="174"/>
-      <c r="AO7" s="174"/>
-      <c r="AP7" s="174"/>
+      <c r="AL7" s="199"/>
+      <c r="AM7" s="199"/>
+      <c r="AN7" s="199"/>
+      <c r="AO7" s="199"/>
+      <c r="AP7" s="199"/>
       <c r="AQ7" s="3"/>
     </row>
     <row r="8" spans="1:53" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2624,62 +2624,62 @@
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
       <c r="F9" s="37"/>
-      <c r="G9" s="191"/>
-      <c r="H9" s="192"/>
-      <c r="I9" s="193"/>
-      <c r="J9" s="160" t="s">
+      <c r="G9" s="216"/>
+      <c r="H9" s="217"/>
+      <c r="I9" s="218"/>
+      <c r="J9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="160"/>
-      <c r="L9" s="160"/>
-      <c r="M9" s="160" t="s">
+      <c r="K9" s="193"/>
+      <c r="L9" s="193"/>
+      <c r="M9" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="N9" s="160"/>
-      <c r="O9" s="160"/>
-      <c r="P9" s="160" t="s">
+      <c r="N9" s="193"/>
+      <c r="O9" s="193"/>
+      <c r="P9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="160"/>
-      <c r="R9" s="160"/>
-      <c r="S9" s="188" t="s">
+      <c r="Q9" s="193"/>
+      <c r="R9" s="193"/>
+      <c r="S9" s="213" t="s">
         <v>19</v>
       </c>
-      <c r="T9" s="189"/>
-      <c r="U9" s="190"/>
-      <c r="V9" s="160" t="s">
+      <c r="T9" s="214"/>
+      <c r="U9" s="215"/>
+      <c r="V9" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="W9" s="160"/>
-      <c r="X9" s="160"/>
+      <c r="W9" s="193"/>
+      <c r="X9" s="193"/>
       <c r="Y9" s="195"/>
       <c r="Z9" s="195"/>
       <c r="AA9" s="195"/>
-      <c r="AB9" s="160" t="s">
+      <c r="AB9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="AC9" s="160"/>
-      <c r="AD9" s="160"/>
+      <c r="AC9" s="193"/>
+      <c r="AD9" s="193"/>
       <c r="AE9" s="194" t="s">
         <v>19</v>
       </c>
       <c r="AF9" s="194"/>
       <c r="AG9" s="194"/>
-      <c r="AH9" s="160" t="s">
+      <c r="AH9" s="193" t="s">
         <v>18</v>
       </c>
-      <c r="AI9" s="160"/>
-      <c r="AJ9" s="160"/>
-      <c r="AK9" s="160" t="s">
+      <c r="AI9" s="193"/>
+      <c r="AJ9" s="193"/>
+      <c r="AK9" s="193" t="s">
         <v>19</v>
       </c>
-      <c r="AL9" s="160"/>
-      <c r="AM9" s="160"/>
-      <c r="AN9" s="160" t="s">
+      <c r="AL9" s="193"/>
+      <c r="AM9" s="193"/>
+      <c r="AN9" s="193" t="s">
         <v>20</v>
       </c>
-      <c r="AO9" s="160"/>
-      <c r="AP9" s="160"/>
+      <c r="AO9" s="193"/>
+      <c r="AP9" s="193"/>
       <c r="AQ9" s="21" t="s">
         <v>40</v>
       </c>
@@ -2719,52 +2719,52 @@
       <c r="D10" s="82"/>
       <c r="E10" s="82"/>
       <c r="F10" s="83"/>
-      <c r="G10" s="160" t="s">
+      <c r="G10" s="193" t="s">
         <v>4</v>
       </c>
-      <c r="H10" s="160"/>
-      <c r="I10" s="160"/>
-      <c r="J10" s="164"/>
-      <c r="K10" s="164"/>
-      <c r="L10" s="164"/>
-      <c r="M10" s="164"/>
-      <c r="N10" s="164"/>
-      <c r="O10" s="164"/>
-      <c r="P10" s="164"/>
-      <c r="Q10" s="164"/>
-      <c r="R10" s="164"/>
-      <c r="S10" s="164"/>
-      <c r="T10" s="164"/>
-      <c r="U10" s="164"/>
-      <c r="V10" s="150">
+      <c r="H10" s="193"/>
+      <c r="I10" s="193"/>
+      <c r="J10" s="179"/>
+      <c r="K10" s="179"/>
+      <c r="L10" s="179"/>
+      <c r="M10" s="179"/>
+      <c r="N10" s="179"/>
+      <c r="O10" s="179"/>
+      <c r="P10" s="179"/>
+      <c r="Q10" s="179"/>
+      <c r="R10" s="179"/>
+      <c r="S10" s="179"/>
+      <c r="T10" s="179"/>
+      <c r="U10" s="179"/>
+      <c r="V10" s="192">
         <f>((M10-J10)+(S10-P10))</f>
         <v>0</v>
       </c>
-      <c r="W10" s="150"/>
-      <c r="X10" s="150"/>
-      <c r="Y10" s="160" t="s">
+      <c r="W10" s="192"/>
+      <c r="X10" s="192"/>
+      <c r="Y10" s="193" t="s">
         <v>4</v>
       </c>
-      <c r="Z10" s="160"/>
-      <c r="AA10" s="160"/>
-      <c r="AB10" s="164"/>
-      <c r="AC10" s="164"/>
-      <c r="AD10" s="164"/>
-      <c r="AE10" s="164"/>
-      <c r="AF10" s="164"/>
-      <c r="AG10" s="164"/>
-      <c r="AH10" s="164"/>
-      <c r="AI10" s="164"/>
-      <c r="AJ10" s="164"/>
-      <c r="AK10" s="164"/>
-      <c r="AL10" s="164"/>
-      <c r="AM10" s="164"/>
-      <c r="AN10" s="150">
+      <c r="Z10" s="193"/>
+      <c r="AA10" s="193"/>
+      <c r="AB10" s="179"/>
+      <c r="AC10" s="179"/>
+      <c r="AD10" s="179"/>
+      <c r="AE10" s="179"/>
+      <c r="AF10" s="179"/>
+      <c r="AG10" s="179"/>
+      <c r="AH10" s="179"/>
+      <c r="AI10" s="179"/>
+      <c r="AJ10" s="179"/>
+      <c r="AK10" s="179"/>
+      <c r="AL10" s="179"/>
+      <c r="AM10" s="179"/>
+      <c r="AN10" s="192">
         <f t="shared" ref="AN10:AN16" si="0">((AE10-AB10)+(AK10-AH10))</f>
         <v>0</v>
       </c>
-      <c r="AO10" s="150"/>
-      <c r="AP10" s="150"/>
+      <c r="AO10" s="192"/>
+      <c r="AP10" s="192"/>
       <c r="AQ10" s="22">
         <f>MIN(8/24,V10)</f>
         <v>0</v>
@@ -2814,68 +2814,68 @@
       <c r="D11" s="82"/>
       <c r="E11" s="82"/>
       <c r="F11" s="83"/>
-      <c r="G11" s="160" t="s">
+      <c r="G11" s="193" t="s">
         <v>5</v>
       </c>
-      <c r="H11" s="160"/>
-      <c r="I11" s="160"/>
-      <c r="J11" s="164">
+      <c r="H11" s="193"/>
+      <c r="I11" s="193"/>
+      <c r="J11" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K11" s="164"/>
-      <c r="L11" s="164"/>
-      <c r="M11" s="164">
+      <c r="K11" s="179"/>
+      <c r="L11" s="179"/>
+      <c r="M11" s="179">
         <v>0.5</v>
       </c>
-      <c r="N11" s="164"/>
-      <c r="O11" s="164"/>
-      <c r="P11" s="164">
+      <c r="N11" s="179"/>
+      <c r="O11" s="179"/>
+      <c r="P11" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q11" s="164"/>
-      <c r="R11" s="164"/>
-      <c r="S11" s="164">
+      <c r="Q11" s="179"/>
+      <c r="R11" s="179"/>
+      <c r="S11" s="179">
         <v>0.6875</v>
       </c>
-      <c r="T11" s="164"/>
-      <c r="U11" s="164"/>
-      <c r="V11" s="150">
+      <c r="T11" s="179"/>
+      <c r="U11" s="179"/>
+      <c r="V11" s="192">
         <f t="shared" ref="V11:V16" si="7">((M11-J11)+(S11-P11))</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W11" s="150"/>
-      <c r="X11" s="150"/>
-      <c r="Y11" s="160" t="s">
+      <c r="W11" s="192"/>
+      <c r="X11" s="192"/>
+      <c r="Y11" s="193" t="s">
         <v>5</v>
       </c>
-      <c r="Z11" s="160"/>
-      <c r="AA11" s="160"/>
-      <c r="AB11" s="164">
+      <c r="Z11" s="193"/>
+      <c r="AA11" s="193"/>
+      <c r="AB11" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC11" s="164"/>
-      <c r="AD11" s="164"/>
-      <c r="AE11" s="161">
+      <c r="AC11" s="179"/>
+      <c r="AD11" s="179"/>
+      <c r="AE11" s="196">
         <v>0.5</v>
       </c>
-      <c r="AF11" s="162"/>
-      <c r="AG11" s="163"/>
-      <c r="AH11" s="164">
+      <c r="AF11" s="197"/>
+      <c r="AG11" s="198"/>
+      <c r="AH11" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI11" s="164"/>
-      <c r="AJ11" s="164"/>
-      <c r="AK11" s="164">
+      <c r="AI11" s="179"/>
+      <c r="AJ11" s="179"/>
+      <c r="AK11" s="179">
         <v>0.6875</v>
       </c>
-      <c r="AL11" s="164"/>
-      <c r="AM11" s="164"/>
-      <c r="AN11" s="150">
+      <c r="AL11" s="179"/>
+      <c r="AM11" s="179"/>
+      <c r="AN11" s="192">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO11" s="150"/>
-      <c r="AP11" s="150"/>
+      <c r="AO11" s="192"/>
+      <c r="AP11" s="192"/>
       <c r="AQ11" s="22">
         <f t="shared" ref="AQ11:AQ16" si="8">MIN(8/24,V11)</f>
         <v>0.33333333333333331</v>
@@ -2925,68 +2925,68 @@
       <c r="D12" s="82"/>
       <c r="E12" s="82"/>
       <c r="F12" s="83"/>
-      <c r="G12" s="160" t="s">
+      <c r="G12" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="H12" s="160"/>
-      <c r="I12" s="160"/>
-      <c r="J12" s="164">
+      <c r="H12" s="193"/>
+      <c r="I12" s="193"/>
+      <c r="J12" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K12" s="164"/>
-      <c r="L12" s="164"/>
-      <c r="M12" s="164">
+      <c r="K12" s="179"/>
+      <c r="L12" s="179"/>
+      <c r="M12" s="179">
         <v>0.5</v>
       </c>
-      <c r="N12" s="164"/>
-      <c r="O12" s="164"/>
-      <c r="P12" s="164">
+      <c r="N12" s="179"/>
+      <c r="O12" s="179"/>
+      <c r="P12" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q12" s="164"/>
-      <c r="R12" s="164"/>
-      <c r="S12" s="164">
+      <c r="Q12" s="179"/>
+      <c r="R12" s="179"/>
+      <c r="S12" s="179">
         <v>0.6875</v>
       </c>
-      <c r="T12" s="164"/>
-      <c r="U12" s="164"/>
-      <c r="V12" s="150">
+      <c r="T12" s="179"/>
+      <c r="U12" s="179"/>
+      <c r="V12" s="192">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W12" s="150"/>
-      <c r="X12" s="150"/>
-      <c r="Y12" s="160" t="s">
+      <c r="W12" s="192"/>
+      <c r="X12" s="192"/>
+      <c r="Y12" s="193" t="s">
         <v>6</v>
       </c>
-      <c r="Z12" s="160"/>
-      <c r="AA12" s="160"/>
-      <c r="AB12" s="164">
+      <c r="Z12" s="193"/>
+      <c r="AA12" s="193"/>
+      <c r="AB12" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC12" s="164"/>
-      <c r="AD12" s="164"/>
-      <c r="AE12" s="161">
+      <c r="AC12" s="179"/>
+      <c r="AD12" s="179"/>
+      <c r="AE12" s="196">
         <v>0.5</v>
       </c>
-      <c r="AF12" s="162"/>
-      <c r="AG12" s="163"/>
-      <c r="AH12" s="164">
+      <c r="AF12" s="197"/>
+      <c r="AG12" s="198"/>
+      <c r="AH12" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI12" s="164"/>
-      <c r="AJ12" s="164"/>
-      <c r="AK12" s="164">
+      <c r="AI12" s="179"/>
+      <c r="AJ12" s="179"/>
+      <c r="AK12" s="179">
         <v>0.6875</v>
       </c>
-      <c r="AL12" s="164"/>
-      <c r="AM12" s="164"/>
-      <c r="AN12" s="150">
+      <c r="AL12" s="179"/>
+      <c r="AM12" s="179"/>
+      <c r="AN12" s="192">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO12" s="150"/>
-      <c r="AP12" s="150"/>
+      <c r="AO12" s="192"/>
+      <c r="AP12" s="192"/>
       <c r="AQ12" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3036,68 +3036,68 @@
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
       <c r="F13" s="83"/>
-      <c r="G13" s="160" t="s">
+      <c r="G13" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="160"/>
-      <c r="I13" s="160"/>
-      <c r="J13" s="164">
+      <c r="H13" s="193"/>
+      <c r="I13" s="193"/>
+      <c r="J13" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K13" s="164"/>
-      <c r="L13" s="164"/>
-      <c r="M13" s="164">
+      <c r="K13" s="179"/>
+      <c r="L13" s="179"/>
+      <c r="M13" s="179">
         <v>0.5</v>
       </c>
-      <c r="N13" s="164"/>
-      <c r="O13" s="164"/>
-      <c r="P13" s="164">
+      <c r="N13" s="179"/>
+      <c r="O13" s="179"/>
+      <c r="P13" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q13" s="164"/>
-      <c r="R13" s="164"/>
-      <c r="S13" s="164">
+      <c r="Q13" s="179"/>
+      <c r="R13" s="179"/>
+      <c r="S13" s="179">
         <v>0.6875</v>
       </c>
-      <c r="T13" s="164"/>
-      <c r="U13" s="164"/>
-      <c r="V13" s="150">
+      <c r="T13" s="179"/>
+      <c r="U13" s="179"/>
+      <c r="V13" s="192">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W13" s="150"/>
-      <c r="X13" s="150"/>
-      <c r="Y13" s="160" t="s">
+      <c r="W13" s="192"/>
+      <c r="X13" s="192"/>
+      <c r="Y13" s="193" t="s">
         <v>7</v>
       </c>
-      <c r="Z13" s="160"/>
-      <c r="AA13" s="160"/>
-      <c r="AB13" s="164">
+      <c r="Z13" s="193"/>
+      <c r="AA13" s="193"/>
+      <c r="AB13" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC13" s="164"/>
-      <c r="AD13" s="164"/>
-      <c r="AE13" s="161">
+      <c r="AC13" s="179"/>
+      <c r="AD13" s="179"/>
+      <c r="AE13" s="196">
         <v>0.5</v>
       </c>
-      <c r="AF13" s="162"/>
-      <c r="AG13" s="163"/>
-      <c r="AH13" s="164">
+      <c r="AF13" s="197"/>
+      <c r="AG13" s="198"/>
+      <c r="AH13" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI13" s="164"/>
-      <c r="AJ13" s="164"/>
-      <c r="AK13" s="164">
+      <c r="AI13" s="179"/>
+      <c r="AJ13" s="179"/>
+      <c r="AK13" s="179">
         <v>0.6875</v>
       </c>
-      <c r="AL13" s="164"/>
-      <c r="AM13" s="164"/>
-      <c r="AN13" s="150">
+      <c r="AL13" s="179"/>
+      <c r="AM13" s="179"/>
+      <c r="AN13" s="192">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO13" s="150"/>
-      <c r="AP13" s="150"/>
+      <c r="AO13" s="192"/>
+      <c r="AP13" s="192"/>
       <c r="AQ13" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3147,68 +3147,68 @@
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="56"/>
-      <c r="G14" s="160" t="s">
+      <c r="G14" s="193" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="160"/>
-      <c r="I14" s="160"/>
-      <c r="J14" s="164">
+      <c r="H14" s="193"/>
+      <c r="I14" s="193"/>
+      <c r="J14" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K14" s="164"/>
-      <c r="L14" s="164"/>
-      <c r="M14" s="164">
+      <c r="K14" s="179"/>
+      <c r="L14" s="179"/>
+      <c r="M14" s="179">
         <v>0.5</v>
       </c>
-      <c r="N14" s="164"/>
-      <c r="O14" s="164"/>
-      <c r="P14" s="164">
+      <c r="N14" s="179"/>
+      <c r="O14" s="179"/>
+      <c r="P14" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q14" s="164"/>
-      <c r="R14" s="164"/>
-      <c r="S14" s="164">
+      <c r="Q14" s="179"/>
+      <c r="R14" s="179"/>
+      <c r="S14" s="179">
         <v>0.6875</v>
       </c>
-      <c r="T14" s="164"/>
-      <c r="U14" s="164"/>
-      <c r="V14" s="150">
+      <c r="T14" s="179"/>
+      <c r="U14" s="179"/>
+      <c r="V14" s="192">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W14" s="150"/>
-      <c r="X14" s="150"/>
-      <c r="Y14" s="160" t="s">
+      <c r="W14" s="192"/>
+      <c r="X14" s="192"/>
+      <c r="Y14" s="193" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="160"/>
-      <c r="AA14" s="160"/>
-      <c r="AB14" s="164">
+      <c r="Z14" s="193"/>
+      <c r="AA14" s="193"/>
+      <c r="AB14" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC14" s="164"/>
-      <c r="AD14" s="164"/>
-      <c r="AE14" s="161">
+      <c r="AC14" s="179"/>
+      <c r="AD14" s="179"/>
+      <c r="AE14" s="196">
         <v>0.5</v>
       </c>
-      <c r="AF14" s="162"/>
-      <c r="AG14" s="163"/>
-      <c r="AH14" s="164">
+      <c r="AF14" s="197"/>
+      <c r="AG14" s="198"/>
+      <c r="AH14" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI14" s="164"/>
-      <c r="AJ14" s="164"/>
-      <c r="AK14" s="164">
+      <c r="AI14" s="179"/>
+      <c r="AJ14" s="179"/>
+      <c r="AK14" s="179">
         <v>0.6875</v>
       </c>
-      <c r="AL14" s="164"/>
-      <c r="AM14" s="164"/>
-      <c r="AN14" s="150">
+      <c r="AL14" s="179"/>
+      <c r="AM14" s="179"/>
+      <c r="AN14" s="192">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO14" s="150"/>
-      <c r="AP14" s="150"/>
+      <c r="AO14" s="192"/>
+      <c r="AP14" s="192"/>
       <c r="AQ14" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3258,68 +3258,68 @@
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="56"/>
-      <c r="G15" s="160" t="s">
+      <c r="G15" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="160"/>
-      <c r="I15" s="160"/>
-      <c r="J15" s="164">
+      <c r="H15" s="193"/>
+      <c r="I15" s="193"/>
+      <c r="J15" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K15" s="164"/>
-      <c r="L15" s="164"/>
-      <c r="M15" s="164">
+      <c r="K15" s="179"/>
+      <c r="L15" s="179"/>
+      <c r="M15" s="179">
         <v>0.5</v>
       </c>
-      <c r="N15" s="164"/>
-      <c r="O15" s="164"/>
-      <c r="P15" s="164">
+      <c r="N15" s="179"/>
+      <c r="O15" s="179"/>
+      <c r="P15" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="Q15" s="164"/>
-      <c r="R15" s="164"/>
-      <c r="S15" s="164">
+      <c r="Q15" s="179"/>
+      <c r="R15" s="179"/>
+      <c r="S15" s="179">
         <v>0.6875</v>
       </c>
-      <c r="T15" s="164"/>
-      <c r="U15" s="164"/>
-      <c r="V15" s="150">
+      <c r="T15" s="179"/>
+      <c r="U15" s="179"/>
+      <c r="V15" s="192">
         <f t="shared" si="7"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="W15" s="150"/>
-      <c r="X15" s="150"/>
-      <c r="Y15" s="160" t="s">
+      <c r="W15" s="192"/>
+      <c r="X15" s="192"/>
+      <c r="Y15" s="193" t="s">
         <v>9</v>
       </c>
-      <c r="Z15" s="160"/>
-      <c r="AA15" s="160"/>
-      <c r="AB15" s="164">
+      <c r="Z15" s="193"/>
+      <c r="AA15" s="193"/>
+      <c r="AB15" s="179">
         <v>0.33333333333333331</v>
       </c>
-      <c r="AC15" s="164"/>
-      <c r="AD15" s="164"/>
-      <c r="AE15" s="161">
+      <c r="AC15" s="179"/>
+      <c r="AD15" s="179"/>
+      <c r="AE15" s="196">
         <v>0.5</v>
       </c>
-      <c r="AF15" s="162"/>
-      <c r="AG15" s="163"/>
-      <c r="AH15" s="164">
+      <c r="AF15" s="197"/>
+      <c r="AG15" s="198"/>
+      <c r="AH15" s="179">
         <v>0.52083333333333337</v>
       </c>
-      <c r="AI15" s="164"/>
-      <c r="AJ15" s="164"/>
-      <c r="AK15" s="164">
+      <c r="AI15" s="179"/>
+      <c r="AJ15" s="179"/>
+      <c r="AK15" s="179">
         <v>0.6875</v>
       </c>
-      <c r="AL15" s="164"/>
-      <c r="AM15" s="164"/>
-      <c r="AN15" s="150">
+      <c r="AL15" s="179"/>
+      <c r="AM15" s="179"/>
+      <c r="AN15" s="192">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="AO15" s="150"/>
-      <c r="AP15" s="150"/>
+      <c r="AO15" s="192"/>
+      <c r="AP15" s="192"/>
       <c r="AQ15" s="22">
         <f t="shared" si="8"/>
         <v>0.33333333333333331</v>
@@ -3369,52 +3369,52 @@
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="55"/>
-      <c r="G16" s="160" t="s">
+      <c r="G16" s="193" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="160"/>
-      <c r="I16" s="160"/>
-      <c r="J16" s="164"/>
-      <c r="K16" s="164"/>
-      <c r="L16" s="164"/>
-      <c r="M16" s="164"/>
-      <c r="N16" s="164"/>
-      <c r="O16" s="164"/>
-      <c r="P16" s="164"/>
-      <c r="Q16" s="164"/>
-      <c r="R16" s="164"/>
-      <c r="S16" s="164"/>
-      <c r="T16" s="164"/>
-      <c r="U16" s="164"/>
-      <c r="V16" s="150">
+      <c r="H16" s="193"/>
+      <c r="I16" s="193"/>
+      <c r="J16" s="179"/>
+      <c r="K16" s="179"/>
+      <c r="L16" s="179"/>
+      <c r="M16" s="179"/>
+      <c r="N16" s="179"/>
+      <c r="O16" s="179"/>
+      <c r="P16" s="179"/>
+      <c r="Q16" s="179"/>
+      <c r="R16" s="179"/>
+      <c r="S16" s="179"/>
+      <c r="T16" s="179"/>
+      <c r="U16" s="179"/>
+      <c r="V16" s="192">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="W16" s="150"/>
-      <c r="X16" s="150"/>
-      <c r="Y16" s="160" t="s">
+      <c r="W16" s="192"/>
+      <c r="X16" s="192"/>
+      <c r="Y16" s="193" t="s">
         <v>10</v>
       </c>
-      <c r="Z16" s="160"/>
-      <c r="AA16" s="160"/>
-      <c r="AB16" s="164"/>
-      <c r="AC16" s="164"/>
-      <c r="AD16" s="164"/>
-      <c r="AE16" s="164"/>
-      <c r="AF16" s="164"/>
-      <c r="AG16" s="164"/>
-      <c r="AH16" s="164"/>
-      <c r="AI16" s="164"/>
-      <c r="AJ16" s="164"/>
-      <c r="AK16" s="164"/>
-      <c r="AL16" s="164"/>
-      <c r="AM16" s="164"/>
-      <c r="AN16" s="150">
+      <c r="Z16" s="193"/>
+      <c r="AA16" s="193"/>
+      <c r="AB16" s="179"/>
+      <c r="AC16" s="179"/>
+      <c r="AD16" s="179"/>
+      <c r="AE16" s="179"/>
+      <c r="AF16" s="179"/>
+      <c r="AG16" s="179"/>
+      <c r="AH16" s="179"/>
+      <c r="AI16" s="179"/>
+      <c r="AJ16" s="179"/>
+      <c r="AK16" s="179"/>
+      <c r="AL16" s="179"/>
+      <c r="AM16" s="179"/>
+      <c r="AN16" s="192">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AO16" s="150"/>
-      <c r="AP16" s="150"/>
+      <c r="AO16" s="192"/>
+      <c r="AP16" s="192"/>
       <c r="AQ16" s="22">
         <f t="shared" si="8"/>
         <v>0</v>
@@ -3568,50 +3568,50 @@
       <c r="D19" s="46"/>
       <c r="E19" s="46"/>
       <c r="F19" s="46"/>
-      <c r="G19" s="220"/>
-      <c r="H19" s="220"/>
-      <c r="I19" s="220"/>
-      <c r="J19" s="220"/>
-      <c r="K19" s="220"/>
-      <c r="L19" s="220"/>
-      <c r="M19" s="220"/>
-      <c r="N19" s="220"/>
-      <c r="O19" s="220"/>
-      <c r="P19" s="220"/>
-      <c r="Q19" s="220"/>
+      <c r="G19" s="158"/>
+      <c r="H19" s="158"/>
+      <c r="I19" s="158"/>
+      <c r="J19" s="158"/>
+      <c r="K19" s="158"/>
+      <c r="L19" s="158"/>
+      <c r="M19" s="158"/>
+      <c r="N19" s="158"/>
+      <c r="O19" s="158"/>
+      <c r="P19" s="158"/>
+      <c r="Q19" s="158"/>
       <c r="R19" s="62"/>
-      <c r="S19" s="225" t="s">
+      <c r="S19" s="163" t="s">
         <v>62</v>
       </c>
-      <c r="T19" s="225"/>
-      <c r="U19" s="225"/>
-      <c r="V19" s="225"/>
-      <c r="W19" s="225"/>
-      <c r="Y19" s="225">
-        <v>41887</v>
-      </c>
-      <c r="Z19" s="226"/>
-      <c r="AA19" s="226"/>
-      <c r="AB19" s="226"/>
-      <c r="AD19" s="229" t="s">
+      <c r="T19" s="163"/>
+      <c r="U19" s="163"/>
+      <c r="V19" s="163"/>
+      <c r="W19" s="163"/>
+      <c r="Y19" s="163">
+        <v>41901</v>
+      </c>
+      <c r="Z19" s="164"/>
+      <c r="AA19" s="164"/>
+      <c r="AB19" s="164"/>
+      <c r="AD19" s="168" t="s">
         <v>33</v>
       </c>
-      <c r="AE19" s="230"/>
-      <c r="AF19" s="230"/>
-      <c r="AG19" s="230"/>
-      <c r="AH19" s="231"/>
-      <c r="AI19" s="165" t="s">
+      <c r="AE19" s="169"/>
+      <c r="AF19" s="169"/>
+      <c r="AG19" s="169"/>
+      <c r="AH19" s="170"/>
+      <c r="AI19" s="156" t="s">
         <v>21</v>
       </c>
-      <c r="AJ19" s="166"/>
-      <c r="AK19" s="166"/>
-      <c r="AL19" s="166"/>
-      <c r="AM19" s="166"/>
-      <c r="AO19" s="167">
+      <c r="AJ19" s="157"/>
+      <c r="AK19" s="157"/>
+      <c r="AL19" s="157"/>
+      <c r="AM19" s="157"/>
+      <c r="AO19" s="177">
         <f>+AQ19+AW19</f>
         <v>3.333333333333333</v>
       </c>
-      <c r="AP19" s="168"/>
+      <c r="AP19" s="178"/>
       <c r="AQ19" s="26">
         <f>MIN(SUM(AQ10:AQ16),40/24)</f>
         <v>1.6666666666666665</v>
@@ -3637,33 +3637,33 @@
       <c r="D20" s="47"/>
       <c r="E20" s="47"/>
       <c r="F20" s="47"/>
-      <c r="G20" s="221"/>
-      <c r="H20" s="221"/>
-      <c r="I20" s="221"/>
-      <c r="J20" s="221"/>
-      <c r="K20" s="221"/>
-      <c r="L20" s="221"/>
-      <c r="M20" s="221"/>
-      <c r="N20" s="221"/>
-      <c r="O20" s="221"/>
-      <c r="P20" s="221"/>
-      <c r="Q20" s="221"/>
+      <c r="G20" s="159"/>
+      <c r="H20" s="159"/>
+      <c r="I20" s="159"/>
+      <c r="J20" s="159"/>
+      <c r="K20" s="159"/>
+      <c r="L20" s="159"/>
+      <c r="M20" s="159"/>
+      <c r="N20" s="159"/>
+      <c r="O20" s="159"/>
+      <c r="P20" s="159"/>
+      <c r="Q20" s="159"/>
       <c r="R20" s="63"/>
-      <c r="S20" s="224"/>
-      <c r="T20" s="224"/>
-      <c r="U20" s="224"/>
-      <c r="V20" s="224"/>
-      <c r="W20" s="224"/>
-      <c r="Y20" s="197"/>
-      <c r="Z20" s="197"/>
-      <c r="AA20" s="197"/>
-      <c r="AB20" s="197"/>
+      <c r="S20" s="162"/>
+      <c r="T20" s="162"/>
+      <c r="U20" s="162"/>
+      <c r="V20" s="162"/>
+      <c r="W20" s="162"/>
+      <c r="Y20" s="165"/>
+      <c r="Z20" s="165"/>
+      <c r="AA20" s="165"/>
+      <c r="AB20" s="165"/>
       <c r="AC20" s="48"/>
-      <c r="AD20" s="232"/>
-      <c r="AE20" s="233"/>
-      <c r="AF20" s="233"/>
-      <c r="AG20" s="233"/>
-      <c r="AH20" s="234"/>
+      <c r="AD20" s="171"/>
+      <c r="AE20" s="172"/>
+      <c r="AF20" s="172"/>
+      <c r="AG20" s="172"/>
+      <c r="AH20" s="173"/>
       <c r="AM20" s="66"/>
       <c r="AO20" s="65"/>
       <c r="AP20" s="65"/>
@@ -3700,35 +3700,35 @@
       <c r="P21" s="35"/>
       <c r="Q21" s="50"/>
       <c r="R21" s="35"/>
-      <c r="S21" s="227" t="s">
+      <c r="S21" s="166" t="s">
         <v>28</v>
       </c>
-      <c r="T21" s="227"/>
-      <c r="U21" s="227"/>
-      <c r="V21" s="227"/>
-      <c r="W21" s="227"/>
-      <c r="Y21" s="206" t="s">
+      <c r="T21" s="166"/>
+      <c r="U21" s="166"/>
+      <c r="V21" s="166"/>
+      <c r="W21" s="166"/>
+      <c r="Y21" s="191" t="s">
         <v>26</v>
       </c>
-      <c r="Z21" s="206"/>
-      <c r="AA21" s="206"/>
-      <c r="AD21" s="232"/>
-      <c r="AE21" s="233"/>
-      <c r="AF21" s="233"/>
-      <c r="AG21" s="233"/>
-      <c r="AH21" s="234"/>
-      <c r="AI21" s="165" t="s">
+      <c r="Z21" s="191"/>
+      <c r="AA21" s="191"/>
+      <c r="AD21" s="171"/>
+      <c r="AE21" s="172"/>
+      <c r="AF21" s="172"/>
+      <c r="AG21" s="172"/>
+      <c r="AH21" s="173"/>
+      <c r="AI21" s="156" t="s">
         <v>24</v>
       </c>
-      <c r="AJ21" s="166"/>
-      <c r="AK21" s="166"/>
-      <c r="AL21" s="166"/>
-      <c r="AM21" s="166"/>
-      <c r="AO21" s="167">
+      <c r="AJ21" s="157"/>
+      <c r="AK21" s="157"/>
+      <c r="AL21" s="157"/>
+      <c r="AM21" s="157"/>
+      <c r="AO21" s="177">
         <f>+AR21+AX21</f>
         <v>0</v>
       </c>
-      <c r="AP21" s="168"/>
+      <c r="AP21" s="178"/>
       <c r="AQ21" s="19"/>
       <c r="AR21" s="20">
         <f>SUM(AR10:AR16)+MAX(0,SUM(AQ10:AQ16)-40/24)</f>
@@ -3774,11 +3774,11 @@
       <c r="Y22" s="51"/>
       <c r="Z22" s="51"/>
       <c r="AA22" s="51"/>
-      <c r="AD22" s="232"/>
-      <c r="AE22" s="233"/>
-      <c r="AF22" s="233"/>
-      <c r="AG22" s="233"/>
-      <c r="AH22" s="234"/>
+      <c r="AD22" s="171"/>
+      <c r="AE22" s="172"/>
+      <c r="AF22" s="172"/>
+      <c r="AG22" s="172"/>
+      <c r="AH22" s="173"/>
       <c r="AL22" s="28"/>
       <c r="AM22" s="66"/>
       <c r="AN22" s="23"/>
@@ -3797,32 +3797,32 @@
       <c r="BA22" s="6"/>
     </row>
     <row r="23" spans="1:59" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G23" s="222" t="s">
+      <c r="G23" s="160" t="s">
         <v>31</v>
       </c>
-      <c r="H23" s="222"/>
-      <c r="I23" s="222"/>
-      <c r="J23" s="222"/>
-      <c r="K23" s="222"/>
-      <c r="L23" s="222"/>
-      <c r="M23" s="222"/>
-      <c r="N23" s="222"/>
-      <c r="O23" s="222"/>
-      <c r="P23" s="222"/>
-      <c r="Q23" s="222"/>
-      <c r="R23" s="222"/>
-      <c r="S23" s="222"/>
-      <c r="T23" s="222"/>
-      <c r="U23" s="222"/>
-      <c r="V23" s="222"/>
-      <c r="W23" s="222"/>
-      <c r="X23" s="222"/>
+      <c r="H23" s="160"/>
+      <c r="I23" s="160"/>
+      <c r="J23" s="160"/>
+      <c r="K23" s="160"/>
+      <c r="L23" s="160"/>
+      <c r="M23" s="160"/>
+      <c r="N23" s="160"/>
+      <c r="O23" s="160"/>
+      <c r="P23" s="160"/>
+      <c r="Q23" s="160"/>
+      <c r="R23" s="160"/>
+      <c r="S23" s="160"/>
+      <c r="T23" s="160"/>
+      <c r="U23" s="160"/>
+      <c r="V23" s="160"/>
+      <c r="W23" s="160"/>
+      <c r="X23" s="160"/>
       <c r="AC23" s="48"/>
-      <c r="AD23" s="232"/>
-      <c r="AE23" s="233"/>
-      <c r="AF23" s="233"/>
-      <c r="AG23" s="233"/>
-      <c r="AH23" s="234"/>
+      <c r="AD23" s="171"/>
+      <c r="AE23" s="172"/>
+      <c r="AF23" s="172"/>
+      <c r="AG23" s="172"/>
+      <c r="AH23" s="173"/>
       <c r="AM23" s="66"/>
       <c r="AO23" s="65"/>
       <c r="AP23" s="65"/>
@@ -3839,41 +3839,41 @@
       <c r="BA23" s="6"/>
     </row>
     <row r="24" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G24" s="222"/>
-      <c r="H24" s="222"/>
-      <c r="I24" s="222"/>
-      <c r="J24" s="222"/>
-      <c r="K24" s="222"/>
-      <c r="L24" s="222"/>
-      <c r="M24" s="222"/>
-      <c r="N24" s="222"/>
-      <c r="O24" s="222"/>
-      <c r="P24" s="222"/>
-      <c r="Q24" s="222"/>
-      <c r="R24" s="222"/>
-      <c r="S24" s="222"/>
-      <c r="T24" s="222"/>
-      <c r="U24" s="222"/>
-      <c r="V24" s="222"/>
-      <c r="W24" s="222"/>
-      <c r="X24" s="222"/>
-      <c r="AD24" s="232"/>
-      <c r="AE24" s="233"/>
-      <c r="AF24" s="233"/>
-      <c r="AG24" s="233"/>
-      <c r="AH24" s="234"/>
-      <c r="AI24" s="165" t="s">
+      <c r="G24" s="160"/>
+      <c r="H24" s="160"/>
+      <c r="I24" s="160"/>
+      <c r="J24" s="160"/>
+      <c r="K24" s="160"/>
+      <c r="L24" s="160"/>
+      <c r="M24" s="160"/>
+      <c r="N24" s="160"/>
+      <c r="O24" s="160"/>
+      <c r="P24" s="160"/>
+      <c r="Q24" s="160"/>
+      <c r="R24" s="160"/>
+      <c r="S24" s="160"/>
+      <c r="T24" s="160"/>
+      <c r="U24" s="160"/>
+      <c r="V24" s="160"/>
+      <c r="W24" s="160"/>
+      <c r="X24" s="160"/>
+      <c r="AD24" s="171"/>
+      <c r="AE24" s="172"/>
+      <c r="AF24" s="172"/>
+      <c r="AG24" s="172"/>
+      <c r="AH24" s="173"/>
+      <c r="AI24" s="156" t="s">
         <v>23</v>
       </c>
-      <c r="AJ24" s="166"/>
-      <c r="AK24" s="166"/>
-      <c r="AL24" s="166"/>
-      <c r="AM24" s="166"/>
-      <c r="AO24" s="167">
+      <c r="AJ24" s="157"/>
+      <c r="AK24" s="157"/>
+      <c r="AL24" s="157"/>
+      <c r="AM24" s="157"/>
+      <c r="AO24" s="177">
         <f>+AS24+AY24</f>
         <v>0</v>
       </c>
-      <c r="AP24" s="168"/>
+      <c r="AP24" s="178"/>
       <c r="AQ24" s="19"/>
       <c r="AR24" s="19"/>
       <c r="AS24" s="20">
@@ -3893,30 +3893,30 @@
       <c r="BA24" s="6"/>
     </row>
     <row r="25" spans="1:59" ht="6.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G25" s="222"/>
-      <c r="H25" s="222"/>
-      <c r="I25" s="222"/>
-      <c r="J25" s="222"/>
-      <c r="K25" s="222"/>
-      <c r="L25" s="222"/>
-      <c r="M25" s="222"/>
-      <c r="N25" s="222"/>
-      <c r="O25" s="222"/>
-      <c r="P25" s="222"/>
-      <c r="Q25" s="222"/>
-      <c r="R25" s="222"/>
-      <c r="S25" s="222"/>
-      <c r="T25" s="222"/>
-      <c r="U25" s="222"/>
-      <c r="V25" s="222"/>
-      <c r="W25" s="222"/>
-      <c r="X25" s="222"/>
+      <c r="G25" s="160"/>
+      <c r="H25" s="160"/>
+      <c r="I25" s="160"/>
+      <c r="J25" s="160"/>
+      <c r="K25" s="160"/>
+      <c r="L25" s="160"/>
+      <c r="M25" s="160"/>
+      <c r="N25" s="160"/>
+      <c r="O25" s="160"/>
+      <c r="P25" s="160"/>
+      <c r="Q25" s="160"/>
+      <c r="R25" s="160"/>
+      <c r="S25" s="160"/>
+      <c r="T25" s="160"/>
+      <c r="U25" s="160"/>
+      <c r="V25" s="160"/>
+      <c r="W25" s="160"/>
+      <c r="X25" s="160"/>
       <c r="AC25" s="48"/>
-      <c r="AD25" s="232"/>
-      <c r="AE25" s="233"/>
-      <c r="AF25" s="233"/>
-      <c r="AG25" s="233"/>
-      <c r="AH25" s="234"/>
+      <c r="AD25" s="171"/>
+      <c r="AE25" s="172"/>
+      <c r="AF25" s="172"/>
+      <c r="AG25" s="172"/>
+      <c r="AH25" s="173"/>
       <c r="AM25" s="66"/>
       <c r="AO25" s="65"/>
       <c r="AP25" s="65"/>
@@ -3939,45 +3939,45 @@
       <c r="D26" s="47"/>
       <c r="E26" s="47"/>
       <c r="F26" s="47"/>
-      <c r="G26" s="220"/>
-      <c r="H26" s="220"/>
-      <c r="I26" s="220"/>
-      <c r="J26" s="220"/>
-      <c r="K26" s="220"/>
-      <c r="L26" s="220"/>
-      <c r="M26" s="220"/>
-      <c r="N26" s="220"/>
-      <c r="O26" s="220"/>
-      <c r="P26" s="220"/>
-      <c r="Q26" s="220"/>
+      <c r="G26" s="158"/>
+      <c r="H26" s="158"/>
+      <c r="I26" s="158"/>
+      <c r="J26" s="158"/>
+      <c r="K26" s="158"/>
+      <c r="L26" s="158"/>
+      <c r="M26" s="158"/>
+      <c r="N26" s="158"/>
+      <c r="O26" s="158"/>
+      <c r="P26" s="158"/>
+      <c r="Q26" s="158"/>
       <c r="R26" s="64"/>
-      <c r="S26" s="223"/>
-      <c r="T26" s="223"/>
-      <c r="U26" s="223"/>
-      <c r="V26" s="223"/>
-      <c r="W26" s="223"/>
+      <c r="S26" s="161"/>
+      <c r="T26" s="161"/>
+      <c r="U26" s="161"/>
+      <c r="V26" s="161"/>
+      <c r="W26" s="161"/>
       <c r="X26" s="35"/>
-      <c r="Y26" s="196"/>
-      <c r="Z26" s="196"/>
-      <c r="AA26" s="196"/>
-      <c r="AB26" s="196"/>
-      <c r="AD26" s="232"/>
-      <c r="AE26" s="233"/>
-      <c r="AF26" s="233"/>
-      <c r="AG26" s="233"/>
-      <c r="AH26" s="234"/>
-      <c r="AI26" s="165" t="s">
+      <c r="Y26" s="180"/>
+      <c r="Z26" s="180"/>
+      <c r="AA26" s="180"/>
+      <c r="AB26" s="180"/>
+      <c r="AD26" s="171"/>
+      <c r="AE26" s="172"/>
+      <c r="AF26" s="172"/>
+      <c r="AG26" s="172"/>
+      <c r="AH26" s="173"/>
+      <c r="AI26" s="156" t="s">
         <v>22</v>
       </c>
-      <c r="AJ26" s="166"/>
-      <c r="AK26" s="166"/>
-      <c r="AL26" s="166"/>
-      <c r="AM26" s="166"/>
-      <c r="AO26" s="169">
+      <c r="AJ26" s="157"/>
+      <c r="AK26" s="157"/>
+      <c r="AL26" s="157"/>
+      <c r="AM26" s="157"/>
+      <c r="AO26" s="221">
         <f>AT26+AZ26</f>
         <v>3.333333333333333</v>
       </c>
-      <c r="AP26" s="170"/>
+      <c r="AP26" s="222"/>
       <c r="AQ26" s="19"/>
       <c r="AR26" s="19"/>
       <c r="AS26" s="19"/>
@@ -4003,33 +4003,33 @@
       <c r="D27" s="47"/>
       <c r="E27" s="47"/>
       <c r="F27" s="47"/>
-      <c r="G27" s="220"/>
-      <c r="H27" s="220"/>
-      <c r="I27" s="220"/>
-      <c r="J27" s="220"/>
-      <c r="K27" s="220"/>
-      <c r="L27" s="220"/>
-      <c r="M27" s="220"/>
-      <c r="N27" s="220"/>
-      <c r="O27" s="220"/>
-      <c r="P27" s="220"/>
-      <c r="Q27" s="220"/>
+      <c r="G27" s="158"/>
+      <c r="H27" s="158"/>
+      <c r="I27" s="158"/>
+      <c r="J27" s="158"/>
+      <c r="K27" s="158"/>
+      <c r="L27" s="158"/>
+      <c r="M27" s="158"/>
+      <c r="N27" s="158"/>
+      <c r="O27" s="158"/>
+      <c r="P27" s="158"/>
+      <c r="Q27" s="158"/>
       <c r="R27" s="64"/>
-      <c r="S27" s="223"/>
-      <c r="T27" s="223"/>
-      <c r="U27" s="223"/>
-      <c r="V27" s="223"/>
-      <c r="W27" s="223"/>
+      <c r="S27" s="161"/>
+      <c r="T27" s="161"/>
+      <c r="U27" s="161"/>
+      <c r="V27" s="161"/>
+      <c r="W27" s="161"/>
       <c r="X27" s="35"/>
-      <c r="Y27" s="196"/>
-      <c r="Z27" s="196"/>
-      <c r="AA27" s="196"/>
-      <c r="AB27" s="196"/>
-      <c r="AD27" s="232"/>
-      <c r="AE27" s="233"/>
-      <c r="AF27" s="233"/>
-      <c r="AG27" s="233"/>
-      <c r="AH27" s="234"/>
+      <c r="Y27" s="180"/>
+      <c r="Z27" s="180"/>
+      <c r="AA27" s="180"/>
+      <c r="AB27" s="180"/>
+      <c r="AD27" s="171"/>
+      <c r="AE27" s="172"/>
+      <c r="AF27" s="172"/>
+      <c r="AG27" s="172"/>
+      <c r="AH27" s="173"/>
       <c r="AM27" s="74"/>
       <c r="AO27" s="76"/>
       <c r="AP27" s="76"/>
@@ -4046,43 +4046,43 @@
       <c r="BA27" s="6"/>
     </row>
     <row r="28" spans="1:59" ht="18.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="G28" s="221"/>
-      <c r="H28" s="221"/>
-      <c r="I28" s="221"/>
-      <c r="J28" s="221"/>
-      <c r="K28" s="221"/>
-      <c r="L28" s="221"/>
-      <c r="M28" s="221"/>
-      <c r="N28" s="221"/>
-      <c r="O28" s="221"/>
-      <c r="P28" s="221"/>
-      <c r="Q28" s="221"/>
+      <c r="G28" s="159"/>
+      <c r="H28" s="159"/>
+      <c r="I28" s="159"/>
+      <c r="J28" s="159"/>
+      <c r="K28" s="159"/>
+      <c r="L28" s="159"/>
+      <c r="M28" s="159"/>
+      <c r="N28" s="159"/>
+      <c r="O28" s="159"/>
+      <c r="P28" s="159"/>
+      <c r="Q28" s="159"/>
       <c r="R28" s="35"/>
-      <c r="S28" s="224"/>
-      <c r="T28" s="224"/>
-      <c r="U28" s="224"/>
-      <c r="V28" s="224"/>
-      <c r="W28" s="224"/>
+      <c r="S28" s="162"/>
+      <c r="T28" s="162"/>
+      <c r="U28" s="162"/>
+      <c r="V28" s="162"/>
+      <c r="W28" s="162"/>
       <c r="X28" s="35"/>
-      <c r="Y28" s="197"/>
-      <c r="Z28" s="197"/>
-      <c r="AA28" s="197"/>
-      <c r="AB28" s="197"/>
+      <c r="Y28" s="165"/>
+      <c r="Z28" s="165"/>
+      <c r="AA28" s="165"/>
+      <c r="AB28" s="165"/>
       <c r="AC28" s="52"/>
-      <c r="AD28" s="232"/>
-      <c r="AE28" s="233"/>
-      <c r="AF28" s="233"/>
-      <c r="AG28" s="233"/>
-      <c r="AH28" s="234"/>
-      <c r="AI28" s="165" t="s">
+      <c r="AD28" s="171"/>
+      <c r="AE28" s="172"/>
+      <c r="AF28" s="172"/>
+      <c r="AG28" s="172"/>
+      <c r="AH28" s="173"/>
+      <c r="AI28" s="156" t="s">
         <v>47</v>
       </c>
-      <c r="AJ28" s="166"/>
-      <c r="AK28" s="166"/>
-      <c r="AL28" s="166"/>
-      <c r="AM28" s="166"/>
-      <c r="AO28" s="171"/>
-      <c r="AP28" s="172"/>
+      <c r="AJ28" s="157"/>
+      <c r="AK28" s="157"/>
+      <c r="AL28" s="157"/>
+      <c r="AM28" s="157"/>
+      <c r="AO28" s="223"/>
+      <c r="AP28" s="224"/>
       <c r="AQ28" s="19"/>
       <c r="AR28" s="19"/>
       <c r="AS28" s="19"/>
@@ -4110,25 +4110,25 @@
       <c r="O29" s="35"/>
       <c r="P29" s="35"/>
       <c r="R29" s="35"/>
-      <c r="S29" s="228" t="s">
+      <c r="S29" s="167" t="s">
         <v>29</v>
       </c>
-      <c r="T29" s="228"/>
-      <c r="U29" s="228"/>
-      <c r="V29" s="228"/>
-      <c r="W29" s="228"/>
+      <c r="T29" s="167"/>
+      <c r="U29" s="167"/>
+      <c r="V29" s="167"/>
+      <c r="W29" s="167"/>
       <c r="X29" s="35"/>
-      <c r="Y29" s="159" t="s">
+      <c r="Y29" s="220" t="s">
         <v>26</v>
       </c>
-      <c r="Z29" s="159"/>
-      <c r="AA29" s="159"/>
+      <c r="Z29" s="220"/>
+      <c r="AA29" s="220"/>
       <c r="AC29" s="52"/>
-      <c r="AD29" s="235"/>
-      <c r="AE29" s="236"/>
-      <c r="AF29" s="236"/>
-      <c r="AG29" s="236"/>
-      <c r="AH29" s="237"/>
+      <c r="AD29" s="174"/>
+      <c r="AE29" s="175"/>
+      <c r="AF29" s="175"/>
+      <c r="AG29" s="175"/>
+      <c r="AH29" s="176"/>
       <c r="AO29" s="27"/>
       <c r="AP29" s="27"/>
       <c r="AQ29" s="19"/>
@@ -4199,88 +4199,88 @@
       <c r="BA31" s="102"/>
       <c r="BB31" s="102"/>
       <c r="BC31" s="92"/>
-      <c r="BD31" s="200" t="s">
+      <c r="BD31" s="183" t="s">
         <v>45</v>
       </c>
-      <c r="BE31" s="201"/>
-      <c r="BF31" s="210" t="s">
+      <c r="BE31" s="184"/>
+      <c r="BF31" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="BG31" s="211"/>
+      <c r="BG31" s="144"/>
     </row>
     <row r="32" spans="1:59" s="2" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="207" t="s">
+      <c r="B32" s="147" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="208"/>
-      <c r="D32" s="208"/>
-      <c r="E32" s="208"/>
-      <c r="F32" s="208"/>
-      <c r="G32" s="208"/>
-      <c r="H32" s="208"/>
-      <c r="I32" s="208"/>
-      <c r="J32" s="208"/>
-      <c r="K32" s="208"/>
-      <c r="L32" s="208"/>
-      <c r="M32" s="208"/>
-      <c r="N32" s="209"/>
-      <c r="O32" s="207" t="s">
+      <c r="C32" s="149"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="149"/>
+      <c r="F32" s="149"/>
+      <c r="G32" s="149"/>
+      <c r="H32" s="149"/>
+      <c r="I32" s="149"/>
+      <c r="J32" s="149"/>
+      <c r="K32" s="149"/>
+      <c r="L32" s="149"/>
+      <c r="M32" s="149"/>
+      <c r="N32" s="148"/>
+      <c r="O32" s="147" t="s">
         <v>49</v>
       </c>
-      <c r="P32" s="209"/>
-      <c r="Q32" s="207" t="s">
+      <c r="P32" s="148"/>
+      <c r="Q32" s="147" t="s">
         <v>50</v>
       </c>
-      <c r="R32" s="209"/>
-      <c r="S32" s="207" t="s">
+      <c r="R32" s="148"/>
+      <c r="S32" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="T32" s="208"/>
-      <c r="U32" s="208"/>
-      <c r="V32" s="209"/>
-      <c r="W32" s="207" t="s">
+      <c r="T32" s="149"/>
+      <c r="U32" s="149"/>
+      <c r="V32" s="148"/>
+      <c r="W32" s="147" t="s">
         <v>53</v>
       </c>
-      <c r="X32" s="208"/>
-      <c r="Y32" s="208"/>
-      <c r="Z32" s="208"/>
-      <c r="AA32" s="208"/>
-      <c r="AB32" s="208"/>
-      <c r="AC32" s="208"/>
-      <c r="AD32" s="209"/>
-      <c r="AE32" s="214" t="s">
+      <c r="X32" s="149"/>
+      <c r="Y32" s="149"/>
+      <c r="Z32" s="149"/>
+      <c r="AA32" s="149"/>
+      <c r="AB32" s="149"/>
+      <c r="AC32" s="149"/>
+      <c r="AD32" s="148"/>
+      <c r="AE32" s="150" t="s">
         <v>52</v>
       </c>
-      <c r="AF32" s="215"/>
-      <c r="AG32" s="215"/>
-      <c r="AH32" s="215"/>
-      <c r="AI32" s="215"/>
-      <c r="AJ32" s="215"/>
-      <c r="AK32" s="215"/>
-      <c r="AL32" s="215"/>
-      <c r="AM32" s="215"/>
-      <c r="AN32" s="216"/>
-      <c r="AO32" s="217" t="s">
+      <c r="AF32" s="151"/>
+      <c r="AG32" s="151"/>
+      <c r="AH32" s="151"/>
+      <c r="AI32" s="151"/>
+      <c r="AJ32" s="151"/>
+      <c r="AK32" s="151"/>
+      <c r="AL32" s="151"/>
+      <c r="AM32" s="151"/>
+      <c r="AN32" s="152"/>
+      <c r="AO32" s="153" t="s">
         <v>54</v>
       </c>
-      <c r="AP32" s="218"/>
-      <c r="AQ32" s="218"/>
-      <c r="AR32" s="218"/>
-      <c r="AS32" s="218"/>
-      <c r="AT32" s="218"/>
-      <c r="AU32" s="218"/>
-      <c r="AV32" s="218"/>
-      <c r="AW32" s="218"/>
-      <c r="AX32" s="218"/>
-      <c r="AY32" s="218"/>
-      <c r="AZ32" s="218"/>
-      <c r="BA32" s="218"/>
-      <c r="BB32" s="218"/>
-      <c r="BC32" s="219"/>
-      <c r="BD32" s="202"/>
-      <c r="BE32" s="203"/>
-      <c r="BF32" s="212"/>
-      <c r="BG32" s="213"/>
+      <c r="AP32" s="154"/>
+      <c r="AQ32" s="154"/>
+      <c r="AR32" s="154"/>
+      <c r="AS32" s="154"/>
+      <c r="AT32" s="154"/>
+      <c r="AU32" s="154"/>
+      <c r="AV32" s="154"/>
+      <c r="AW32" s="154"/>
+      <c r="AX32" s="154"/>
+      <c r="AY32" s="154"/>
+      <c r="AZ32" s="154"/>
+      <c r="BA32" s="154"/>
+      <c r="BB32" s="154"/>
+      <c r="BC32" s="155"/>
+      <c r="BD32" s="185"/>
+      <c r="BE32" s="186"/>
+      <c r="BF32" s="145"/>
+      <c r="BG32" s="146"/>
     </row>
     <row r="33" spans="2:59" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="104"/>
@@ -4333,12 +4333,12 @@
       <c r="AW33" s="120"/>
       <c r="AX33" s="120"/>
       <c r="AY33" s="120"/>
-      <c r="AZ33" s="146"/>
-      <c r="BA33" s="147"/>
+      <c r="AZ33" s="236"/>
+      <c r="BA33" s="237"/>
       <c r="BB33" s="120"/>
       <c r="BC33" s="121"/>
-      <c r="BD33" s="204"/>
-      <c r="BE33" s="205"/>
+      <c r="BD33" s="189"/>
+      <c r="BE33" s="190"/>
       <c r="BF33" s="122"/>
       <c r="BG33" s="123"/>
     </row>
@@ -4393,12 +4393,12 @@
       <c r="AW34" s="126"/>
       <c r="AX34" s="126"/>
       <c r="AY34" s="126"/>
-      <c r="AZ34" s="148"/>
-      <c r="BA34" s="149"/>
+      <c r="AZ34" s="187"/>
+      <c r="BA34" s="188"/>
       <c r="BB34" s="126"/>
       <c r="BC34" s="127"/>
-      <c r="BD34" s="151"/>
-      <c r="BE34" s="152"/>
+      <c r="BD34" s="225"/>
+      <c r="BE34" s="226"/>
       <c r="BF34" s="128"/>
       <c r="BG34" s="129"/>
     </row>
@@ -4453,12 +4453,12 @@
       <c r="AW35" s="126"/>
       <c r="AX35" s="126"/>
       <c r="AY35" s="126"/>
-      <c r="AZ35" s="148"/>
-      <c r="BA35" s="149"/>
+      <c r="AZ35" s="187"/>
+      <c r="BA35" s="188"/>
       <c r="BB35" s="126"/>
       <c r="BC35" s="127"/>
-      <c r="BD35" s="151"/>
-      <c r="BE35" s="152"/>
+      <c r="BD35" s="225"/>
+      <c r="BE35" s="226"/>
       <c r="BF35" s="128"/>
       <c r="BG35" s="129"/>
     </row>
@@ -4513,12 +4513,12 @@
       <c r="AW36" s="126"/>
       <c r="AX36" s="126"/>
       <c r="AY36" s="126"/>
-      <c r="AZ36" s="148"/>
-      <c r="BA36" s="149"/>
+      <c r="AZ36" s="187"/>
+      <c r="BA36" s="188"/>
       <c r="BB36" s="126"/>
       <c r="BC36" s="127"/>
-      <c r="BD36" s="151"/>
-      <c r="BE36" s="152"/>
+      <c r="BD36" s="225"/>
+      <c r="BE36" s="226"/>
       <c r="BF36" s="128"/>
       <c r="BG36" s="129"/>
     </row>
@@ -4573,12 +4573,12 @@
       <c r="AW37" s="126"/>
       <c r="AX37" s="126"/>
       <c r="AY37" s="126"/>
-      <c r="AZ37" s="148"/>
-      <c r="BA37" s="149"/>
+      <c r="AZ37" s="187"/>
+      <c r="BA37" s="188"/>
       <c r="BB37" s="126"/>
       <c r="BC37" s="127"/>
-      <c r="BD37" s="153"/>
-      <c r="BE37" s="154"/>
+      <c r="BD37" s="227"/>
+      <c r="BE37" s="228"/>
       <c r="BF37" s="130"/>
       <c r="BG37" s="131"/>
     </row>
@@ -4633,12 +4633,12 @@
       <c r="AW38" s="126"/>
       <c r="AX38" s="126"/>
       <c r="AY38" s="126"/>
-      <c r="AZ38" s="148"/>
-      <c r="BA38" s="149"/>
+      <c r="AZ38" s="187"/>
+      <c r="BA38" s="188"/>
       <c r="BB38" s="126"/>
       <c r="BC38" s="127"/>
-      <c r="BD38" s="151"/>
-      <c r="BE38" s="152"/>
+      <c r="BD38" s="225"/>
+      <c r="BE38" s="226"/>
       <c r="BF38" s="128"/>
       <c r="BG38" s="129"/>
     </row>
@@ -4693,57 +4693,57 @@
       <c r="AW39" s="139"/>
       <c r="AX39" s="139"/>
       <c r="AY39" s="139"/>
-      <c r="AZ39" s="155"/>
-      <c r="BA39" s="156"/>
+      <c r="AZ39" s="229"/>
+      <c r="BA39" s="230"/>
       <c r="BB39" s="139"/>
       <c r="BC39" s="140"/>
-      <c r="BD39" s="198"/>
-      <c r="BE39" s="199"/>
+      <c r="BD39" s="181"/>
+      <c r="BE39" s="182"/>
       <c r="BF39" s="141"/>
       <c r="BG39" s="142"/>
     </row>
     <row r="40" spans="2:59" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="143" t="s">
+      <c r="B40" s="233" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="143"/>
-      <c r="D40" s="143"/>
-      <c r="E40" s="143"/>
-      <c r="F40" s="143"/>
-      <c r="G40" s="143"/>
-      <c r="H40" s="143"/>
-      <c r="I40" s="143"/>
+      <c r="C40" s="233"/>
+      <c r="D40" s="233"/>
+      <c r="E40" s="233"/>
+      <c r="F40" s="233"/>
+      <c r="G40" s="233"/>
+      <c r="H40" s="233"/>
+      <c r="I40" s="233"/>
       <c r="AC40" s="66"/>
       <c r="AD40" s="66"/>
       <c r="AE40" s="66"/>
       <c r="AF40" s="66"/>
       <c r="AG40" s="81"/>
-      <c r="AH40" s="145" t="s">
+      <c r="AH40" s="235" t="s">
         <v>37</v>
       </c>
-      <c r="AI40" s="145"/>
-      <c r="AJ40" s="145"/>
-      <c r="AK40" s="145"/>
-      <c r="AL40" s="145"/>
+      <c r="AI40" s="235"/>
+      <c r="AJ40" s="235"/>
+      <c r="AK40" s="235"/>
+      <c r="AL40" s="235"/>
       <c r="AM40" s="103"/>
       <c r="AO40" s="87"/>
-      <c r="BD40" s="157" t="str">
+      <c r="BD40" s="231" t="str">
         <f>IF(SUM(BD33:BD39)=0,"",SUM(BD33:BD39))</f>
         <v/>
       </c>
-      <c r="BE40" s="158"/>
+      <c r="BE40" s="232"/>
     </row>
     <row r="41" spans="2:59" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B41" s="144" t="s">
+      <c r="B41" s="234" t="s">
         <v>56</v>
       </c>
-      <c r="C41" s="144"/>
-      <c r="D41" s="144"/>
-      <c r="E41" s="144"/>
-      <c r="F41" s="144"/>
-      <c r="G41" s="144"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144"/>
+      <c r="C41" s="234"/>
+      <c r="D41" s="234"/>
+      <c r="E41" s="234"/>
+      <c r="F41" s="234"/>
+      <c r="G41" s="234"/>
+      <c r="H41" s="234"/>
+      <c r="I41" s="234"/>
       <c r="AC41" s="66"/>
       <c r="AD41" s="66"/>
       <c r="AE41" s="66"/>
@@ -4756,16 +4756,16 @@
       </c>
     </row>
     <row r="42" spans="2:59" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="B42" s="144" t="s">
+      <c r="B42" s="234" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="144"/>
-      <c r="D42" s="144"/>
-      <c r="E42" s="144"/>
-      <c r="F42" s="144"/>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144"/>
+      <c r="C42" s="234"/>
+      <c r="D42" s="234"/>
+      <c r="E42" s="234"/>
+      <c r="F42" s="234"/>
+      <c r="G42" s="234"/>
+      <c r="H42" s="234"/>
+      <c r="I42" s="234"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="54"/>
@@ -4779,25 +4779,119 @@
     <protectedRange password="EB2E" sqref="AN10:AO17 V10:W17" name="Range1"/>
   </protectedRanges>
   <mergeCells count="156">
-    <mergeCell ref="BF31:BG32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="S32:V32"/>
-    <mergeCell ref="W32:AD32"/>
-    <mergeCell ref="AE32:AN32"/>
-    <mergeCell ref="AO32:BC32"/>
-    <mergeCell ref="AI19:AM19"/>
-    <mergeCell ref="AI24:AM24"/>
-    <mergeCell ref="AI26:AM26"/>
-    <mergeCell ref="G26:Q28"/>
-    <mergeCell ref="G23:X25"/>
-    <mergeCell ref="S26:W28"/>
-    <mergeCell ref="S19:W20"/>
-    <mergeCell ref="G19:Q20"/>
-    <mergeCell ref="Y19:AB20"/>
-    <mergeCell ref="S21:W21"/>
-    <mergeCell ref="S29:W29"/>
-    <mergeCell ref="AD19:AH29"/>
-    <mergeCell ref="AO24:AP24"/>
+    <mergeCell ref="B40:I40"/>
+    <mergeCell ref="B41:I41"/>
+    <mergeCell ref="B42:I42"/>
+    <mergeCell ref="AH40:AL40"/>
+    <mergeCell ref="AZ33:BA33"/>
+    <mergeCell ref="AZ34:BA34"/>
+    <mergeCell ref="AZ35:BA35"/>
+    <mergeCell ref="AZ36:BA36"/>
+    <mergeCell ref="AZ37:BA37"/>
+    <mergeCell ref="AN16:AP16"/>
+    <mergeCell ref="AN15:AP15"/>
+    <mergeCell ref="BD34:BE34"/>
+    <mergeCell ref="BD35:BE35"/>
+    <mergeCell ref="BD36:BE36"/>
+    <mergeCell ref="BD37:BE37"/>
+    <mergeCell ref="BD38:BE38"/>
+    <mergeCell ref="AZ39:BA39"/>
+    <mergeCell ref="BD40:BE40"/>
+    <mergeCell ref="AN14:AP14"/>
+    <mergeCell ref="Y29:AA29"/>
+    <mergeCell ref="Y15:AA15"/>
+    <mergeCell ref="AE15:AG15"/>
+    <mergeCell ref="AH15:AJ15"/>
+    <mergeCell ref="AH10:AJ10"/>
+    <mergeCell ref="AE11:AG11"/>
+    <mergeCell ref="AE12:AG12"/>
+    <mergeCell ref="Y13:AA13"/>
+    <mergeCell ref="AB15:AD15"/>
+    <mergeCell ref="AI21:AM21"/>
+    <mergeCell ref="AH16:AJ16"/>
+    <mergeCell ref="AN12:AP12"/>
+    <mergeCell ref="AK10:AM10"/>
+    <mergeCell ref="AN11:AP11"/>
+    <mergeCell ref="AH13:AJ13"/>
+    <mergeCell ref="AH14:AJ14"/>
+    <mergeCell ref="AO19:AP19"/>
+    <mergeCell ref="AN13:AP13"/>
+    <mergeCell ref="AN10:AP10"/>
+    <mergeCell ref="AO26:AP26"/>
+    <mergeCell ref="AO21:AP21"/>
+    <mergeCell ref="AO28:AP28"/>
+    <mergeCell ref="AI28:AM28"/>
+    <mergeCell ref="G1:AJ1"/>
+    <mergeCell ref="AK11:AM11"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="AK12:AM12"/>
+    <mergeCell ref="AK13:AM13"/>
+    <mergeCell ref="AK14:AM14"/>
+    <mergeCell ref="AK15:AM15"/>
+    <mergeCell ref="AK16:AM16"/>
+    <mergeCell ref="S16:U16"/>
+    <mergeCell ref="V14:X14"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="P15:R15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="P16:R16"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="Y16:AA16"/>
+    <mergeCell ref="V15:X15"/>
+    <mergeCell ref="S15:U15"/>
+    <mergeCell ref="AH9:AJ9"/>
+    <mergeCell ref="AH11:AJ11"/>
+    <mergeCell ref="AH12:AJ12"/>
+    <mergeCell ref="AB14:AD14"/>
+    <mergeCell ref="AK7:AP7"/>
+    <mergeCell ref="AE4:AI4"/>
+    <mergeCell ref="Y4:AC4"/>
+    <mergeCell ref="AK5:AP6"/>
+    <mergeCell ref="X6:AI6"/>
+    <mergeCell ref="AA7:AI7"/>
+    <mergeCell ref="Y5:AC5"/>
+    <mergeCell ref="AE5:AI5"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="P6:T7"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="S9:U9"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="AB11:AD11"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="V12:X12"/>
+    <mergeCell ref="AB12:AD12"/>
+    <mergeCell ref="AN9:AP9"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="S14:U14"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="V9:X9"/>
+    <mergeCell ref="AK9:AM9"/>
+    <mergeCell ref="Y11:AA11"/>
+    <mergeCell ref="Y12:AA12"/>
+    <mergeCell ref="AE10:AG10"/>
+    <mergeCell ref="AE9:AG9"/>
+    <mergeCell ref="AB10:AD10"/>
+    <mergeCell ref="Y10:AA10"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="AB9:AD9"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="V13:X13"/>
+    <mergeCell ref="AE14:AG14"/>
+    <mergeCell ref="AE13:AG13"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="AB13:AD13"/>
+    <mergeCell ref="Y14:AA14"/>
     <mergeCell ref="AB16:AD16"/>
     <mergeCell ref="Y26:AB28"/>
     <mergeCell ref="BD39:BE39"/>
@@ -4822,119 +4916,25 @@
     <mergeCell ref="P12:R12"/>
     <mergeCell ref="P13:R13"/>
     <mergeCell ref="P11:R11"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="S14:U14"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="V9:X9"/>
-    <mergeCell ref="AK9:AM9"/>
-    <mergeCell ref="Y11:AA11"/>
-    <mergeCell ref="Y12:AA12"/>
-    <mergeCell ref="AE10:AG10"/>
-    <mergeCell ref="AE9:AG9"/>
-    <mergeCell ref="AB10:AD10"/>
-    <mergeCell ref="Y10:AA10"/>
-    <mergeCell ref="Y9:AA9"/>
-    <mergeCell ref="AB9:AD9"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="V13:X13"/>
-    <mergeCell ref="AE14:AG14"/>
-    <mergeCell ref="AE13:AG13"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="AB13:AD13"/>
-    <mergeCell ref="Y14:AA14"/>
-    <mergeCell ref="AK7:AP7"/>
-    <mergeCell ref="AE4:AI4"/>
-    <mergeCell ref="Y4:AC4"/>
-    <mergeCell ref="AK5:AP6"/>
-    <mergeCell ref="X6:AI6"/>
-    <mergeCell ref="AA7:AI7"/>
-    <mergeCell ref="Y5:AC5"/>
-    <mergeCell ref="AE5:AI5"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="P6:T7"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="S9:U9"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="AB11:AD11"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J10:L10"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="V12:X12"/>
-    <mergeCell ref="AB12:AD12"/>
-    <mergeCell ref="AN9:AP9"/>
-    <mergeCell ref="G1:AJ1"/>
-    <mergeCell ref="AK11:AM11"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="AK12:AM12"/>
-    <mergeCell ref="AK13:AM13"/>
-    <mergeCell ref="AK14:AM14"/>
-    <mergeCell ref="AK15:AM15"/>
-    <mergeCell ref="AK16:AM16"/>
-    <mergeCell ref="S16:U16"/>
-    <mergeCell ref="V14:X14"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="P15:R15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="P16:R16"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="Y16:AA16"/>
-    <mergeCell ref="V15:X15"/>
-    <mergeCell ref="S15:U15"/>
-    <mergeCell ref="AH9:AJ9"/>
-    <mergeCell ref="AH11:AJ11"/>
-    <mergeCell ref="AH12:AJ12"/>
-    <mergeCell ref="AB14:AD14"/>
-    <mergeCell ref="AN14:AP14"/>
-    <mergeCell ref="Y29:AA29"/>
-    <mergeCell ref="Y15:AA15"/>
-    <mergeCell ref="AE15:AG15"/>
-    <mergeCell ref="AH15:AJ15"/>
-    <mergeCell ref="AH10:AJ10"/>
-    <mergeCell ref="AE11:AG11"/>
-    <mergeCell ref="AE12:AG12"/>
-    <mergeCell ref="Y13:AA13"/>
-    <mergeCell ref="AB15:AD15"/>
-    <mergeCell ref="AI21:AM21"/>
-    <mergeCell ref="AH16:AJ16"/>
-    <mergeCell ref="AN12:AP12"/>
-    <mergeCell ref="AK10:AM10"/>
-    <mergeCell ref="AN11:AP11"/>
-    <mergeCell ref="AH13:AJ13"/>
-    <mergeCell ref="AH14:AJ14"/>
-    <mergeCell ref="AO19:AP19"/>
-    <mergeCell ref="AN13:AP13"/>
-    <mergeCell ref="AN10:AP10"/>
-    <mergeCell ref="AO26:AP26"/>
-    <mergeCell ref="AO21:AP21"/>
-    <mergeCell ref="AO28:AP28"/>
-    <mergeCell ref="AI28:AM28"/>
-    <mergeCell ref="AN16:AP16"/>
-    <mergeCell ref="AN15:AP15"/>
-    <mergeCell ref="BD34:BE34"/>
-    <mergeCell ref="BD35:BE35"/>
-    <mergeCell ref="BD36:BE36"/>
-    <mergeCell ref="BD37:BE37"/>
-    <mergeCell ref="BD38:BE38"/>
-    <mergeCell ref="AZ39:BA39"/>
-    <mergeCell ref="BD40:BE40"/>
-    <mergeCell ref="B40:I40"/>
-    <mergeCell ref="B41:I41"/>
-    <mergeCell ref="B42:I42"/>
-    <mergeCell ref="AH40:AL40"/>
-    <mergeCell ref="AZ33:BA33"/>
-    <mergeCell ref="AZ34:BA34"/>
-    <mergeCell ref="AZ35:BA35"/>
-    <mergeCell ref="AZ36:BA36"/>
-    <mergeCell ref="AZ37:BA37"/>
+    <mergeCell ref="BF31:BG32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="S32:V32"/>
+    <mergeCell ref="W32:AD32"/>
+    <mergeCell ref="AE32:AN32"/>
+    <mergeCell ref="AO32:BC32"/>
+    <mergeCell ref="AI19:AM19"/>
+    <mergeCell ref="AI24:AM24"/>
+    <mergeCell ref="AI26:AM26"/>
+    <mergeCell ref="G26:Q28"/>
+    <mergeCell ref="G23:X25"/>
+    <mergeCell ref="S26:W28"/>
+    <mergeCell ref="S19:W20"/>
+    <mergeCell ref="G19:Q20"/>
+    <mergeCell ref="Y19:AB20"/>
+    <mergeCell ref="S21:W21"/>
+    <mergeCell ref="S29:W29"/>
+    <mergeCell ref="AD19:AH29"/>
+    <mergeCell ref="AO24:AP24"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <dataValidations xWindow="252" yWindow="215" count="4">

</xml_diff>